<commit_message>
added test cases that derive from config.edn
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36B6555-2246-BB4B-A3F1-CFC22FDDF383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9B28B1-077A-AC4F-82D2-756C6FD342ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="-19740" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="940" yWindow="-19040" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
xlsx tests - 480 assertions working
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A12E43-274B-4640-9967-D9FBEF98C9A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E3F5B1-586C-734A-8798-3F7C93AC7AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="-19660" windowWidth="29540" windowHeight="19040" firstSheet="2" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1820" yWindow="-19660" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="270">
   <si>
     <t>Notes</t>
   </si>
@@ -607,9 +607,6 @@
   </si>
   <si>
     <t>Recipient cholesterol at registration</t>
-  </si>
-  <si>
-    <t>Interaction between transplant type and disease group</t>
   </si>
   <si>
     <t>Negative</t>
@@ -1574,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E50BA8A-672F-1740-8DE6-439CBC2BCF16}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1669,7 +1666,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1677,7 +1674,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1701,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37:K38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1731,7 +1728,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>40</v>
@@ -1757,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="55"/>
       <c r="F2" s="63" t="s">
@@ -1766,7 +1763,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1776,14 +1773,14 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="60" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1793,14 +1790,14 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
       <c r="I4" s="60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1810,14 +1807,14 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E5" s="55"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1827,7 +1824,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
@@ -2092,7 +2089,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>67</v>
@@ -2198,7 +2195,7 @@
         <v>130</v>
       </c>
       <c r="I30" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2237,9 +2234,7 @@
       <c r="I33" s="60"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1">
-      <c r="A34" s="68" t="s">
-        <v>89</v>
-      </c>
+      <c r="A34" s="68"/>
       <c r="B34" s="14" t="s">
         <v>94</v>
       </c>
@@ -2253,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
@@ -2350,7 +2345,7 @@
         <v>7.2209999999999996E-2</v>
       </c>
       <c r="I40" s="62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2367,7 +2362,7 @@
         <v>-0.29171999999999998</v>
       </c>
       <c r="I41" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2408,7 +2403,7 @@
         <v>137</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
@@ -35727,7 +35722,7 @@
         <v>137</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -35735,7 +35730,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -35747,8 +35742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -35818,7 +35813,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="55"/>
       <c r="F2" s="63"/>
@@ -35830,7 +35825,7 @@
       <c r="J2" s="55"/>
       <c r="K2" s="55"/>
       <c r="L2" s="60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -35840,7 +35835,7 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
@@ -35858,7 +35853,7 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
@@ -35876,7 +35871,7 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E5" s="55"/>
       <c r="F5" s="55"/>
@@ -35894,7 +35889,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
@@ -36156,7 +36151,7 @@
         <v>50</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>129</v>
@@ -36506,7 +36501,7 @@
       <c r="B31"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" s="29">
         <v>0.28376000000000001</v>
@@ -36532,7 +36527,7 @@
       <c r="B32"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E32" s="29">
         <v>0.23757</v>
@@ -36554,7 +36549,7 @@
       <c r="B33"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E33" s="29">
         <v>-0.69055999999999995</v>
@@ -36581,7 +36576,7 @@
         <v>110</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
@@ -36591,7 +36586,7 @@
         <v>130</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K34" s="14"/>
       <c r="L34" s="12" t="s">
@@ -36681,12 +36676,8 @@
       <c r="H38" s="32">
         <v>-8.1760000000000003E-4</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>253</v>
-      </c>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
       <c r="K38" s="14"/>
       <c r="N38" s="3"/>
     </row>
@@ -36699,9 +36690,14 @@
         <v>24</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="I39" s="14"/>
+        <v>260</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>252</v>
+      </c>
       <c r="K39" s="14"/>
       <c r="L39" s="12" t="s">
         <v>165</v>
@@ -36748,11 +36744,11 @@
         <v>130</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K41" s="14"/>
       <c r="L41" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1">
@@ -36796,7 +36792,7 @@
         <v>130</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="12" t="s">
@@ -36817,7 +36813,7 @@
     </row>
     <row r="45" spans="1:14" s="12" customFormat="1" ht="16">
       <c r="A45" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B45" s="19" t="s">
         <v>67</v>
@@ -37528,7 +37524,7 @@
         <v>132</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F1" s="38" t="s">
         <v>167</v>
@@ -37543,7 +37539,7 @@
         <v>170</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -37575,7 +37571,7 @@
         <v>3.55</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -37607,7 +37603,7 @@
         <v>63</v>
       </c>
       <c r="J3" s="64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37627,7 +37623,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -37647,12 +37643,12 @@
         <v>0</v>
       </c>
       <c r="J5" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>24</v>
@@ -37679,15 +37675,15 @@
         <v>63</v>
       </c>
       <c r="J6" s="64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="A7" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7">
         <v>-2.2000000000000002</v>
@@ -37703,12 +37699,12 @@
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1">
       <c r="A8" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>110</v>
@@ -37730,7 +37726,7 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1">
       <c r="A9" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="49" t="s">
         <v>162</v>
@@ -37749,15 +37745,15 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1">
       <c r="A10" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" s="45">
         <v>1.3</v>
@@ -37772,7 +37768,7 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1">
       <c r="A11" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" s="49" t="s">
         <v>24</v>
@@ -37787,12 +37783,12 @@
         <v>0</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1">
       <c r="A12" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12" s="49" t="s">
         <v>125</v>
@@ -37949,7 +37945,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -44028,15 +44024,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>28</v>
@@ -44076,7 +44072,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="41" t="s">
         <v>184</v>
@@ -44100,7 +44096,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B11" s="14">
         <v>4.9000000000000004</v>
@@ -44111,15 +44107,15 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -44138,8 +44134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -44170,7 +44166,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>40</v>
@@ -44196,7 +44192,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="55"/>
       <c r="F2" s="63" t="s">
@@ -44205,7 +44201,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -44215,14 +44211,14 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="60" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -44232,14 +44228,14 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
       <c r="I4" s="60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -44249,14 +44245,14 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E5" s="55"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -44266,7 +44262,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
@@ -44284,7 +44280,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>
       <c r="I7" s="60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -44292,13 +44288,13 @@
         <v>174</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="E8" s="42">
         <v>-0.27407999999999999</v>
@@ -44307,7 +44303,7 @@
         <v>46</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I8" s="12"/>
     </row>
@@ -44317,10 +44313,10 @@
         <v>175</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="43">
         <v>0</v>
@@ -44343,7 +44339,7 @@
         <v>67</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>29</v>
@@ -44355,10 +44351,10 @@
         <v>46</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -44367,7 +44363,7 @@
         <v>66</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>28</v>
@@ -44376,7 +44372,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -44407,20 +44403,20 @@
         <v>46</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="68"/>
       <c r="B15" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>115</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E15" s="44">
         <v>-0.31792999999999999</v>
@@ -44456,7 +44452,7 @@
         <v>178</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>40</v>
@@ -44585,7 +44581,7 @@
       <c r="B26" s="40"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E26" s="44">
         <v>-4.6809999999999997E-2</v>
@@ -44597,7 +44593,7 @@
       <c r="B27" s="40"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E27" s="44">
         <v>1.5200000000000001E-3</v>
@@ -44609,7 +44605,7 @@
       <c r="B28" s="40"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E28" s="44">
         <v>-3.4199999999999999E-3</v>
@@ -44625,17 +44621,17 @@
         <v>24</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E29" s="44"/>
       <c r="F29" s="3" t="s">
         <v>130</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -44652,7 +44648,7 @@
       </c>
       <c r="B31" s="41"/>
       <c r="C31" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>158</v>
@@ -44691,7 +44687,7 @@
         <v>130</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I33" s="12"/>
     </row>
@@ -44721,7 +44717,7 @@
         <v>130</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I35" s="12"/>
     </row>
@@ -44739,7 +44735,7 @@
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>158</v>
@@ -44751,7 +44747,7 @@
         <v>130</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I37" s="12"/>
     </row>
@@ -44770,35 +44766,33 @@
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="68" t="s">
-        <v>188</v>
-      </c>
+      <c r="A40" s="68"/>
       <c r="B40" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="E40" s="44">
         <v>-0.27877999999999997</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="68"/>
       <c r="B41" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E41" s="44">
         <v>0.34847</v>
@@ -44807,13 +44801,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="B42" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E42" s="46">
         <v>0</v>
@@ -44822,13 +44816,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="B43" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E43" s="46">
         <v>0</v>
@@ -44837,13 +44831,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="B44" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E44" s="46">
         <v>0</v>
@@ -44852,13 +44846,13 @@
     </row>
     <row r="45" spans="1:9">
       <c r="B45" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E45" s="46">
         <v>0</v>
@@ -44867,13 +44861,13 @@
     </row>
     <row r="46" spans="1:9">
       <c r="B46" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E46" s="46">
         <v>0</v>
@@ -44882,13 +44876,13 @@
     </row>
     <row r="47" spans="1:9">
       <c r="B47" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E47" s="46">
         <v>0</v>
@@ -44969,7 +44963,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1" s="10"/>
     </row>

</xml_diff>

<commit_message>
revisions to xlsx to comply
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E3F5B1-586C-734A-8798-3F7C93AC7AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53D65FF-3C8E-4B4A-A15C-87E4083E1DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="-19660" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
@@ -1698,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:A35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
routing starter, removed 10x debugger
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53D65FF-3C8E-4B4A-A15C-87E4083E1DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E6EDED-7FBC-CE47-9ADF-EFE5A479F0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="-19660" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1800" yWindow="-21320" windowWidth="29540" windowHeight="19040" firstSheet="2" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3341" uniqueCount="270">
   <si>
     <t>Notes</t>
   </si>
@@ -1165,13 +1165,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1771,7 +1771,9 @@
       <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="16" t="s">
         <v>235</v>
       </c>
@@ -1788,7 +1790,9 @@
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="16" t="s">
         <v>236</v>
       </c>
@@ -1805,7 +1809,9 @@
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="16" t="s">
         <v>237</v>
       </c>
@@ -1822,7 +1828,9 @@
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="16" t="s">
         <v>255</v>
       </c>
@@ -2234,7 +2242,7 @@
       <c r="I33" s="60"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="14" t="s">
         <v>94</v>
       </c>
@@ -2252,7 +2260,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
-      <c r="A35" s="68"/>
+      <c r="A35" s="69"/>
       <c r="B35" s="14" t="s">
         <v>90</v>
       </c>
@@ -35583,7 +35591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA849B77-A729-9F4B-AFFB-4400AE5F1FC9}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -35742,8 +35750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -35833,7 +35841,9 @@
       <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="16" t="s">
         <v>235</v>
       </c>
@@ -35851,7 +35861,9 @@
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="16" t="s">
         <v>236</v>
       </c>
@@ -35869,7 +35881,9 @@
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="16" t="s">
         <v>237</v>
       </c>
@@ -35887,7 +35901,9 @@
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="16" t="s">
         <v>255</v>
       </c>
@@ -36123,7 +36139,7 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:12" ht="16">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="68" t="s">
         <v>75</v>
       </c>
       <c r="B16" s="19">
@@ -36158,7 +36174,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="16">
-      <c r="A17" s="67"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="22" t="s">
         <v>85</v>
       </c>
@@ -38098,7 +38114,7 @@
       <c r="C12" s="3">
         <v>0.79270650573773382</v>
       </c>
-      <c r="F12" s="68"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:14">
@@ -38111,7 +38127,7 @@
       <c r="C13" s="3">
         <v>0.77714124234773851</v>
       </c>
-      <c r="F13" s="68"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="11" t="s">
@@ -44023,7 +44039,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="67" t="s">
         <v>199</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -44031,7 +44047,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="67" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -44039,7 +44055,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="67" t="s">
         <v>115</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -44047,7 +44063,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="67" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -44055,7 +44071,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="67" t="s">
         <v>136</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -44063,7 +44079,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="67" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -44071,7 +44087,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="67" t="s">
         <v>215</v>
       </c>
       <c r="B8" s="41" t="s">
@@ -44079,7 +44095,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="67" t="s">
         <v>110</v>
       </c>
       <c r="B9" s="14">
@@ -44087,7 +44103,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="67" t="s">
         <v>162</v>
       </c>
       <c r="B10" s="14">
@@ -44095,7 +44111,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="67" t="s">
         <v>216</v>
       </c>
       <c r="B11" s="14">
@@ -44103,7 +44119,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="67" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -44111,7 +44127,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="67" t="s">
         <v>204</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -44134,8 +44150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:A41"/>
+    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -44209,7 +44225,9 @@
       <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="16" t="s">
         <v>235</v>
       </c>
@@ -44226,7 +44244,9 @@
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="16" t="s">
         <v>236</v>
       </c>
@@ -44243,7 +44263,9 @@
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="16" t="s">
         <v>237</v>
       </c>
@@ -44260,7 +44282,9 @@
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="16" t="s">
         <v>255</v>
       </c>
@@ -44384,7 +44408,7 @@
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>177</v>
       </c>
       <c r="B14" s="14">
@@ -44408,7 +44432,7 @@
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="68"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="14" t="s">
         <v>189</v>
       </c>
@@ -44473,7 +44497,9 @@
       <c r="B19" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="D19" s="16" t="s">
         <v>121</v>
       </c>
@@ -44766,7 +44792,7 @@
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="68"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="3" t="s">
         <v>191</v>
       </c>
@@ -44784,7 +44810,7 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="68"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="3" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
All inputs sheets have factors filled in
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E6EDED-7FBC-CE47-9ADF-EFE5A479F0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E1BEA9-DDBF-FB4D-AB89-79747E4B4DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="-21320" windowWidth="29540" windowHeight="19040" firstSheet="2" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1800" yWindow="-21320" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1698,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
@@ -35591,7 +35591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA849B77-A729-9F4B-AFFB-4400AE5F1FC9}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -35750,8 +35750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -44150,7 +44150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
spreadsheet tests passing after addition of order
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E1BEA9-DDBF-FB4D-AB89-79747E4B4DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3134CA-6056-F043-BA47-1C871EA9141A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="-21320" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="10" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="7" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3341" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="271">
   <si>
     <t>Notes</t>
   </si>
@@ -854,17 +854,21 @@
   <si>
     <t>:unused</t>
   </si>
+  <si>
+    <t>:order</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -928,6 +932,13 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1007,11 +1018,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1172,8 +1184,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1050B777-A2D7-D942-9E8B-7FC0C917BD88}"/>
   </cellStyles>
@@ -1696,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1710,11 +1747,12 @@
     <col min="4" max="4" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="3"/>
-    <col min="9" max="9" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="3"/>
+    <col min="9" max="9" width="8.83203125" style="77"/>
+    <col min="10" max="10" width="32" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -1739,11 +1777,14 @@
       <c r="H1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>173</v>
       </c>
@@ -1762,11 +1803,14 @@
       </c>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="60" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="55"/>
       <c r="B3" s="63" t="s">
         <v>81</v>
@@ -1781,11 +1825,14 @@
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="60" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="55"/>
       <c r="B4" s="63" t="s">
         <v>20</v>
@@ -1800,11 +1847,14 @@
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="60" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="55"/>
       <c r="B5" s="63" t="s">
         <v>21</v>
@@ -1819,11 +1869,14 @@
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="60" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="55"/>
       <c r="B6" s="63" t="s">
         <v>19</v>
@@ -1838,9 +1891,12 @@
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="55"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="60"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="55"/>
       <c r="B7" s="55"/>
       <c r="C7" s="16"/>
@@ -1849,9 +1905,10 @@
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="60"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="76"/>
+      <c r="J7" s="60"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="39" t="s">
         <v>44</v>
       </c>
@@ -1870,9 +1927,12 @@
       <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="60"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="77">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J8" s="60"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="39"/>
       <c r="B9" s="14" t="s">
         <v>47</v>
@@ -1886,17 +1946,20 @@
       <c r="E9" s="3">
         <v>0</v>
       </c>
-      <c r="I9" s="60"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="77">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J9" s="60"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="39"/>
       <c r="B10" s="14"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="42"/>
-      <c r="I10" s="60"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="60"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="39" t="s">
         <v>72</v>
       </c>
@@ -1915,9 +1978,12 @@
       <c r="F11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="60"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="77">
+        <v>1.2</v>
+      </c>
+      <c r="J11" s="60"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="39"/>
       <c r="B12" s="14" t="s">
         <v>55</v>
@@ -1931,17 +1997,20 @@
       <c r="E12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="60"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="77">
+        <v>1.2</v>
+      </c>
+      <c r="J12" s="60"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="39"/>
       <c r="B13" s="14"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="44"/>
-      <c r="I13" s="60"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="J13" s="60"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="50" t="s">
         <v>57</v>
       </c>
@@ -1960,9 +2029,12 @@
       <c r="F14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="60"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="I14" s="77">
+        <v>1.3</v>
+      </c>
+      <c r="J14" s="60"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="50"/>
       <c r="B15" s="14" t="s">
         <v>60</v>
@@ -1976,9 +2048,12 @@
       <c r="E15" s="3">
         <v>-9.4829999999999998E-2</v>
       </c>
-      <c r="I15" s="60"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="77">
+        <v>1.3</v>
+      </c>
+      <c r="J15" s="60"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="39"/>
       <c r="B16" s="14" t="s">
         <v>62</v>
@@ -1992,9 +2067,12 @@
       <c r="E16" s="3">
         <v>-2.5999999999999999E-3</v>
       </c>
-      <c r="I16" s="60"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" s="77">
+        <v>1.3</v>
+      </c>
+      <c r="J16" s="60"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="39"/>
       <c r="B17" s="14" t="s">
         <v>64</v>
@@ -2008,17 +2086,20 @@
       <c r="E17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="60"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="77">
+        <v>1.3</v>
+      </c>
+      <c r="J17" s="60"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="39"/>
       <c r="B18" s="14"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="44"/>
-      <c r="I18" s="60"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="60"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="39" t="s">
         <v>77</v>
       </c>
@@ -2037,9 +2118,12 @@
       <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="60"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="77">
+        <v>1.4</v>
+      </c>
+      <c r="J19" s="60"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="39"/>
       <c r="B20" s="14" t="s">
         <v>83</v>
@@ -2053,9 +2137,12 @@
       <c r="E20" s="3">
         <v>0.51051999999999997</v>
       </c>
-      <c r="I20" s="60"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20" s="77">
+        <v>1.4</v>
+      </c>
+      <c r="J20" s="60"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="39"/>
       <c r="B21" s="14" t="s">
         <v>84</v>
@@ -2069,9 +2156,12 @@
       <c r="E21" s="3">
         <v>0.62370000000000003</v>
       </c>
-      <c r="I21" s="60"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="77">
+        <v>1.4</v>
+      </c>
+      <c r="J21" s="60"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="39"/>
       <c r="B22" s="14" t="s">
         <v>76</v>
@@ -2085,17 +2175,20 @@
       <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="I22" s="60"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22" s="77">
+        <v>1.4</v>
+      </c>
+      <c r="J22" s="60"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="39"/>
       <c r="B23" s="14"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="44"/>
-      <c r="I23" s="60"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="60"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="39" t="s">
         <v>224</v>
       </c>
@@ -2114,9 +2207,12 @@
       <c r="F24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="60"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24" s="77">
+        <v>1.5</v>
+      </c>
+      <c r="J24" s="60"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="39"/>
       <c r="B25" s="14" t="s">
         <v>66</v>
@@ -2130,17 +2226,20 @@
       <c r="E25" s="3">
         <v>0</v>
       </c>
-      <c r="I25" s="60"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1">
+      <c r="I25" s="77">
+        <v>1.5</v>
+      </c>
+      <c r="J25" s="60"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1">
       <c r="A26" s="50"/>
       <c r="B26" s="40"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="44"/>
-      <c r="I26" s="60"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1">
+      <c r="J26" s="60"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1">
       <c r="A27" s="50" t="s">
         <v>73</v>
       </c>
@@ -2159,9 +2258,12 @@
       <c r="F27" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="60"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1">
+      <c r="I27" s="77">
+        <v>1.6</v>
+      </c>
+      <c r="J27" s="60"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="50"/>
       <c r="B28" s="40" t="s">
         <v>66</v>
@@ -2175,17 +2277,20 @@
       <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="60"/>
-    </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1">
+      <c r="I28" s="77">
+        <v>1.6</v>
+      </c>
+      <c r="J28" s="60"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="50"/>
       <c r="B29" s="40"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="44"/>
-      <c r="I29" s="60"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="60"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="39" t="s">
         <v>69</v>
       </c>
@@ -2202,19 +2307,22 @@
       <c r="F30" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I30" s="60" t="s">
+      <c r="I30" s="77">
+        <v>1.7</v>
+      </c>
+      <c r="J30" s="60" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31" s="39"/>
       <c r="B31" s="41"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="44"/>
-      <c r="I31" s="60"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="60"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="39" t="s">
         <v>71</v>
       </c>
@@ -2231,17 +2339,20 @@
       <c r="F32" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I32" s="60"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="I32" s="77">
+        <v>1.8</v>
+      </c>
+      <c r="J32" s="60"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="39"/>
       <c r="B33" s="41"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
       <c r="E33" s="44"/>
-      <c r="I33" s="60"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1">
+      <c r="J33" s="60"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="69"/>
       <c r="B34" s="14" t="s">
         <v>94</v>
@@ -2255,11 +2366,11 @@
       <c r="E34" s="3">
         <v>0</v>
       </c>
-      <c r="I34" s="60" t="s">
+      <c r="J34" s="60" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1">
+    <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="69"/>
       <c r="B35" s="14" t="s">
         <v>90</v>
@@ -2273,9 +2384,9 @@
       <c r="E35" s="3">
         <v>-0.10414</v>
       </c>
-      <c r="I35" s="60"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="60"/>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="39"/>
       <c r="B36" s="41" t="s">
         <v>91</v>
@@ -2289,9 +2400,9 @@
       <c r="E36" s="3">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="I36" s="60"/>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="60"/>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="39"/>
       <c r="B37" s="14" t="s">
         <v>92</v>
@@ -2305,9 +2416,9 @@
       <c r="E37" s="3">
         <v>1.8270000000000002E-2</v>
       </c>
-      <c r="I37" s="60"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="60"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="B38" s="41" t="s">
         <v>93</v>
       </c>
@@ -2320,9 +2431,9 @@
       <c r="E38" s="3">
         <v>-8.7040000000000006E-2</v>
       </c>
-      <c r="I38" s="60"/>
-    </row>
-    <row r="39" spans="1:9" ht="14.25" customHeight="1">
+      <c r="J38" s="60"/>
+    </row>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="51"/>
       <c r="B39" s="14" t="s">
         <v>99</v>
@@ -2336,9 +2447,9 @@
       <c r="E39" s="3">
         <v>0</v>
       </c>
-      <c r="I39" s="60"/>
-    </row>
-    <row r="40" spans="1:9" ht="14.25" customHeight="1">
+      <c r="J39" s="60"/>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1">
       <c r="A40" s="51"/>
       <c r="B40" s="14" t="s">
         <v>95</v>
@@ -2352,11 +2463,11 @@
       <c r="E40" s="3">
         <v>7.2209999999999996E-2</v>
       </c>
-      <c r="I40" s="62" t="s">
+      <c r="J40" s="62" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:10">
       <c r="B41" s="40" t="s">
         <v>96</v>
       </c>
@@ -2369,11 +2480,11 @@
       <c r="E41" s="3">
         <v>-0.29171999999999998</v>
       </c>
-      <c r="I41" s="62" t="s">
+      <c r="J41" s="62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:10">
       <c r="B42" s="3" t="s">
         <v>97</v>
       </c>
@@ -2386,9 +2497,9 @@
       <c r="E42" s="3">
         <v>-0.36563000000000001</v>
       </c>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="B43" s="3" t="s">
         <v>98</v>
       </c>
@@ -2401,9 +2512,9 @@
       <c r="E43" s="3">
         <v>7.6780000000000001E-2</v>
       </c>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="B44" s="14" t="s">
         <v>104</v>
       </c>
@@ -2416,9 +2527,9 @@
       <c r="E44" s="3">
         <v>0</v>
       </c>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="B45" s="3" t="s">
         <v>100</v>
       </c>
@@ -2431,9 +2542,9 @@
       <c r="E45" s="3">
         <v>0.47683999999999999</v>
       </c>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="B46" s="3" t="s">
         <v>101</v>
       </c>
@@ -2446,9 +2557,9 @@
       <c r="E46" s="3">
         <v>0.38514999999999999</v>
       </c>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="B47" s="3" t="s">
         <v>102</v>
       </c>
@@ -2461,9 +2572,9 @@
       <c r="E47" s="3">
         <v>-0.22559999999999999</v>
       </c>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="13"/>
+    </row>
+    <row r="48" spans="1:10">
       <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
@@ -2476,9 +2587,9 @@
       <c r="E48" s="3">
         <v>0.57589999999999997</v>
       </c>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" spans="2:9">
+      <c r="J48" s="13"/>
+    </row>
+    <row r="49" spans="2:10">
       <c r="B49" s="14" t="s">
         <v>109</v>
       </c>
@@ -2491,9 +2602,9 @@
       <c r="E49" s="3">
         <v>0</v>
       </c>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="2:9">
+      <c r="J49" s="13"/>
+    </row>
+    <row r="50" spans="2:10">
       <c r="B50" s="3" t="s">
         <v>105</v>
       </c>
@@ -2506,9 +2617,9 @@
       <c r="E50" s="3">
         <v>0</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="2:9">
+      <c r="J50" s="13"/>
+    </row>
+    <row r="51" spans="2:10">
       <c r="B51" s="3" t="s">
         <v>106</v>
       </c>
@@ -2521,9 +2632,9 @@
       <c r="E51" s="3">
         <v>0</v>
       </c>
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" spans="2:9">
+      <c r="J51" s="13"/>
+    </row>
+    <row r="52" spans="2:10">
       <c r="B52" s="3" t="s">
         <v>107</v>
       </c>
@@ -2536,9 +2647,9 @@
       <c r="E52" s="3">
         <v>0</v>
       </c>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="2:9">
+      <c r="J52" s="13"/>
+    </row>
+    <row r="53" spans="2:10">
       <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
@@ -2551,7 +2662,7 @@
       <c r="E53" s="3">
         <v>0</v>
       </c>
-      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -35748,31 +35859,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="42.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="72" customWidth="1"/>
+    <col min="13" max="13" width="60.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -35806,11 +35918,14 @@
       <c r="K1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="70" t="s">
+        <v>270</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="55" t="s">
         <v>173</v>
       </c>
@@ -35832,11 +35947,14 @@
       </c>
       <c r="J2" s="55"/>
       <c r="K2" s="55"/>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="M2" s="60" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="55"/>
       <c r="B3" s="63" t="s">
         <v>81</v>
@@ -35854,9 +35972,12 @@
       <c r="I3" s="55"/>
       <c r="J3" s="55"/>
       <c r="K3" s="55"/>
-      <c r="L3" s="60"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="55"/>
       <c r="B4" s="63" t="s">
         <v>20</v>
@@ -35874,9 +35995,12 @@
       <c r="I4" s="55"/>
       <c r="J4" s="55"/>
       <c r="K4" s="55"/>
-      <c r="L4" s="60"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="60"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="55"/>
       <c r="B5" s="63" t="s">
         <v>21</v>
@@ -35894,9 +36018,12 @@
       <c r="I5" s="55"/>
       <c r="J5" s="55"/>
       <c r="K5" s="55"/>
-      <c r="L5" s="60"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="L5" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="60"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="55"/>
       <c r="B6" s="63" t="s">
         <v>19</v>
@@ -35914,9 +36041,12 @@
       <c r="I6" s="55"/>
       <c r="J6" s="55"/>
       <c r="K6" s="55"/>
-      <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="60"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="55"/>
       <c r="B7" s="63"/>
       <c r="C7" s="16"/>
@@ -35928,9 +36058,10 @@
       <c r="I7" s="55"/>
       <c r="J7" s="55"/>
       <c r="K7" s="55"/>
-      <c r="L7" s="60"/>
-    </row>
-    <row r="8" spans="1:12" ht="16">
+      <c r="L7" s="71"/>
+      <c r="M7" s="60"/>
+    </row>
+    <row r="8" spans="1:13" ht="16">
       <c r="A8" s="21" t="s">
         <v>44</v>
       </c>
@@ -35962,8 +36093,11 @@
       <c r="K8" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="16">
+      <c r="L8" s="72">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16">
       <c r="A9" s="21"/>
       <c r="B9" s="19" t="s">
         <v>47</v>
@@ -35988,11 +36122,14 @@
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="72">
+        <v>1.08</v>
+      </c>
+      <c r="M9" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16">
+    <row r="10" spans="1:13" ht="16">
       <c r="A10" s="21"/>
       <c r="B10" s="19"/>
       <c r="C10" s="16"/>
@@ -36004,7 +36141,7 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:12" ht="16">
+    <row r="11" spans="1:13" ht="16">
       <c r="A11" s="21" t="s">
         <v>77</v>
       </c>
@@ -36038,11 +36175,14 @@
       <c r="K11" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="72">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16">
+    <row r="12" spans="1:13" ht="16">
       <c r="A12" s="21"/>
       <c r="B12" s="19" t="s">
         <v>83</v>
@@ -36067,8 +36207,11 @@
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" ht="16">
+      <c r="L12" s="72">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
       <c r="A13" s="21"/>
       <c r="B13" s="19" t="s">
         <v>84</v>
@@ -36096,8 +36239,11 @@
         <v>127</v>
       </c>
       <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" ht="16">
+      <c r="L13" s="72">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="21"/>
       <c r="B14" s="19" t="s">
         <v>76</v>
@@ -36125,8 +36271,11 @@
         <v>128</v>
       </c>
       <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" ht="16">
+      <c r="L14" s="72">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="21"/>
       <c r="B15" s="19"/>
       <c r="C15" s="16"/>
@@ -36138,7 +36287,7 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:12" ht="16">
+    <row r="16" spans="1:13" ht="16">
       <c r="A16" s="68" t="s">
         <v>75</v>
       </c>
@@ -36172,8 +36321,11 @@
       <c r="K16" s="14" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="16">
+      <c r="L16" s="72">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16">
       <c r="A17" s="68"/>
       <c r="B17" s="22" t="s">
         <v>85</v>
@@ -36199,8 +36351,11 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:12" ht="16">
+      <c r="L17" s="72">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16">
       <c r="A18" s="21"/>
       <c r="B18" s="19" t="s">
         <v>74</v>
@@ -36226,11 +36381,14 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="72">
+        <v>1.03</v>
+      </c>
+      <c r="M18" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16">
+    <row r="19" spans="1:13" ht="16">
       <c r="A19" s="21"/>
       <c r="B19" s="19"/>
       <c r="C19" s="16"/>
@@ -36243,7 +36401,7 @@
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:12" ht="16">
+    <row r="20" spans="1:13" ht="16">
       <c r="A20" s="23" t="s">
         <v>73</v>
       </c>
@@ -36275,8 +36433,11 @@
       <c r="K20" s="14" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="16">
+      <c r="L20" s="72">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16">
       <c r="A21" s="23"/>
       <c r="B21" s="24" t="s">
         <v>66</v>
@@ -36302,11 +36463,14 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="72">
+        <v>1.07</v>
+      </c>
+      <c r="M21" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16">
+    <row r="22" spans="1:13" ht="16">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
@@ -36318,7 +36482,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:12" ht="16">
+    <row r="23" spans="1:13" ht="16">
       <c r="A23" s="21" t="s">
         <v>79</v>
       </c>
@@ -36350,8 +36514,11 @@
       <c r="K23" s="14" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="16">
+      <c r="L23" s="72">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16">
       <c r="A24" s="21"/>
       <c r="B24" s="19" t="s">
         <v>87</v>
@@ -36376,8 +36543,11 @@
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:12" ht="16">
+      <c r="L24" s="72">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16">
       <c r="A25" s="21"/>
       <c r="B25" s="19" t="s">
         <v>88</v>
@@ -36402,8 +36572,11 @@
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="1:12" ht="16">
+      <c r="L25" s="72">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16">
       <c r="A26" s="21"/>
       <c r="B26" s="19" t="s">
         <v>78</v>
@@ -36429,8 +36602,11 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:12" ht="16">
+      <c r="L26" s="72">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="16">
       <c r="A27" s="21"/>
       <c r="B27" s="19"/>
       <c r="C27" s="16"/>
@@ -36442,7 +36618,7 @@
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:12" ht="16">
+    <row r="28" spans="1:13" ht="16">
       <c r="A28" s="21" t="s">
         <v>72</v>
       </c>
@@ -36472,8 +36648,11 @@
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="1:12" ht="16">
+      <c r="L28" s="72">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16">
       <c r="A29" s="21"/>
       <c r="B29" s="19" t="s">
         <v>55</v>
@@ -36499,8 +36678,11 @@
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:12" ht="16">
+      <c r="L29" s="72">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="16">
       <c r="A30" s="21"/>
       <c r="B30" s="19"/>
       <c r="C30" s="16"/>
@@ -36512,7 +36694,7 @@
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="1:12" ht="16">
+    <row r="31" spans="1:13" ht="16">
       <c r="A31" s="25"/>
       <c r="B31"/>
       <c r="C31" s="16"/>
@@ -36534,11 +36716,11 @@
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="12" t="s">
+      <c r="M31" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="16">
+    <row r="32" spans="1:13" ht="16">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32" s="16"/>
@@ -36560,7 +36742,7 @@
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="1:14" ht="16">
+    <row r="33" spans="1:15" ht="16">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33" s="16"/>
@@ -36583,7 +36765,7 @@
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="1:14" ht="16">
+    <row r="34" spans="1:15" ht="16">
       <c r="A34" s="25" t="s">
         <v>70</v>
       </c>
@@ -36605,11 +36787,14 @@
         <v>241</v>
       </c>
       <c r="K34" s="14"/>
-      <c r="L34" s="12" t="s">
+      <c r="L34" s="72">
+        <v>1.06</v>
+      </c>
+      <c r="M34" s="12" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16">
+    <row r="35" spans="1:15" ht="16">
       <c r="A35" s="25"/>
       <c r="B35" s="24"/>
       <c r="C35" s="16"/>
@@ -36622,7 +36807,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
     </row>
-    <row r="36" spans="1:14" ht="16">
+    <row r="36" spans="1:15" ht="16">
       <c r="A36" s="25"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
@@ -36644,11 +36829,11 @@
       <c r="I36"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
-      <c r="L36" s="12" t="s">
+      <c r="M36" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="12" customFormat="1" ht="16">
+    <row r="37" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A37" s="25"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
@@ -36670,10 +36855,11 @@
       <c r="I37"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="13"/>
-      <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" s="12" customFormat="1" ht="16">
+      <c r="L37" s="72"/>
+      <c r="M37" s="13"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A38" s="25"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
@@ -36695,9 +36881,10 @@
       <c r="I38" s="54"/>
       <c r="J38" s="54"/>
       <c r="K38" s="14"/>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" ht="16">
+      <c r="L38" s="72"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" ht="16">
       <c r="A39" s="25" t="s">
         <v>69</v>
       </c>
@@ -36715,11 +36902,14 @@
         <v>252</v>
       </c>
       <c r="K39" s="14"/>
-      <c r="L39" s="12" t="s">
+      <c r="L39" s="72">
+        <v>1.01</v>
+      </c>
+      <c r="M39" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="12" customFormat="1" ht="16">
+    <row r="40" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A40" s="25"/>
       <c r="B40" s="24"/>
       <c r="C40" s="16"/>
@@ -36731,9 +36921,10 @@
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
-      <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" ht="16">
+      <c r="L40" s="72"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="1:15" ht="16">
       <c r="A41" s="21" t="s">
         <v>71</v>
       </c>
@@ -36763,11 +36954,14 @@
         <v>253</v>
       </c>
       <c r="K41" s="14"/>
-      <c r="L41" s="18" t="s">
+      <c r="L41" s="72">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M41" s="18" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A42" s="25"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
@@ -36779,9 +36973,10 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" s="12" customFormat="1" ht="16">
+      <c r="L42" s="72"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A43" s="21" t="s">
         <v>68</v>
       </c>
@@ -36811,12 +37006,13 @@
         <v>240</v>
       </c>
       <c r="K43" s="3"/>
-      <c r="L43" s="12" t="s">
+      <c r="L43" s="72"/>
+      <c r="M43" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" ht="16">
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" ht="16">
       <c r="A44" s="21"/>
       <c r="B44" s="26"/>
       <c r="C44" s="34"/>
@@ -36827,7 +37023,7 @@
       <c r="H44" s="30"/>
       <c r="I44" s="14"/>
     </row>
-    <row r="45" spans="1:14" s="12" customFormat="1" ht="16">
+    <row r="45" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A45" s="21" t="s">
         <v>224</v>
       </c>
@@ -36857,9 +37053,10 @@
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" s="12" customFormat="1" ht="16">
+      <c r="L45" s="72"/>
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A46" s="21"/>
       <c r="B46" s="19" t="s">
         <v>66</v>
@@ -36885,9 +37082,10 @@
       <c r="I46" s="37"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="N46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" ht="16">
+      <c r="L46" s="72"/>
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="1:15" ht="16">
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="34"/>
@@ -36897,7 +37095,7 @@
       <c r="G47" s="30"/>
       <c r="H47" s="30"/>
     </row>
-    <row r="48" spans="1:14" ht="16">
+    <row r="48" spans="1:15" ht="16">
       <c r="A48" s="23" t="s">
         <v>57</v>
       </c>
@@ -36925,8 +37123,11 @@
       <c r="I48" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="16">
+      <c r="L48" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="16">
       <c r="A49" s="23"/>
       <c r="B49" s="19" t="s">
         <v>60</v>
@@ -36949,9 +37150,12 @@
       <c r="H49" s="29">
         <v>-7.1730000000000002E-2</v>
       </c>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" ht="16">
+      <c r="L49" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M49" s="18"/>
+    </row>
+    <row r="50" spans="1:13" ht="16">
       <c r="A50" s="21"/>
       <c r="B50" s="19" t="s">
         <v>62</v>
@@ -36974,9 +37178,12 @@
       <c r="H50" s="29">
         <v>-0.41354000000000002</v>
       </c>
-      <c r="L50" s="18"/>
-    </row>
-    <row r="51" spans="1:12" ht="16">
+      <c r="L50" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M50" s="18"/>
+    </row>
+    <row r="51" spans="1:13" ht="16">
       <c r="A51" s="21"/>
       <c r="B51" s="19" t="s">
         <v>64</v>
@@ -36999,8 +37206,11 @@
       <c r="H51" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="16">
+      <c r="L51" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="16">
       <c r="A52" s="21"/>
       <c r="B52" s="19"/>
       <c r="C52" s="34"/>
@@ -37010,7 +37220,7 @@
       <c r="G52" s="30"/>
       <c r="H52" s="30"/>
     </row>
-    <row r="53" spans="1:12" ht="16">
+    <row r="53" spans="1:13" ht="16">
       <c r="B53" s="19" t="s">
         <v>90</v>
       </c>
@@ -37032,11 +37242,11 @@
       <c r="H53" s="29">
         <v>-0.33476</v>
       </c>
-      <c r="L53" s="12" t="s">
+      <c r="M53" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="16">
+    <row r="54" spans="1:13" ht="16">
       <c r="B54" s="26" t="s">
         <v>91</v>
       </c>
@@ -37058,11 +37268,11 @@
       <c r="H54" s="29">
         <v>-0.25944</v>
       </c>
-      <c r="L54" s="12" t="s">
+      <c r="M54" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16">
+    <row r="55" spans="1:13" ht="16">
       <c r="A55" s="21"/>
       <c r="B55" s="19" t="s">
         <v>92</v>
@@ -37086,7 +37296,7 @@
         <v>-0.52005999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="16">
+    <row r="56" spans="1:13" ht="16">
       <c r="A56" s="21"/>
       <c r="B56" s="26" t="s">
         <v>93</v>
@@ -37110,7 +37320,7 @@
         <v>0.21389</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="16">
+    <row r="57" spans="1:13" ht="16">
       <c r="A57" s="21"/>
       <c r="B57" s="26" t="s">
         <v>94</v>
@@ -37134,7 +37344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="16">
+    <row r="58" spans="1:13" ht="16">
       <c r="A58"/>
       <c r="B58" s="19" t="s">
         <v>95</v>
@@ -37158,7 +37368,7 @@
         <v>-0.22592999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="16">
+    <row r="59" spans="1:13" ht="16">
       <c r="A59" s="27"/>
       <c r="B59" s="24" t="s">
         <v>96</v>
@@ -37182,7 +37392,7 @@
         <v>-0.67791000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="16">
+    <row r="60" spans="1:13" ht="16">
       <c r="A60" s="27"/>
       <c r="B60" t="s">
         <v>97</v>
@@ -37206,7 +37416,7 @@
         <v>-1.9220000000000001E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="16">
+    <row r="61" spans="1:13" ht="16">
       <c r="A61"/>
       <c r="B61" t="s">
         <v>98</v>
@@ -37230,7 +37440,7 @@
         <v>-0.22169</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="16">
+    <row r="62" spans="1:13" ht="16">
       <c r="A62"/>
       <c r="B62" t="s">
         <v>99</v>
@@ -37254,7 +37464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="16">
+    <row r="63" spans="1:13" ht="16">
       <c r="A63"/>
       <c r="B63" t="s">
         <v>100</v>
@@ -37278,7 +37488,7 @@
         <v>-0.64468999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="16">
+    <row r="64" spans="1:13" ht="16">
       <c r="A64"/>
       <c r="B64" t="s">
         <v>101</v>
@@ -44148,10 +44358,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -44160,15 +44370,15 @@
     <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -44193,11 +44403,14 @@
       <c r="H1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>173</v>
       </c>
@@ -44216,11 +44429,14 @@
       </c>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="60" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="55"/>
       <c r="B3" s="63" t="s">
         <v>81</v>
@@ -44235,11 +44451,14 @@
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="60" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="55"/>
       <c r="B4" s="63" t="s">
         <v>20</v>
@@ -44254,11 +44473,14 @@
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="60" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="55"/>
       <c r="B5" s="63" t="s">
         <v>21</v>
@@ -44273,11 +44495,14 @@
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="60" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="55"/>
       <c r="B6" s="63" t="s">
         <v>19</v>
@@ -44292,9 +44517,12 @@
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="55"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="60"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="55"/>
       <c r="B7" s="55"/>
       <c r="C7" s="16"/>
@@ -44303,11 +44531,12 @@
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="73"/>
+      <c r="J7" s="60" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="39" t="s">
         <v>174</v>
       </c>
@@ -44329,9 +44558,12 @@
       <c r="H8" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+      <c r="I8" s="74">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="39"/>
       <c r="B9" s="14" t="s">
         <v>175</v>
@@ -44345,17 +44577,21 @@
       <c r="E9" s="43">
         <v>0</v>
       </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="I9" s="74">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="39"/>
       <c r="B10" s="14"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="42"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="I10" s="74"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="39" t="s">
         <v>176</v>
       </c>
@@ -44377,11 +44613,14 @@
       <c r="H11" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="74">
+        <v>2.1</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="39"/>
       <c r="B12" s="14" t="s">
         <v>66</v>
@@ -44395,19 +44634,23 @@
       <c r="E12" s="46">
         <v>0</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="74">
+        <v>2.1</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="39"/>
       <c r="B13" s="14"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="44"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13" s="74"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="69" t="s">
         <v>177</v>
       </c>
@@ -44429,9 +44672,12 @@
       <c r="G14" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14" s="74">
+        <v>1.4</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="69"/>
       <c r="B15" s="14" t="s">
         <v>189</v>
@@ -44445,9 +44691,12 @@
       <c r="E15" s="44">
         <v>-0.31792999999999999</v>
       </c>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="74">
+        <v>1.4</v>
+      </c>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="47"/>
       <c r="B16" s="14" t="s">
         <v>74</v>
@@ -44461,17 +44710,21 @@
       <c r="E16" s="46">
         <v>0</v>
       </c>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" s="74">
+        <v>1.4</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="39"/>
       <c r="B17" s="14"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="44"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="74"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="39" t="s">
         <v>178</v>
       </c>
@@ -44490,9 +44743,12 @@
       <c r="F18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18" s="74">
+        <v>1.6</v>
+      </c>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="39"/>
       <c r="B19" s="14" t="s">
         <v>179</v>
@@ -44506,17 +44762,21 @@
       <c r="E19" s="46">
         <v>0</v>
       </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="74">
+        <v>1.6</v>
+      </c>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="39"/>
       <c r="B20" s="14"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="44"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="I20" s="74"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="39" t="s">
         <v>180</v>
       </c>
@@ -44538,9 +44798,12 @@
       <c r="G21" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1">
+      <c r="I21" s="74">
+        <v>1.7</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="39"/>
       <c r="B22" s="14" t="s">
         <v>83</v>
@@ -44555,9 +44818,12 @@
         <v>0.21873999999999999</v>
       </c>
       <c r="G22" s="14"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1">
+      <c r="I22" s="74">
+        <v>1.7</v>
+      </c>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="A23" s="39"/>
       <c r="B23" s="14" t="s">
         <v>84</v>
@@ -44574,9 +44840,12 @@
       <c r="G23" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="I23" s="74">
+        <v>1.7</v>
+      </c>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="A24" s="39"/>
       <c r="B24" s="14" t="s">
         <v>76</v>
@@ -44593,17 +44862,21 @@
       <c r="G24" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24" s="74">
+        <v>1.7</v>
+      </c>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="39"/>
       <c r="B25" s="14"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="44"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="74"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="B26" s="40"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
@@ -44612,9 +44885,10 @@
       <c r="E26" s="44">
         <v>-4.6809999999999997E-2</v>
       </c>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26" s="74"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="47"/>
       <c r="B27" s="40"/>
       <c r="C27" s="16"/>
@@ -44624,9 +44898,10 @@
       <c r="E27" s="44">
         <v>1.5200000000000001E-3</v>
       </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27" s="74"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="47"/>
       <c r="B28" s="40"/>
       <c r="C28" s="16"/>
@@ -44636,9 +44911,10 @@
       <c r="E28" s="44">
         <v>-3.4199999999999999E-3</v>
       </c>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" ht="15">
+      <c r="I28" s="74"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" ht="15">
       <c r="A29" s="47" t="s">
         <v>181</v>
       </c>
@@ -44656,19 +44932,23 @@
       <c r="G29" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="74">
+        <v>1.2</v>
+      </c>
+      <c r="J29" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" s="39"/>
       <c r="B30" s="40"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
       <c r="E30" s="44"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" s="74"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="39" t="s">
         <v>183</v>
       </c>
@@ -44685,17 +44965,21 @@
       <c r="F31" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="I31" s="74">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="39"/>
       <c r="B32" s="41"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="44"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="I32" s="74"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="39" t="s">
         <v>185</v>
       </c>
@@ -44715,17 +44999,21 @@
       <c r="G33" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="I33" s="74">
+        <v>1.5</v>
+      </c>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="39"/>
       <c r="B34" s="14"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
       <c r="E34" s="44"/>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="I34" s="74"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="39" t="s">
         <v>186</v>
       </c>
@@ -44745,17 +45033,21 @@
       <c r="G35" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="I35" s="74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="39"/>
       <c r="B36" s="14"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
       <c r="E36" s="44"/>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="I36" s="74"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="39" t="s">
         <v>187</v>
       </c>
@@ -44775,23 +45067,28 @@
       <c r="G37" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="I37" s="74">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="44"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="I38" s="74"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="39"/>
       <c r="B39" s="40"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
       <c r="E39" s="44"/>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="I39" s="74"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="69"/>
       <c r="B40" s="3" t="s">
         <v>191</v>
@@ -44805,11 +45102,12 @@
       <c r="E40" s="44">
         <v>-0.27877999999999997</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I40" s="74"/>
+      <c r="J40" s="12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:10">
       <c r="A41" s="69"/>
       <c r="B41" s="3" t="s">
         <v>192</v>
@@ -44823,9 +45121,10 @@
       <c r="E41" s="44">
         <v>0.34847</v>
       </c>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="I41" s="74"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10">
       <c r="B42" s="3" t="s">
         <v>193</v>
       </c>
@@ -44838,9 +45137,10 @@
       <c r="E42" s="46">
         <v>0</v>
       </c>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="I42" s="74"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="B43" s="3" t="s">
         <v>194</v>
       </c>
@@ -44853,9 +45153,10 @@
       <c r="E43" s="46">
         <v>0</v>
       </c>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="I43" s="74"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="B44" s="3" t="s">
         <v>195</v>
       </c>
@@ -44868,9 +45169,10 @@
       <c r="E44" s="46">
         <v>0</v>
       </c>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="I44" s="74"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="B45" s="3" t="s">
         <v>196</v>
       </c>
@@ -44883,9 +45185,10 @@
       <c r="E45" s="46">
         <v>0</v>
       </c>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="I45" s="74"/>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="B46" s="3" t="s">
         <v>197</v>
       </c>
@@ -44898,9 +45201,10 @@
       <c r="E46" s="46">
         <v>0</v>
       </c>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="I46" s="74"/>
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="B47" s="3" t="s">
         <v>198</v>
       </c>
@@ -44913,7 +45217,8 @@
       <c r="E47" s="46">
         <v>0</v>
       </c>
-      <c r="I47" s="12"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="12"/>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" s="14"/>
@@ -44950,6 +45255,7 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A40:A41"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
lung centres rendered from xlsx
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D97906-5B84-D148-8A74-91FA8F871B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453BDCE6-D44C-2942-ADDB-2B508F022853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="4040" windowWidth="29540" windowHeight="19040" activeTab="1" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="3620" yWindow="1140" windowWidth="29540" windowHeight="19040" activeTab="1" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -904,21 +904,6 @@
     <t>:link</t>
   </si>
   <si>
-    <t>lung/assets/pap.jpg</t>
-  </si>
-  <si>
-    <t>lung/assets/hare.jpg</t>
-  </si>
-  <si>
-    <t>lung/assets/birm.jpg</t>
-  </si>
-  <si>
-    <t>lung/assets/man.jpg</t>
-  </si>
-  <si>
-    <t>lung/assets/new.jpg</t>
-  </si>
-  <si>
     <t>https://www.rbht.nhs.uk/our-services/lung/transplantation-lung</t>
   </si>
   <si>
@@ -932,6 +917,21 @@
   </si>
   <si>
     <t>http://www.newcastle-hospitals.org.uk/services/cardiothoracic_services_cardiopulmonary-heart-andor-lung-transplant.aspx</t>
+  </si>
+  <si>
+    <t>assets/lung/pap.png</t>
+  </si>
+  <si>
+    <t>assets/lung/hare.png</t>
+  </si>
+  <si>
+    <t>assets/lung/birm.png</t>
+  </si>
+  <si>
+    <t>assets/lung/man.png</t>
+  </si>
+  <si>
+    <t>assets/lung/new.png</t>
   </si>
 </sst>
 </file>
@@ -1287,15 +1287,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -13047,7 +13047,7 @@
       <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
-      <c r="A34" s="77"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="14" t="s">
         <v>94</v>
       </c>
@@ -13065,7 +13065,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="77"/>
+      <c r="A35" s="79"/>
       <c r="B35" s="14" t="s">
         <v>90</v>
       </c>
@@ -13372,7 +13372,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13406,11 +13406,11 @@
       <c r="B2" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>292</v>
+      <c r="C2" s="76" t="s">
+        <v>287</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="E2" t="s">
         <v>280</v>
@@ -13423,11 +13423,11 @@
       <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>291</v>
+      <c r="C3" s="76" t="s">
+        <v>286</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E3" t="s">
         <v>282</v>
@@ -13440,11 +13440,11 @@
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="77" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="59" t="s">
         <v>293</v>
-      </c>
-      <c r="D4" s="59" t="s">
-        <v>288</v>
       </c>
       <c r="E4" t="s">
         <v>279</v>
@@ -13457,11 +13457,11 @@
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="76" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="59" t="s">
         <v>294</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>289</v>
       </c>
       <c r="E5" t="s">
         <v>284</v>
@@ -13474,11 +13474,11 @@
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="59" t="s">
         <v>295</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>290</v>
       </c>
       <c r="E6" t="s">
         <v>283</v>
@@ -47111,7 +47111,7 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:13" ht="16">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="78" t="s">
         <v>75</v>
       </c>
       <c r="B16" s="19">
@@ -47149,7 +47149,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="16">
-      <c r="A17" s="76"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="22" t="s">
         <v>85</v>
       </c>
@@ -49147,7 +49147,7 @@
       <c r="C12" s="3">
         <v>0.79270650573773382</v>
       </c>
-      <c r="F12" s="77"/>
+      <c r="F12" s="79"/>
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:14">
@@ -49160,7 +49160,7 @@
       <c r="C13" s="3">
         <v>0.77714124234773851</v>
       </c>
-      <c r="F13" s="77"/>
+      <c r="F13" s="79"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="11" t="s">
@@ -55474,7 +55474,7 @@
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="79" t="s">
         <v>177</v>
       </c>
       <c r="B14" s="14">
@@ -55501,7 +55501,7 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="77"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="14" t="s">
         <v>189</v>
       </c>
@@ -55912,7 +55912,7 @@
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="77"/>
+      <c r="A40" s="79"/>
       <c r="B40" s="3" t="s">
         <v>191</v>
       </c>
@@ -55931,7 +55931,7 @@
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="77"/>
+      <c r="A41" s="79"/>
       <c r="B41" s="3" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
kidney home and tools.txt
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453BDCE6-D44C-2942-ADDB-2B508F022853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDEDAF-C741-7C4D-ABB8-D0F24CDAD849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1140" windowWidth="29540" windowHeight="19040" activeTab="1" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
     <sheet name="centres" sheetId="15" r:id="rId2"/>
-    <sheet name="waiting-baseline-cifs" sheetId="6" r:id="rId3"/>
-    <sheet name="waiting-baseline-vars" sheetId="4" r:id="rId4"/>
-    <sheet name="waiting-inputs" sheetId="5" r:id="rId5"/>
-    <sheet name="numerics" sheetId="7" r:id="rId6"/>
-    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId7"/>
-    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId8"/>
-    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId9"/>
-    <sheet name="from-listing-baseline-cifs" sheetId="13" r:id="rId10"/>
-    <sheet name="from-listing-baseline-vars" sheetId="14" r:id="rId11"/>
-    <sheet name="from-listing-inputs" sheetId="12" r:id="rId12"/>
+    <sheet name="tools" sheetId="16" r:id="rId3"/>
+    <sheet name="waiting-baseline-cifs" sheetId="6" r:id="rId4"/>
+    <sheet name="waiting-baseline-vars" sheetId="4" r:id="rId5"/>
+    <sheet name="waiting-inputs" sheetId="5" r:id="rId6"/>
+    <sheet name="numerics" sheetId="7" r:id="rId7"/>
+    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId8"/>
+    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId9"/>
+    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId10"/>
+    <sheet name="from-listing-baseline-cifs" sheetId="13" r:id="rId11"/>
+    <sheet name="from-listing-baseline-vars" sheetId="14" r:id="rId12"/>
+    <sheet name="from-listing-inputs" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3374" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="300">
   <si>
     <t>Notes</t>
   </si>
@@ -933,6 +934,18 @@
   <si>
     <t>assets/lung/new.png</t>
   </si>
+  <si>
+    <t>Competing risks</t>
+  </si>
+  <si>
+    <t>Survival post transplant</t>
+  </si>
+  <si>
+    <t>while waiting</t>
+  </si>
+  <si>
+    <t>over time</t>
+  </si>
 </sst>
 </file>
 
@@ -1695,6 +1708,911 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
+  <dimension ref="A1:J61"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="47.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A2" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="60" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="55"/>
+      <c r="B3" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="55"/>
+      <c r="B4" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="55"/>
+      <c r="B5" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="60" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="55"/>
+      <c r="B6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="60"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="42">
+        <v>-0.27407999999999999</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="I8" s="72">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1">
+      <c r="A9" s="39"/>
+      <c r="B9" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="43">
+        <v>0</v>
+      </c>
+      <c r="I9" s="72">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="42"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
+      <c r="A11" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="44">
+        <v>-0.29988999999999999</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="I11" s="72">
+        <v>2.1</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="39"/>
+      <c r="B12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="46">
+        <v>0</v>
+      </c>
+      <c r="I12" s="72">
+        <v>2.1</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="39"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="44"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="44">
+        <v>-0.51788000000000001</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" s="72">
+        <v>1.4</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="79"/>
+      <c r="B15" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" s="44">
+        <v>-0.31792999999999999</v>
+      </c>
+      <c r="I15" s="72">
+        <v>1.4</v>
+      </c>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="47"/>
+      <c r="B16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="46">
+        <v>0</v>
+      </c>
+      <c r="I16" s="72">
+        <v>1.4</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="39"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="44"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="44">
+        <v>-4.5809999999999997E-2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="72">
+        <v>1.6</v>
+      </c>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="39"/>
+      <c r="B19" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="46">
+        <v>0</v>
+      </c>
+      <c r="I19" s="72">
+        <v>1.6</v>
+      </c>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="39"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="44"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1">
+      <c r="A21" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="44">
+        <v>-0.49712000000000001</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1">
+      <c r="A22" s="39"/>
+      <c r="B22" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="44">
+        <v>0.21873999999999999</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="I22" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1">
+      <c r="A23" s="39"/>
+      <c r="B23" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="44">
+        <v>-0.13768</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="46">
+        <v>0</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="39"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="44"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" s="40"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E26" s="44">
+        <v>-4.6809999999999997E-2</v>
+      </c>
+      <c r="I26" s="72"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="47"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="E27" s="44">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="I27" s="72"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="47"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28" s="44">
+        <v>-3.4199999999999999E-3</v>
+      </c>
+      <c r="I28" s="72"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="E29" s="44"/>
+      <c r="F29" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I29" s="72">
+        <v>1.2</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="44"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="44">
+        <v>0.12</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I31" s="72">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="39"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="44"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="41"/>
+      <c r="C33" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="44">
+        <v>-1.8380000000000001E-2</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="I33" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="39"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="44"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" s="41"/>
+      <c r="C35" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="48">
+        <v>-5.1040000000000005E-4</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I35" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="39"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="44"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="44">
+        <v>-0.33889999999999998</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I37" s="72">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="44"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="44"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="79"/>
+      <c r="B40" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E40" s="44">
+        <v>-0.27877999999999997</v>
+      </c>
+      <c r="I40" s="72"/>
+      <c r="J40" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="79"/>
+      <c r="B41" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" s="44">
+        <v>0.34847</v>
+      </c>
+      <c r="I41" s="72"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="B42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="46">
+        <v>0</v>
+      </c>
+      <c r="I42" s="72"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="B43" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="46">
+        <v>0</v>
+      </c>
+      <c r="I43" s="72"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="B44" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" s="46">
+        <v>0</v>
+      </c>
+      <c r="I44" s="72"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="B45" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E45" s="46">
+        <v>0</v>
+      </c>
+      <c r="I45" s="72"/>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="46">
+        <v>0</v>
+      </c>
+      <c r="I46" s="72"/>
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="B47" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="E47" s="46">
+        <v>0</v>
+      </c>
+      <c r="I47" s="72"/>
+      <c r="J47" s="12"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="14"/>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" s="40"/>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="14"/>
+    </row>
+    <row r="56" spans="5:5">
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="5:5">
+      <c r="E57" s="40"/>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="5:5">
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="5:5">
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="5:5">
+      <c r="E61" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A40:A41"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF04EBC3-ECA7-4644-80EC-2F16BAB62C89}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
@@ -12298,7 +13216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E50BA8A-672F-1740-8DE6-439CBC2BCF16}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -12425,7 +13343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J53"/>
   <sheetViews>
@@ -13371,8 +14289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A6C1CE-31BA-6441-9BF7-3656CF7F494F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13497,6 +14415,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:L3206"/>
   <sheetViews>
@@ -46521,7 +47492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA849B77-A729-9F4B-AFFB-4400AE5F1FC9}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -46680,7 +47651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O72"/>
   <sheetViews>
@@ -48536,7 +49507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0253E0-6F04-2243-A5A9-874E3053166B}">
   <dimension ref="A1:J34"/>
   <sheetViews>
@@ -48960,7 +49931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
@@ -55049,7 +56020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -55177,909 +56148,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:J61"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="47.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="73" t="s">
-        <v>270</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A2" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="J2" s="60" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="55"/>
-      <c r="B3" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="60" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="55"/>
-      <c r="B4" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="J4" s="60" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="55"/>
-      <c r="B5" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="J5" s="60" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="55"/>
-      <c r="B6" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="J6" s="60"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="60" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="42">
-        <v>-0.27407999999999999</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="I8" s="72">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="43">
-        <v>0</v>
-      </c>
-      <c r="I9" s="72">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="42"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="A11" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="44">
-        <v>-0.29988999999999999</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="I11" s="72">
-        <v>2.1</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="39"/>
-      <c r="B12" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="46">
-        <v>0</v>
-      </c>
-      <c r="I12" s="72">
-        <v>2.1</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="44"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="44">
-        <v>-0.51788000000000001</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="I14" s="72">
-        <v>1.4</v>
-      </c>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="79"/>
-      <c r="B15" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="E15" s="44">
-        <v>-0.31792999999999999</v>
-      </c>
-      <c r="I15" s="72">
-        <v>1.4</v>
-      </c>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="46">
-        <v>0</v>
-      </c>
-      <c r="I16" s="72">
-        <v>1.4</v>
-      </c>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="44"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="44">
-        <v>-4.5809999999999997E-2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="72">
-        <v>1.6</v>
-      </c>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="46">
-        <v>0</v>
-      </c>
-      <c r="I19" s="72">
-        <v>1.6</v>
-      </c>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="44"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1">
-      <c r="A21" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="44">
-        <v>-0.49712000000000001</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="I21" s="72">
-        <v>1.7</v>
-      </c>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" s="44">
-        <v>0.21873999999999999</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="I22" s="72">
-        <v>1.7</v>
-      </c>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1">
-      <c r="A23" s="39"/>
-      <c r="B23" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="44">
-        <v>-0.13768</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I23" s="72">
-        <v>1.7</v>
-      </c>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="46">
-        <v>0</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I24" s="72">
-        <v>1.7</v>
-      </c>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="39"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="44"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="B26" s="40"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="E26" s="44">
-        <v>-4.6809999999999997E-2</v>
-      </c>
-      <c r="I26" s="72"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="47"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="E27" s="44">
-        <v>1.5200000000000001E-3</v>
-      </c>
-      <c r="I27" s="72"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="47"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="E28" s="44">
-        <v>-3.4199999999999999E-3</v>
-      </c>
-      <c r="I28" s="72"/>
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I29" s="72">
-        <v>1.2</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="39"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="44"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="44">
-        <v>0.12</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I31" s="72">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J31" s="12"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="39"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="44"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="44">
-        <v>-1.8380000000000001E-2</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="I33" s="72">
-        <v>1.5</v>
-      </c>
-      <c r="J33" s="12"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="39"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="44"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="48">
-        <v>-5.1040000000000005E-4</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="I35" s="72">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="39"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="44"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="44">
-        <v>-0.33889999999999998</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="I37" s="72">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="44"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="12"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="39"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="44"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="12"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="79"/>
-      <c r="B40" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="44">
-        <v>-0.27877999999999997</v>
-      </c>
-      <c r="I40" s="72"/>
-      <c r="J40" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="79"/>
-      <c r="B41" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E41" s="44">
-        <v>0.34847</v>
-      </c>
-      <c r="I41" s="72"/>
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="B42" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="E42" s="46">
-        <v>0</v>
-      </c>
-      <c r="I42" s="72"/>
-      <c r="J42" s="12"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="B43" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E43" s="46">
-        <v>0</v>
-      </c>
-      <c r="I43" s="72"/>
-      <c r="J43" s="12"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="B44" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="46">
-        <v>0</v>
-      </c>
-      <c r="I44" s="72"/>
-      <c r="J44" s="12"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="B45" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="E45" s="46">
-        <v>0</v>
-      </c>
-      <c r="I45" s="72"/>
-      <c r="J45" s="12"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="B46" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="E46" s="46">
-        <v>0</v>
-      </c>
-      <c r="I46" s="72"/>
-      <c r="J46" s="12"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="B47" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E47" s="46">
-        <v>0</v>
-      </c>
-      <c r="I47" s="72"/>
-      <c r="J47" s="12"/>
-    </row>
-    <row r="49" spans="5:5">
-      <c r="E49" s="14"/>
-    </row>
-    <row r="53" spans="5:5">
-      <c r="E53" s="40"/>
-    </row>
-    <row r="54" spans="5:5">
-      <c r="E54" s="14"/>
-    </row>
-    <row r="55" spans="5:5">
-      <c r="E55" s="14"/>
-    </row>
-    <row r="56" spans="5:5">
-      <c r="E56" s="14"/>
-    </row>
-    <row r="57" spans="5:5">
-      <c r="E57" s="40"/>
-    </row>
-    <row r="58" spans="5:5">
-      <c r="E58" s="14"/>
-    </row>
-    <row r="59" spans="5:5">
-      <c r="E59" s="14"/>
-    </row>
-    <row r="60" spans="5:5">
-      <c r="E60" s="14"/>
-    </row>
-    <row r="61" spans="5:5">
-      <c r="E61" s="40"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A40:A41"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
generic mobile home from config
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDEDAF-C741-7C4D-ABB8-D0F24CDAD849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620AFCBF-FD25-8440-A6AC-C9BC68E7D27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="1" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -884,9 +884,6 @@
     <t>new</t>
   </si>
   <si>
-    <t>Queen Elizabeth's Hospital</t>
-  </si>
-  <si>
     <t>Royal Papworth Hospital</t>
   </si>
   <si>
@@ -894,12 +891,6 @@
   </si>
   <si>
     <t>Harefield Hospital</t>
-  </si>
-  <si>
-    <t>Institute of Transplantation</t>
-  </si>
-  <si>
-    <t>University Hospital</t>
   </si>
   <si>
     <t>:link</t>
@@ -945,6 +936,15 @@
   </si>
   <si>
     <t>over time</t>
+  </si>
+  <si>
+    <t>Manchester University Hospital</t>
+  </si>
+  <si>
+    <t>Birmingham Queen Elizabeth's Hospital</t>
+  </si>
+  <si>
+    <t>Newcastle Institute of Transplantation</t>
   </si>
 </sst>
 </file>
@@ -14289,8 +14289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A6C1CE-31BA-6441-9BF7-3656CF7F494F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14308,13 +14308,13 @@
         <v>271</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
         <v>277</v>
       </c>
       <c r="E1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14325,13 +14325,13 @@
         <v>80</v>
       </c>
       <c r="C2" s="76" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14342,13 +14342,13 @@
         <v>81</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -14359,13 +14359,13 @@
         <v>20</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E4" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14376,13 +14376,13 @@
         <v>21</v>
       </c>
       <c r="C5" s="76" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E5" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -14393,13 +14393,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -14418,8 +14418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14430,36 +14430,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="B1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C1" t="s">
-        <v>281</v>
+      <c r="B1" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="35" t="s">
         <v>172</v>
       </c>
       <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
         <v>296</v>
-      </c>
-      <c r="C2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C3" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -47655,7 +47655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reinstated survival from listing
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620AFCBF-FD25-8440-A6AC-C9BC68E7D27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558288FD-2D3A-0E42-9794-1F32DB9716B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="1" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="302">
   <si>
     <t>Notes</t>
   </si>
@@ -946,6 +946,12 @@
   <si>
     <t>Newcastle Institute of Transplantation</t>
   </si>
+  <si>
+    <t>Survival from listing</t>
+  </si>
+  <si>
+    <t>from listing</t>
+  </si>
 </sst>
 </file>
 
@@ -14289,7 +14295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A6C1CE-31BA-6441-9BF7-3656CF7F494F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -14416,10 +14422,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39:F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14460,6 +14466,17 @@
       </c>
       <c r="C3" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed centre linking issue
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558288FD-2D3A-0E42-9794-1F32DB9716B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BA8C89-30A9-3A41-ACA0-B7A9251F480C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="-19960" windowWidth="29540" windowHeight="19040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
@@ -932,12 +932,6 @@
     <t>Survival post transplant</t>
   </si>
   <si>
-    <t>while waiting</t>
-  </si>
-  <si>
-    <t>over time</t>
-  </si>
-  <si>
     <t>Manchester University Hospital</t>
   </si>
   <si>
@@ -950,7 +944,13 @@
     <t>Survival from listing</t>
   </si>
   <si>
-    <t>from listing</t>
+    <t>Survival expectations after a lung transplant</t>
+  </si>
+  <si>
+    <t>Survival expectations from the time that a patient is listed for a transplant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The risks of possible outcomes while waiting for a transplant </t>
   </si>
 </sst>
 </file>
@@ -14371,7 +14371,7 @@
         <v>290</v>
       </c>
       <c r="E4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14388,7 +14388,7 @@
         <v>291</v>
       </c>
       <c r="E5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -14405,7 +14405,7 @@
         <v>292</v>
       </c>
       <c r="E6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -14425,14 +14425,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="113" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -14454,7 +14454,7 @@
         <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14465,7 +14465,7 @@
         <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14473,10 +14473,10 @@
         <v>223</v>
       </c>
       <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" t="s">
         <v>300</v>
-      </c>
-      <c r="C4" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to transform data on store
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97736B2-BDE3-614D-9279-0E41D3F857FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE45F594-E729-AE46-A594-AFF4930894A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="-22320" windowWidth="29540" windowHeight="19040" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="4000" yWindow="-22320" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="292">
   <si>
     <t>Notes</t>
   </si>
@@ -2458,7 +2458,7 @@
   <dimension ref="A1:N1015"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:I25"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13189,7 +13189,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -47384,7 +47384,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="C30" sqref="C30:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -48081,104 +48081,110 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:15" ht="16">
-      <c r="A25" s="25"/>
-      <c r="B25"/>
-      <c r="C25" s="16"/>
+      <c r="A25" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="D25" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="69">
+        <v>1.06</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="16">
+      <c r="A26" s="25"/>
+      <c r="B26"/>
+      <c r="C26" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E26" s="29">
         <v>0.28376000000000001</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F26" s="29">
         <v>3.2649999999999998E-2</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G26" s="29">
         <v>-0.52522999999999997</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H26" s="29">
         <v>-0.1124</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="M25" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="16">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="E26" s="29">
-        <v>0.23757</v>
-      </c>
-      <c r="F26" s="29">
-        <v>0.13516</v>
-      </c>
-      <c r="G26" s="29">
-        <v>-0.59109</v>
-      </c>
-      <c r="H26" s="29">
-        <v>0.25652000000000003</v>
-      </c>
+      <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
+      <c r="M26" s="12" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="16">
       <c r="A27"/>
       <c r="B27"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="D27" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E27" s="29">
-        <v>-0.69055999999999995</v>
+        <v>0.23757</v>
       </c>
       <c r="F27" s="29">
-        <v>-0.45455000000000001</v>
+        <v>0.13516</v>
       </c>
       <c r="G27" s="29">
-        <v>1.65744</v>
+        <v>-0.59109</v>
       </c>
       <c r="H27" s="29">
-        <v>-0.47989999999999999</v>
-      </c>
-      <c r="I27" s="14"/>
+        <v>0.25652000000000003</v>
+      </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:15" ht="16">
-      <c r="A28" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="24"/>
+      <c r="A28"/>
+      <c r="B28"/>
       <c r="C28" s="16" t="s">
         <v>109</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>230</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="E28" s="29">
+        <v>-0.69055999999999995</v>
+      </c>
+      <c r="F28" s="29">
+        <v>-0.45455000000000001</v>
+      </c>
+      <c r="G28" s="29">
+        <v>1.65744</v>
+      </c>
+      <c r="H28" s="29">
+        <v>-0.47989999999999999</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="69">
-        <v>1.06</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="29" spans="1:15" ht="16">
       <c r="A29" s="25"/>
@@ -48193,107 +48199,113 @@
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:15" ht="16">
-      <c r="A30" s="25"/>
+    <row r="30" spans="1:15" ht="17" customHeight="1">
+      <c r="A30" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="B30" s="24"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="D30" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="29">
-        <v>5.0699999999999999E-3</v>
-      </c>
-      <c r="F30" s="29">
-        <v>6.0069999999999998E-2</v>
-      </c>
-      <c r="G30" s="29">
-        <v>-1.9789999999999999E-2</v>
-      </c>
-      <c r="H30" s="29">
-        <v>-3.1900000000000001E-3</v>
-      </c>
-      <c r="I30"/>
-      <c r="J30" s="14"/>
+        <v>248</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>241</v>
+      </c>
       <c r="K30" s="14"/>
+      <c r="L30" s="69">
+        <v>1.01</v>
+      </c>
       <c r="M30" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="12" customFormat="1" ht="16">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="16">
       <c r="A31" s="25"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="16"/>
+      <c r="C31" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="D31" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" s="32">
-        <v>-4.2719999999999998E-4</v>
+        <v>132</v>
+      </c>
+      <c r="E31" s="29">
+        <v>5.0699999999999999E-3</v>
       </c>
       <c r="F31" s="29">
-        <v>-1.58E-3</v>
+        <v>6.0069999999999998E-2</v>
       </c>
       <c r="G31" s="29">
-        <v>1.58E-3</v>
-      </c>
-      <c r="H31" s="32">
-        <v>3.3849999999999999E-4</v>
+        <v>-1.9789999999999999E-2</v>
+      </c>
+      <c r="H31" s="29">
+        <v>-3.1900000000000001E-3</v>
       </c>
       <c r="I31"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="13"/>
-      <c r="O31" s="3"/>
+      <c r="M31" s="12" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A32" s="25"/>
       <c r="B32" s="24"/>
-      <c r="C32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="D32" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="29">
-        <v>1.92E-3</v>
+        <v>134</v>
+      </c>
+      <c r="E32" s="32">
+        <v>-4.2719999999999998E-4</v>
       </c>
       <c r="F32" s="29">
-        <v>4.47E-3</v>
+        <v>-1.58E-3</v>
       </c>
       <c r="G32" s="29">
-        <v>-5.77E-3</v>
+        <v>1.58E-3</v>
       </c>
       <c r="H32" s="32">
-        <v>-8.1760000000000003E-4</v>
-      </c>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
+        <v>3.3849999999999999E-4</v>
+      </c>
+      <c r="I32"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="69"/>
+      <c r="M32" s="13"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:15" ht="16">
-      <c r="A33" s="25" t="s">
-        <v>68</v>
-      </c>
+    <row r="33" spans="1:15" s="12" customFormat="1" ht="16">
+      <c r="A33" s="25"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>241</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E33" s="29">
+        <v>1.92E-3</v>
+      </c>
+      <c r="F33" s="29">
+        <v>4.47E-3</v>
+      </c>
+      <c r="G33" s="29">
+        <v>-5.77E-3</v>
+      </c>
+      <c r="H33" s="32">
+        <v>-8.1760000000000003E-4</v>
+      </c>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
       <c r="K33" s="14"/>
-      <c r="L33" s="69">
-        <v>1.01</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>164</v>
-      </c>
+      <c r="L33" s="69"/>
+      <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A34" s="25"/>
@@ -55617,7 +55629,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fixed blood-group no-refresh issue
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE45F594-E729-AE46-A594-AFF4930894A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DD1BC7-FB10-5E43-AEA9-9D652F8CFFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="-22320" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
@@ -13188,8 +13188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
secondary colors for uinouts?
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DD1BC7-FB10-5E43-AEA9-9D652F8CFFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED69C36-05A9-274A-BF63-A3707F1C31BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="-22320" windowWidth="29540" windowHeight="19040" firstSheet="3" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="2500" yWindow="460" windowWidth="29540" windowHeight="19040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1679,7 +1679,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:XFD7"/>
+      <selection activeCell="C2" sqref="C2:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13188,7 +13188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -47383,8 +47383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C33"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47553,7 +47553,7 @@
         <v>7.6469999999999996E-2</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>125</v>
@@ -47699,7 +47699,7 @@
         <v>-0.12415</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>228</v>

</xml_diff>

<commit_message>
drive factor registrations from db - WIP
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED69C36-05A9-274A-BF63-A3707F1C31BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7C382-1B7E-6541-97F3-8FC842F5A9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="460" windowWidth="29540" windowHeight="19040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
@@ -47383,20 +47383,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="42.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="10.5" style="3" customWidth="1"/>
@@ -48404,7 +48404,9 @@
         <v>229</v>
       </c>
       <c r="K37" s="3"/>
-      <c r="L37" s="69"/>
+      <c r="L37" s="69">
+        <v>1.1299999999999999</v>
+      </c>
       <c r="M37" s="12" t="s">
         <v>165</v>
       </c>
@@ -48451,7 +48453,9 @@
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="69"/>
+      <c r="L39" s="69">
+        <v>1.1399999999999999</v>
+      </c>
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" s="12" customFormat="1" ht="16">

</xml_diff>

<commit_message>
factors are now data driven
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7C382-1B7E-6541-97F3-8FC842F5A9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FCBBEC-2281-C14F-A1E7-DE211D932027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="460" windowWidth="29540" windowHeight="19040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="640" yWindow="1380" windowWidth="29680" windowHeight="19040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -47383,20 +47383,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="42.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="38" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="10.5" style="3" customWidth="1"/>

</xml_diff>

<commit_message>
Moved index columns to A and B
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FCBBEC-2281-C14F-A1E7-DE211D932027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78581FA-7D15-0E4A-B338-F1B46D261B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1380" windowWidth="29680" windowHeight="19040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="3000" yWindow="1100" windowWidth="29680" windowHeight="19040" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1097,7 +1097,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1276,6 +1276,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1678,16 +1690,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C41"/>
+    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="47.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
@@ -1698,16 +1710,16 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>291</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>246</v>
@@ -1729,17 +1741,17 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>198</v>
       </c>
       <c r="E2" s="42">
         <v>-0.27407999999999999</v>
@@ -1756,15 +1768,15 @@
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>199</v>
       </c>
       <c r="E3" s="43">
         <v>0</v>
@@ -1775,26 +1787,26 @@
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="42"/>
       <c r="I4" s="70"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="44">
         <v>-0.29988999999999999</v>
@@ -1813,15 +1825,15 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="39"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="E6" s="46">
         <v>0</v>
@@ -1834,26 +1846,26 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="39"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="44"/>
       <c r="I7" s="70"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="14">
+      <c r="D8" s="14">
         <v>0</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="E8" s="44">
         <v>-0.51788000000000001</v>
@@ -1870,15 +1882,15 @@
       <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="76"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="76"/>
+      <c r="D9" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="E9" s="44">
         <v>-0.31792999999999999</v>
@@ -1889,15 +1901,15 @@
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="47"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>162</v>
       </c>
       <c r="E10" s="46">
         <v>0</v>
@@ -1908,26 +1920,26 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="39"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="44"/>
       <c r="I11" s="70"/>
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="E12" s="44">
         <v>-4.5809999999999997E-2</v>
@@ -1941,15 +1953,15 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="E13" s="46">
         <v>0</v>
@@ -1960,26 +1972,26 @@
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="44"/>
       <c r="I14" s="70"/>
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="E15" s="44">
         <v>-0.49712000000000001</v>
@@ -1996,15 +2008,15 @@
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="E16" s="44">
         <v>0.21873999999999999</v>
@@ -2016,15 +2028,15 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="E17" s="44">
         <v>-0.13768</v>
@@ -2038,15 +2050,15 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="E18" s="46">
         <v>0</v>
@@ -2060,20 +2072,20 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="44"/>
       <c r="I19" s="70"/>
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="B20" s="40"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16" t="s">
         <v>253</v>
       </c>
+      <c r="D20" s="40"/>
       <c r="E20" s="44">
         <v>-4.6809999999999997E-2</v>
       </c>
@@ -2081,12 +2093,12 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="47"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16" t="s">
         <v>254</v>
       </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="44">
         <v>1.5200000000000001E-3</v>
       </c>
@@ -2094,12 +2106,12 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="47"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16" t="s">
         <v>255</v>
       </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="44">
         <v>-3.4199999999999999E-3</v>
       </c>
@@ -2107,16 +2119,16 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>256</v>
-      </c>
+      <c r="D23" s="40"/>
       <c r="E23" s="44"/>
       <c r="F23" s="3" t="s">
         <v>129</v>
@@ -2132,25 +2144,25 @@
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="44"/>
       <c r="I24" s="70"/>
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D25" s="41"/>
       <c r="E25" s="44">
         <v>0.12</v>
       </c>
@@ -2163,25 +2175,25 @@
       <c r="J25" s="12"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="39"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="44"/>
       <c r="I26" s="70"/>
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D27" s="41"/>
       <c r="E27" s="44">
         <v>-1.8380000000000001E-2</v>
       </c>
@@ -2197,25 +2209,25 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="39"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="44"/>
       <c r="I28" s="70"/>
       <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D29" s="41"/>
       <c r="E29" s="48">
         <v>-5.1040000000000005E-4</v>
       </c>
@@ -2231,25 +2243,25 @@
       <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="39"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="44"/>
       <c r="I30" s="70"/>
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D31" s="41"/>
       <c r="E31" s="44">
         <v>-0.33889999999999998</v>
       </c>
@@ -2265,31 +2277,31 @@
       <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="E32" s="44"/>
       <c r="I32" s="70"/>
       <c r="J32" s="12"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
       <c r="E33" s="44"/>
       <c r="I33" s="70"/>
       <c r="J33" s="12"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="76"/>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="76"/>
+      <c r="D34" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>203</v>
       </c>
       <c r="E34" s="44">
         <v>-0.27877999999999997</v>
@@ -2300,15 +2312,15 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="76"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C35" s="76"/>
+      <c r="D35" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>204</v>
       </c>
       <c r="E35" s="44">
         <v>0.34847</v>
@@ -2317,14 +2329,14 @@
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="E36" s="46">
         <v>0</v>
@@ -2333,14 +2345,14 @@
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>205</v>
       </c>
       <c r="E37" s="46">
         <v>0</v>
@@ -2349,14 +2361,14 @@
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="B38" s="3" t="s">
+      <c r="A38" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>207</v>
       </c>
       <c r="E38" s="46">
         <v>0</v>
@@ -2365,14 +2377,14 @@
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>208</v>
       </c>
       <c r="E39" s="46">
         <v>0</v>
@@ -2381,14 +2393,14 @@
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>209</v>
       </c>
       <c r="E40" s="46">
         <v>0</v>
@@ -2397,14 +2409,14 @@
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>210</v>
       </c>
       <c r="E41" s="46">
         <v>0</v>
@@ -2444,8 +2456,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13188,16 +13200,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="3"/>
     <col min="9" max="9" width="8.83203125" style="72"/>
@@ -13207,16 +13219,16 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>291</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>247</v>
@@ -13238,17 +13250,17 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="3">
         <v>2.3810000000000001E-2</v>
@@ -13262,15 +13274,15 @@
       <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="39"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -13281,25 +13293,25 @@
       <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="39"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="42"/>
       <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="E5" s="3">
         <v>-0.14127000000000001</v>
@@ -13313,15 +13325,15 @@
       <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="39"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -13332,25 +13344,25 @@
       <c r="J6" s="60"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="39"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="44"/>
       <c r="J7" s="60"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="E8" s="3">
         <v>-6.2619999999999995E-2</v>
@@ -13364,15 +13376,15 @@
       <c r="J8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="A9" s="50"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="E9" s="3">
         <v>-9.4829999999999998E-2</v>
@@ -13383,15 +13395,15 @@
       <c r="J9" s="60"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="39"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>62</v>
       </c>
       <c r="E10" s="3">
         <v>-2.5999999999999999E-3</v>
@@ -13402,15 +13414,15 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="39"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -13421,25 +13433,25 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="39"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="44"/>
       <c r="J12" s="60"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="E13" s="3">
         <v>0.44096000000000002</v>
@@ -13453,15 +13465,15 @@
       <c r="J13" s="60"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="E14" s="3">
         <v>0.51051999999999997</v>
@@ -13472,15 +13484,15 @@
       <c r="J14" s="60"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="39"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="E15" s="3">
         <v>0.62370000000000003</v>
@@ -13491,15 +13503,15 @@
       <c r="J15" s="60"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="39"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -13510,25 +13522,25 @@
       <c r="J16" s="60"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="44"/>
       <c r="J17" s="60"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="E18" s="3">
         <v>8.8590000000000002E-2</v>
@@ -13542,15 +13554,15 @@
       <c r="J18" s="60"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -13561,25 +13573,25 @@
       <c r="J19" s="60"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20" s="50"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="44"/>
       <c r="J20" s="60"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="D21" s="40" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="E21" s="3">
         <v>-0.71755999999999998</v>
@@ -13593,15 +13605,15 @@
       <c r="J21" s="60"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
-      <c r="A22" s="50"/>
-      <c r="B22" s="40" t="s">
+      <c r="A22" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="50"/>
+      <c r="D22" s="40" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -13612,24 +13624,24 @@
       <c r="J22" s="60"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1">
-      <c r="A23" s="50"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="44"/>
       <c r="J23" s="60"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="3">
         <v>2.82E-3</v>
       </c>
@@ -13644,24 +13656,24 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="39"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="44"/>
       <c r="J25" s="60"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D26" s="41"/>
       <c r="E26" s="3">
         <v>-1.452E-2</v>
       </c>
@@ -13674,23 +13686,23 @@
       <c r="J26" s="60"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="39"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="44"/>
       <c r="J27" s="60"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
-      <c r="A28" s="76"/>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="76"/>
+      <c r="D28" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
@@ -13700,15 +13712,15 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
-      <c r="A29" s="76"/>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="76"/>
+      <c r="D29" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>137</v>
       </c>
       <c r="E29" s="3">
         <v>-0.10414</v>
@@ -13716,15 +13728,15 @@
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="39"/>
-      <c r="B30" s="41" t="s">
+      <c r="A30" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="41" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>138</v>
       </c>
       <c r="E30" s="3">
         <v>2.1700000000000001E-3</v>
@@ -13732,15 +13744,15 @@
       <c r="J30" s="60"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="39"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="E31" s="3">
         <v>1.8270000000000002E-2</v>
@@ -13748,14 +13760,14 @@
       <c r="J31" s="60"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="B32" s="41" t="s">
+      <c r="A32" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="41" t="s">
         <v>92</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>140</v>
       </c>
       <c r="E32" s="3">
         <v>-8.7040000000000006E-2</v>
@@ -13763,15 +13775,15 @@
       <c r="J32" s="60"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="51"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>146</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
@@ -13779,15 +13791,15 @@
       <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A34" s="51"/>
-      <c r="B34" s="14" t="s">
+      <c r="A34" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="51"/>
+      <c r="D34" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>142</v>
       </c>
       <c r="E34" s="3">
         <v>7.2209999999999996E-2</v>
@@ -13797,14 +13809,14 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="B35" s="40" t="s">
+      <c r="A35" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="40" t="s">
         <v>95</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="E35" s="3">
         <v>-0.29171999999999998</v>
@@ -13814,14 +13826,14 @@
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>144</v>
       </c>
       <c r="E36" s="3">
         <v>-0.36563000000000001</v>
@@ -13829,14 +13841,14 @@
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="E37" s="3">
         <v>7.6780000000000001E-2</v>
@@ -13844,14 +13856,14 @@
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>225</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
@@ -13859,14 +13871,14 @@
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="E39" s="3">
         <v>0.47683999999999999</v>
@@ -13874,14 +13886,14 @@
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>148</v>
       </c>
       <c r="E40" s="3">
         <v>0.38514999999999999</v>
@@ -13889,14 +13901,14 @@
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>149</v>
       </c>
       <c r="E41" s="3">
         <v>-0.22559999999999999</v>
@@ -13904,14 +13916,14 @@
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>150</v>
       </c>
       <c r="E42" s="3">
         <v>0.57589999999999997</v>
@@ -13919,14 +13931,14 @@
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="B43" s="14" t="s">
+      <c r="A43" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>156</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
@@ -13934,14 +13946,14 @@
       <c r="J43" s="13"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
@@ -13949,14 +13961,14 @@
       <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="B45" s="3" t="s">
+      <c r="A45" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>153</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
@@ -13964,14 +13976,14 @@
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="B46" s="3" t="s">
+      <c r="A46" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>154</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
@@ -13979,14 +13991,14 @@
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>155</v>
       </c>
       <c r="E47" s="3">
         <v>0</v>
@@ -13995,7 +14007,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -47383,17 +47395,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="42.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38" style="3" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" customWidth="1"/>
@@ -47408,16 +47420,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>291</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>35</v>
@@ -47448,17 +47460,17 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="16">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="E2">
         <v>0.24637999999999999</v>
@@ -47484,15 +47496,15 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="16">
-      <c r="A3" s="21"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="19" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -47516,10 +47528,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="16">
-      <c r="A4" s="21"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -47528,17 +47540,17 @@
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="16">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="E5">
         <v>-0.57060999999999995</v>
@@ -47569,15 +47581,15 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16">
-      <c r="A6" s="21"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="E6">
         <v>-0.34464</v>
@@ -47598,15 +47610,15 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="16">
-      <c r="A7" s="21"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="E7">
         <v>-0.23763999999999999</v>
@@ -47630,15 +47642,15 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="16">
-      <c r="A8" s="21"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -47662,10 +47674,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="16">
-      <c r="A9" s="21"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -47674,17 +47686,17 @@
       <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="16">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="19">
+      <c r="D10" s="19">
         <v>0</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="E10">
         <v>0.30664000000000002</v>
@@ -47712,15 +47724,15 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="16">
-      <c r="A11" s="75"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="E11">
         <v>0.15256</v>
@@ -47742,15 +47754,15 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="16">
-      <c r="A12" s="21"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -47775,10 +47787,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="16">
-      <c r="A13" s="21"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -47788,17 +47800,17 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="16">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="D14" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="E14">
         <v>0.25921</v>
@@ -47824,15 +47836,15 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="16">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -47857,10 +47869,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="16">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -47869,17 +47881,17 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:15" ht="16">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="E17">
         <v>0.39734999999999998</v>
@@ -47905,15 +47917,15 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16">
-      <c r="A18" s="21"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="E18" s="28">
         <v>0.52044000000000001</v>
@@ -47934,15 +47946,15 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16">
-      <c r="A19" s="21"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="19" t="s">
         <v>87</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="E19">
         <v>0.33294000000000001</v>
@@ -47963,15 +47975,15 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="16">
-      <c r="A20" s="21"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -47993,10 +48005,10 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16">
-      <c r="A21" s="21"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -48005,17 +48017,17 @@
       <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:15" ht="16">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="E22">
         <v>-3.7679999999999998E-2</v>
@@ -48039,15 +48051,15 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="16">
-      <c r="A23" s="21"/>
-      <c r="B23" s="19" t="s">
+      <c r="A23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -48069,10 +48081,10 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="16">
-      <c r="A24" s="21"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="19"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
@@ -48081,16 +48093,16 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:15" ht="16">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>252</v>
-      </c>
+      <c r="D25" s="24"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
@@ -48110,14 +48122,14 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="16">
-      <c r="A26" s="25"/>
-      <c r="B26"/>
-      <c r="C26" s="16" t="s">
+      <c r="A26" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="B26" s="16" t="s">
         <v>249</v>
       </c>
+      <c r="C26" s="25"/>
+      <c r="D26"/>
       <c r="E26" s="29">
         <v>0.28376000000000001</v>
       </c>
@@ -48138,14 +48150,14 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="16">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27" s="16" t="s">
+      <c r="A27" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="B27" s="16" t="s">
         <v>250</v>
       </c>
+      <c r="C27"/>
+      <c r="D27"/>
       <c r="E27" s="29">
         <v>0.23757</v>
       </c>
@@ -48161,55 +48173,57 @@
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:15" ht="16">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28" s="16" t="s">
+    <row r="28" spans="1:15" s="54" customFormat="1" ht="16">
+      <c r="A28" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="B28" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="E28" s="29">
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="77">
         <v>-0.69055999999999995</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="77">
         <v>-0.45455000000000001</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="77">
         <v>1.65744</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="77">
         <v>-0.47989999999999999</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="1:15" ht="16">
-      <c r="A29" s="25"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="78"/>
+    </row>
+    <row r="29" spans="1:15" s="54" customFormat="1" ht="16">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="78"/>
     </row>
     <row r="30" spans="1:15" ht="17" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>248</v>
-      </c>
+      <c r="D30" s="24"/>
       <c r="I30" s="3" t="s">
         <v>129</v>
       </c>
@@ -48225,14 +48239,14 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16">
-      <c r="A31" s="25"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="16" t="s">
+      <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="B31" s="16" t="s">
         <v>132</v>
       </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="24"/>
       <c r="E31" s="29">
         <v>5.0699999999999999E-3</v>
       </c>
@@ -48253,14 +48267,14 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A32" s="25"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="16" t="s">
+      <c r="A32" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="B32" s="16" t="s">
         <v>134</v>
       </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="32">
         <v>-4.2719999999999998E-4</v>
       </c>
@@ -48281,14 +48295,14 @@
       <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A33" s="25"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="16" t="s">
+      <c r="A33" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="B33" s="16" t="s">
         <v>133</v>
       </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="29">
         <v>1.92E-3</v>
       </c>
@@ -48308,10 +48322,10 @@
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A34" s="25"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
@@ -48323,16 +48337,16 @@
       <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15" ht="16">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="D35" s="24"/>
       <c r="E35" s="29">
         <v>1.457E-2</v>
       </c>
@@ -48360,10 +48374,10 @@
       </c>
     </row>
     <row r="36" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="24"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -48375,16 +48389,16 @@
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>157</v>
-      </c>
+      <c r="D37" s="26"/>
       <c r="E37" s="32">
         <v>-4.0910000000000002E-4</v>
       </c>
@@ -48413,10 +48427,10 @@
       <c r="O37" s="3"/>
     </row>
     <row r="38" spans="1:15" ht="16">
-      <c r="A38" s="21"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
       <c r="G38" s="30"/>
@@ -48424,17 +48438,17 @@
       <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="D39" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>29</v>
       </c>
       <c r="E39" s="29">
         <v>0.44663999999999998</v>
@@ -48459,15 +48473,15 @@
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" s="12" customFormat="1" ht="16">
-      <c r="A40" s="21"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>28</v>
       </c>
       <c r="E40" s="30">
         <v>0</v>
@@ -48488,27 +48502,27 @@
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="1:15" ht="16">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
       <c r="E41" s="29"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
       <c r="H41" s="30"/>
     </row>
     <row r="42" spans="1:15" ht="16">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="D42" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="E42" s="29">
         <v>-0.78983000000000003</v>
@@ -48530,15 +48544,15 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="16">
-      <c r="A43" s="23"/>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="E43" s="29">
         <v>-0.24740999999999999</v>
@@ -48558,15 +48572,15 @@
       <c r="M43" s="18"/>
     </row>
     <row r="44" spans="1:15" ht="16">
-      <c r="A44" s="21"/>
-      <c r="B44" s="19" t="s">
+      <c r="A44" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="21"/>
+      <c r="D44" s="19" t="s">
         <v>61</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>62</v>
       </c>
       <c r="E44" s="29">
         <v>-0.73794000000000004</v>
@@ -48586,15 +48600,15 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:15" ht="16">
-      <c r="A45" s="21"/>
-      <c r="B45" s="19" t="s">
+      <c r="A45" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="E45" s="30">
         <v>0</v>
@@ -48613,24 +48627,24 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="16">
-      <c r="A46" s="21"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="29"/>
       <c r="F46" s="30"/>
       <c r="G46" s="30"/>
       <c r="H46" s="30"/>
     </row>
     <row r="47" spans="1:15" ht="16">
-      <c r="B47" s="19" t="s">
+      <c r="A47" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="E47" s="29">
         <v>-2.613E-2</v>
@@ -48649,14 +48663,14 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="16">
-      <c r="B48" s="26" t="s">
+      <c r="A48" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>138</v>
       </c>
       <c r="E48" s="29">
         <v>0.31215999999999999</v>
@@ -48675,15 +48689,15 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="16">
-      <c r="A49" s="21"/>
-      <c r="B49" s="19" t="s">
+      <c r="A49" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="21"/>
+      <c r="D49" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="C49" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>139</v>
       </c>
       <c r="E49" s="29">
         <v>-0.11212</v>
@@ -48699,15 +48713,15 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="16">
-      <c r="A50" s="21"/>
-      <c r="B50" s="26" t="s">
+      <c r="A50" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="21"/>
+      <c r="D50" s="26" t="s">
         <v>92</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>140</v>
       </c>
       <c r="E50" s="29">
         <v>0.48975000000000002</v>
@@ -48723,15 +48737,15 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="16">
-      <c r="A51" s="21"/>
-      <c r="B51" s="26" t="s">
+      <c r="A51" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="21"/>
+      <c r="D51" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>141</v>
       </c>
       <c r="E51" s="30">
         <v>0</v>
@@ -48747,15 +48761,15 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="16">
-      <c r="A52"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52"/>
+      <c r="D52" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D52" s="34" t="s">
-        <v>142</v>
       </c>
       <c r="E52" s="29">
         <v>-0.33046999999999999</v>
@@ -48771,15 +48785,15 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="16">
-      <c r="A53" s="27"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="24" t="s">
         <v>95</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>143</v>
       </c>
       <c r="E53" s="29">
         <v>-0.43278</v>
@@ -48795,15 +48809,15 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="16">
-      <c r="A54" s="27"/>
-      <c r="B54" t="s">
+      <c r="A54" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" t="s">
         <v>96</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>144</v>
       </c>
       <c r="E54" s="29">
         <v>-7.2679999999999995E-2</v>
@@ -48819,15 +48833,15 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="16">
-      <c r="A55"/>
-      <c r="B55" t="s">
+      <c r="A55" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55"/>
+      <c r="D55" t="s">
         <v>97</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="E55" s="29">
         <v>-0.22628000000000001</v>
@@ -48843,15 +48857,15 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="16">
-      <c r="A56"/>
-      <c r="B56" t="s">
+      <c r="A56" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56" t="s">
         <v>98</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>146</v>
       </c>
       <c r="E56" s="30">
         <v>0</v>
@@ -48867,15 +48881,15 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="16">
-      <c r="A57"/>
-      <c r="B57" t="s">
+      <c r="A57" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57" t="s">
         <v>99</v>
-      </c>
-      <c r="C57" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="E57" s="29">
         <v>-0.56503999999999999</v>
@@ -48891,15 +48905,15 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="16">
-      <c r="A58"/>
-      <c r="B58" t="s">
+      <c r="A58" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58" t="s">
         <v>100</v>
-      </c>
-      <c r="C58" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>148</v>
       </c>
       <c r="E58" s="29">
         <v>-1.5776300000000001</v>
@@ -48915,15 +48929,15 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="16">
-      <c r="A59"/>
-      <c r="B59" t="s">
+      <c r="A59" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" t="s">
         <v>101</v>
-      </c>
-      <c r="C59" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>149</v>
       </c>
       <c r="E59" s="29">
         <v>-0.10624</v>
@@ -48939,15 +48953,15 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="16">
-      <c r="A60"/>
-      <c r="B60" t="s">
+      <c r="A60" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" t="s">
         <v>102</v>
-      </c>
-      <c r="C60" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>150</v>
       </c>
       <c r="E60" s="29">
         <v>-0.14899999999999999</v>
@@ -48963,15 +48977,15 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="16">
-      <c r="A61"/>
-      <c r="B61" t="s">
+      <c r="A61" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61" t="s">
         <v>103</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>151</v>
       </c>
       <c r="E61" s="30">
         <v>0</v>
@@ -48987,15 +49001,15 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="16">
-      <c r="A62"/>
-      <c r="B62" t="s">
+      <c r="A62" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="s">
         <v>104</v>
-      </c>
-      <c r="C62" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="34" t="s">
-        <v>152</v>
       </c>
       <c r="E62" s="30">
         <v>0</v>
@@ -49011,15 +49025,15 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="16">
-      <c r="A63"/>
-      <c r="B63" t="s">
+      <c r="A63" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63"/>
+      <c r="D63" t="s">
         <v>105</v>
-      </c>
-      <c r="C63" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D63" s="34" t="s">
-        <v>153</v>
       </c>
       <c r="E63" s="30">
         <v>0</v>
@@ -49035,15 +49049,15 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="16">
-      <c r="A64"/>
-      <c r="B64" t="s">
+      <c r="A64" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64" t="s">
         <v>106</v>
-      </c>
-      <c r="C64" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>154</v>
       </c>
       <c r="E64" s="30">
         <v>0</v>
@@ -49059,15 +49073,15 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="16">
-      <c r="A65"/>
-      <c r="B65" t="s">
+      <c r="A65" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65" t="s">
         <v>107</v>
-      </c>
-      <c r="C65" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>155</v>
       </c>
       <c r="E65" s="30">
         <v>0</v>
@@ -49083,15 +49097,15 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="16">
-      <c r="A66"/>
-      <c r="B66" t="s">
+      <c r="A66" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66" t="s">
         <v>108</v>
-      </c>
-      <c r="C66" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D66" s="34" t="s">
-        <v>156</v>
       </c>
       <c r="E66" s="30">
         <v>0</v>
@@ -49108,7 +49122,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revising numerics spreadsheet format
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F3A05-69CA-AD40-87C1-CA9AD625AA93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC22270E-C1B5-FF49-916C-0BD5A6AF933B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="-23500" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="3480" yWindow="-23420" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="301">
   <si>
     <t>Notes</t>
   </si>
@@ -426,9 +426,6 @@
   </si>
   <si>
     <t>:yes?</t>
-  </si>
-  <si>
-    <t>:numeric</t>
   </si>
   <si>
     <t>:min</t>
@@ -919,6 +916,39 @@
   <si>
     <t>:param</t>
   </si>
+  <si>
+    <t>{:dps 2, :knot1 0.94, :knot2 1.63, :knot3 2.22, :knot4 3.55, :max 5, :min 0, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :knot1 21, :knot2 44, :knot3 56, :knot4 63, :max 70, :min 16, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :max 100, :min 10, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :max 100, :min 0, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :knot1 22, :knot2 46, :knot3 56, :knot4 63, :max 70, :min 16, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 4.5, :min -2.2, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 6.8, :min 0.35, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :max 77, :min 1, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 9, :min 1.3, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :max 70, :min 16, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 35.7, :min 14, :type :numeric}</t>
+  </si>
 </sst>
 </file>
 
@@ -1094,7 +1124,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1285,6 +1315,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1687,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F23"/>
+    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1698,7 +1734,7 @@
     <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
     <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -1713,13 +1749,13 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>289</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>37</v>
@@ -1731,7 +1767,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>40</v>
@@ -1739,16 +1775,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>196</v>
-      </c>
       <c r="C2" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="42">
         <v>-0.27407999999999999</v>
@@ -1757,7 +1793,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I2" s="70">
         <v>2.2999999999999998</v>
@@ -1766,14 +1802,14 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" s="43">
         <v>0</v>
@@ -1794,13 +1830,13 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>64</v>
@@ -1812,18 +1848,18 @@
         <v>43</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I5" s="70">
         <v>2.1</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>26</v>
@@ -1839,7 +1875,7 @@
         <v>2.1</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1859,7 +1895,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D8" s="14">
         <v>0</v>
@@ -1871,7 +1907,7 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I8" s="70">
         <v>1.4</v>
@@ -1883,11 +1919,11 @@
         <v>112</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" s="80"/>
       <c r="D9" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E9" s="44">
         <v>-0.31792999999999999</v>
@@ -1902,7 +1938,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="14" t="s">
@@ -1933,10 +1969,10 @@
         <v>117</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="44">
         <v>-4.5809999999999997E-2</v>
@@ -1958,7 +1994,7 @@
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" s="46">
         <v>0</v>
@@ -1979,13 +2015,13 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>79</v>
@@ -2006,7 +2042,7 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>109</v>
@@ -2026,7 +2062,7 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>110</v>
@@ -2048,7 +2084,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>111</v>
@@ -2077,29 +2113,29 @@
       <c r="I19" s="70"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10" ht="75">
       <c r="A20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="44"/>
-      <c r="F20" s="3" t="s">
-        <v>127</v>
+      <c r="F20" s="82" t="s">
+        <v>294</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I20" s="70">
         <v>1.2</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2107,14 +2143,14 @@
         <v>22</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" s="40"/>
       <c r="E21" s="44">
         <v>-4.6809999999999997E-2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I21" s="70"/>
       <c r="J21" s="12"/>
@@ -2124,7 +2160,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="40"/>
@@ -2132,7 +2168,7 @@
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I22" s="70"/>
       <c r="J22" s="12"/>
@@ -2142,7 +2178,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="40"/>
@@ -2150,7 +2186,7 @@
         <v>-3.4199999999999999E-3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I23" s="70"/>
       <c r="J23" s="12"/>
@@ -2164,22 +2200,22 @@
       <c r="I24" s="70"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="44">
         <v>0.12</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>127</v>
+      <c r="F25" s="82" t="s">
+        <v>295</v>
       </c>
       <c r="I25" s="70">
         <v>2.2000000000000002</v>
@@ -2192,28 +2228,29 @@
       <c r="C26" s="39"/>
       <c r="D26" s="41"/>
       <c r="E26" s="44"/>
+      <c r="F26" s="82"/>
       <c r="I26" s="70"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" ht="45">
       <c r="A27" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="41"/>
       <c r="E27" s="44">
         <v>-1.8380000000000001E-2</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>127</v>
+      <c r="F27" s="82" t="s">
+        <v>296</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I27" s="70">
         <v>1.5</v>
@@ -2229,25 +2266,25 @@
       <c r="I28" s="70"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" ht="45">
       <c r="A29" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="48">
         <v>-5.1040000000000005E-4</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>127</v>
+      <c r="F29" s="82" t="s">
+        <v>297</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I29" s="70">
         <v>1.1000000000000001</v>
@@ -2263,25 +2300,25 @@
       <c r="I30" s="70"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" ht="30">
       <c r="A31" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" s="41"/>
       <c r="E31" s="44">
         <v>-0.33889999999999998</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>127</v>
+      <c r="F31" s="82" t="s">
+        <v>298</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I31" s="70">
         <v>2.2999999999999998</v>
@@ -2306,156 +2343,156 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="C34" s="80"/>
       <c r="D34" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E34" s="44">
         <v>-0.27877999999999997</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I34" s="70"/>
       <c r="J34" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C35" s="80"/>
       <c r="D35" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E35" s="44">
         <v>0.34847</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I35" s="70"/>
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="46">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I36" s="70"/>
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E37" s="46">
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I37" s="70"/>
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E38" s="46">
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I38" s="70"/>
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E39" s="46">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I39" s="70"/>
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E40" s="46">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I40" s="70"/>
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E41" s="46">
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I41" s="70"/>
       <c r="J41" s="12"/>
@@ -2535,7 +2572,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -13129,7 +13166,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>26</v>
@@ -13161,7 +13198,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>111</v>
@@ -13169,7 +13206,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>63</v>
@@ -13204,15 +13241,15 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13236,8 +13273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13247,7 +13284,8 @@
     <col min="3" max="3" width="28.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="3"/>
+    <col min="6" max="6" width="15.1640625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="3"/>
     <col min="9" max="9" width="8.83203125" style="72"/>
     <col min="10" max="10" width="32" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="3"/>
@@ -13261,13 +13299,13 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>289</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>37</v>
@@ -13279,7 +13317,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="61" t="s">
         <v>40</v>
@@ -13478,7 +13516,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>108</v>
@@ -13502,7 +13540,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>109</v>
@@ -13521,7 +13559,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>110</v>
@@ -13540,7 +13578,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>111</v>
@@ -13567,13 +13605,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>64</v>
@@ -13591,7 +13629,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>26</v>
@@ -13667,12 +13705,12 @@
       <c r="E23" s="44"/>
       <c r="J23" s="60"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="45">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>66</v>
@@ -13681,14 +13719,14 @@
       <c r="E24" s="3">
         <v>2.82E-3</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>127</v>
+      <c r="F24" s="82" t="s">
+        <v>299</v>
       </c>
       <c r="I24" s="72">
         <v>1.7</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -13699,12 +13737,12 @@
       <c r="E25" s="44"/>
       <c r="J25" s="60"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="42" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>122</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>68</v>
@@ -13713,8 +13751,8 @@
       <c r="E26" s="3">
         <v>-1.452E-2</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>127</v>
+      <c r="F26" s="82" t="s">
+        <v>300</v>
       </c>
       <c r="I26" s="72">
         <v>1.8</v>
@@ -13731,10 +13769,10 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C28" s="80"/>
       <c r="D28" s="14" t="s">
@@ -13744,18 +13782,18 @@
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>135</v>
       </c>
       <c r="C29" s="80"/>
       <c r="D29" s="14" t="s">
@@ -13765,16 +13803,16 @@
         <v>-0.10414</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="41" t="s">
@@ -13784,16 +13822,16 @@
         <v>2.1700000000000001E-3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J30" s="60"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="14" t="s">
@@ -13803,16 +13841,16 @@
         <v>1.8270000000000002E-2</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J31" s="60"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>90</v>
@@ -13821,16 +13859,16 @@
         <v>-8.7040000000000006E-2</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J32" s="60"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
       <c r="A33" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="14" t="s">
@@ -13840,16 +13878,16 @@
         <v>0</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="14" t="s">
@@ -13859,18 +13897,18 @@
         <v>7.2209999999999996E-2</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>93</v>
@@ -13879,18 +13917,18 @@
         <v>-0.29171999999999998</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J35" s="62" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>94</v>
@@ -13899,16 +13937,16 @@
         <v>-0.36563000000000001</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>95</v>
@@ -13917,16 +13955,16 @@
         <v>7.6780000000000001E-2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>101</v>
@@ -13935,16 +13973,16 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>97</v>
@@ -13953,16 +13991,16 @@
         <v>0.47683999999999999</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>98</v>
@@ -13971,16 +14009,16 @@
         <v>0.38514999999999999</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>99</v>
@@ -13989,16 +14027,16 @@
         <v>-0.22559999999999999</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>100</v>
@@ -14007,16 +14045,16 @@
         <v>0.57589999999999997</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>106</v>
@@ -14025,16 +14063,16 @@
         <v>0</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J43" s="13"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>102</v>
@@ -14043,16 +14081,16 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>103</v>
@@ -14061,16 +14099,16 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>104</v>
@@ -14079,16 +14117,16 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>105</v>
@@ -14097,7 +14135,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J47" s="13"/>
     </row>
@@ -14127,104 +14165,104 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="63" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="63" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -14256,46 +14294,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -47364,7 +47402,7 @@
     </row>
     <row r="2" spans="1:9" ht="16">
       <c r="A2" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>26</v>
@@ -47396,7 +47434,7 @@
     </row>
     <row r="6" spans="1:9" ht="16">
       <c r="A6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>111</v>
@@ -47407,7 +47445,7 @@
         <v>112</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16">
@@ -47452,7 +47490,7 @@
     </row>
     <row r="13" spans="1:9" ht="16">
       <c r="A13" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="19">
         <v>9</v>
@@ -47468,10 +47506,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -47479,7 +47517,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -47491,8 +47529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26:I28"/>
+    <sheetView topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47522,10 +47560,10 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>288</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>289</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>33</v>
@@ -47549,7 +47587,7 @@
         <v>39</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>40</v>
@@ -47637,7 +47675,7 @@
     </row>
     <row r="5" spans="1:13" ht="16">
       <c r="A5" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>108</v>
@@ -47678,7 +47716,7 @@
     </row>
     <row r="6" spans="1:13" ht="16">
       <c r="A6" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>109</v>
@@ -47707,7 +47745,7 @@
     </row>
     <row r="7" spans="1:13" ht="16">
       <c r="A7" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>110</v>
@@ -47739,7 +47777,7 @@
     </row>
     <row r="8" spans="1:13" ht="16">
       <c r="A8" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>111</v>
@@ -47810,7 +47848,7 @@
         <v>43</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>126</v>
@@ -48188,12 +48226,12 @@
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
     </row>
-    <row r="25" spans="1:15" ht="16">
+    <row r="25" spans="1:15" ht="76">
       <c r="A25" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>67</v>
@@ -48203,18 +48241,18 @@
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="14" t="s">
-        <v>127</v>
+      <c r="I25" s="81" t="s">
+        <v>290</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="69">
         <v>1.06</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="16">
@@ -48222,7 +48260,7 @@
         <v>107</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26"/>
@@ -48239,12 +48277,12 @@
         <v>-0.1124</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="M26" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="16">
@@ -48252,7 +48290,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -48269,7 +48307,7 @@
         <v>0.25652000000000003</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -48279,7 +48317,7 @@
         <v>107</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
@@ -48296,7 +48334,7 @@
         <v>-0.47989999999999999</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="57"/>
@@ -48316,29 +48354,29 @@
       <c r="K29" s="57"/>
       <c r="L29" s="76"/>
     </row>
-    <row r="30" spans="1:15" ht="17" customHeight="1">
+    <row r="30" spans="1:15" ht="62" customHeight="1">
       <c r="A30" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="24"/>
-      <c r="I30" s="3" t="s">
-        <v>127</v>
+      <c r="I30" s="82" t="s">
+        <v>291</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="69">
         <v>1.01</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="16">
@@ -48346,7 +48384,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="24"/>
@@ -48363,12 +48401,12 @@
         <v>-3.1900000000000001E-3</v>
       </c>
       <c r="I31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
       <c r="M31" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="16">
@@ -48376,7 +48414,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="24"/>
@@ -48393,7 +48431,7 @@
         <v>3.3849999999999999E-4</v>
       </c>
       <c r="I32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -48406,7 +48444,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="24"/>
@@ -48423,7 +48461,7 @@
         <v>-8.1760000000000003E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J33" s="54"/>
       <c r="K33" s="14"/>
@@ -48445,12 +48483,12 @@
       <c r="L34" s="69"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" ht="16">
+    <row r="35" spans="1:15" ht="46">
       <c r="A35" s="16" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>68</v>
@@ -48468,18 +48506,18 @@
       <c r="H35" s="29">
         <v>-1.899E-2</v>
       </c>
-      <c r="I35" s="14" t="s">
-        <v>127</v>
+      <c r="I35" s="81" t="s">
+        <v>292</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K35" s="14"/>
       <c r="L35" s="69">
         <v>1.1200000000000001</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1">
@@ -48497,12 +48535,12 @@
       <c r="L36" s="69"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="1:15" s="12" customFormat="1" ht="16">
+    <row r="37" spans="1:15" s="12" customFormat="1" ht="36" customHeight="1">
       <c r="A37" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>65</v>
@@ -48520,18 +48558,18 @@
       <c r="H37" s="29">
         <v>-4.6100000000000004E-3</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>127</v>
+      <c r="I37" s="82" t="s">
+        <v>293</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="69">
         <v>1.1299999999999999</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O37" s="3"/>
     </row>
@@ -48548,13 +48586,13 @@
     </row>
     <row r="39" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A39" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B39" s="34" t="s">
         <v>27</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>64</v>
@@ -48583,7 +48621,7 @@
     </row>
     <row r="40" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A40" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>26</v>
@@ -48747,10 +48785,10 @@
     </row>
     <row r="47" spans="1:15" ht="16">
       <c r="A47" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="34" t="s">
         <v>134</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>135</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>87</v>
@@ -48773,10 +48811,10 @@
     </row>
     <row r="48" spans="1:15" ht="16">
       <c r="A48" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>88</v>
@@ -48794,15 +48832,15 @@
         <v>-0.25944</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="16">
       <c r="A49" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
@@ -48823,10 +48861,10 @@
     </row>
     <row r="50" spans="1:8" ht="16">
       <c r="A50" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="26" t="s">
@@ -48847,10 +48885,10 @@
     </row>
     <row r="51" spans="1:8" ht="16">
       <c r="A51" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="26" t="s">
@@ -48871,10 +48909,10 @@
     </row>
     <row r="52" spans="1:8" ht="16">
       <c r="A52" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52"/>
       <c r="D52" s="19" t="s">
@@ -48895,10 +48933,10 @@
     </row>
     <row r="53" spans="1:8" ht="16">
       <c r="A53" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="24" t="s">
@@ -48919,10 +48957,10 @@
     </row>
     <row r="54" spans="1:8" ht="16">
       <c r="A54" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" t="s">
@@ -48943,10 +48981,10 @@
     </row>
     <row r="55" spans="1:8" ht="16">
       <c r="A55" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55"/>
       <c r="D55" t="s">
@@ -48967,10 +49005,10 @@
     </row>
     <row r="56" spans="1:8" ht="16">
       <c r="A56" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
@@ -48991,10 +49029,10 @@
     </row>
     <row r="57" spans="1:8" ht="16">
       <c r="A57" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57"/>
       <c r="D57" t="s">
@@ -49015,10 +49053,10 @@
     </row>
     <row r="58" spans="1:8" ht="16">
       <c r="A58" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -49039,10 +49077,10 @@
     </row>
     <row r="59" spans="1:8" ht="16">
       <c r="A59" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
@@ -49063,10 +49101,10 @@
     </row>
     <row r="60" spans="1:8" ht="16">
       <c r="A60" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
@@ -49087,10 +49125,10 @@
     </row>
     <row r="61" spans="1:8" ht="16">
       <c r="A61" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
@@ -49111,10 +49149,10 @@
     </row>
     <row r="62" spans="1:8" ht="16">
       <c r="A62" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
@@ -49135,10 +49173,10 @@
     </row>
     <row r="63" spans="1:8" ht="16">
       <c r="A63" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
@@ -49159,10 +49197,10 @@
     </row>
     <row r="64" spans="1:8" ht="16">
       <c r="A64" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
@@ -49183,10 +49221,10 @@
     </row>
     <row r="65" spans="1:8" ht="16">
       <c r="A65" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
@@ -49207,10 +49245,10 @@
     </row>
     <row r="66" spans="1:8" ht="16">
       <c r="A66" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -49263,39 +49301,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>129</v>
-      </c>
       <c r="E1" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="38" t="s">
-        <v>167</v>
-      </c>
       <c r="J1" s="65" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>107</v>
@@ -49322,12 +49360,12 @@
         <v>3.55</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>22</v>
@@ -49354,12 +49392,12 @@
         <v>63</v>
       </c>
       <c r="J3" s="64" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>122</v>
@@ -49374,15 +49412,15 @@
         <v>0</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -49394,12 +49432,12 @@
         <v>0</v>
       </c>
       <c r="J5" s="64" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>22</v>
@@ -49426,15 +49464,15 @@
         <v>63</v>
       </c>
       <c r="J6" s="64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="A7" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7">
         <v>-2.2000000000000002</v>
@@ -49450,12 +49488,12 @@
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1">
       <c r="A8" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>107</v>
@@ -49477,10 +49515,10 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1">
       <c r="A9" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" s="45">
         <v>1</v>
@@ -49496,15 +49534,15 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1">
       <c r="A10" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" s="45">
         <v>1.3</v>
@@ -49519,7 +49557,7 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1">
       <c r="A11" s="49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="49" t="s">
         <v>22</v>
@@ -49534,12 +49572,12 @@
         <v>0</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1">
       <c r="A12" s="49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B12" s="49" t="s">
         <v>122</v>
@@ -49696,7 +49734,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -55775,15 +55813,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>26</v>
@@ -55794,7 +55832,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -55807,7 +55845,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>111</v>
@@ -55818,15 +55856,15 @@
         <v>22</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -55839,7 +55877,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="14">
         <v>9</v>
@@ -55847,7 +55885,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B11" s="14">
         <v>4.9000000000000004</v>
@@ -55858,15 +55896,15 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>

<commit_message>
revised numerics format. imported splines.
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC22270E-C1B5-FF49-916C-0BD5A6AF933B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42DB404-E5C5-E14A-B649-1FBC332170FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="-23420" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="3480" yWindow="-23420" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13273,8 +13273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -47529,8 +47529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -48354,7 +48354,7 @@
       <c r="K29" s="57"/>
       <c r="L29" s="76"/>
     </row>
-    <row r="30" spans="1:15" ht="62" customHeight="1">
+    <row r="30" spans="1:15" ht="68" customHeight="1">
       <c r="A30" s="16" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
unstring-key on all values. Added :none widget type
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42DB404-E5C5-E14A-B649-1FBC332170FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F413A28-B27B-1747-9FDD-B9AB7B794824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="-23420" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="2400" yWindow="-22420" windowWidth="29680" windowHeight="21500" firstSheet="1" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="302">
   <si>
     <t>Notes</t>
   </si>
@@ -949,6 +949,9 @@
   <si>
     <t>{:dps 1, :max 35.7, :min 14, :type :numeric}</t>
   </si>
+  <si>
+    <t>:none</t>
+  </si>
 </sst>
 </file>
 
@@ -1723,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -47529,17 +47532,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="38" style="3" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" customWidth="1"/>
@@ -48805,6 +48808,9 @@
       <c r="H47" s="29">
         <v>-0.33476</v>
       </c>
+      <c r="I47" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="M47" s="12" t="s">
         <v>86</v>
       </c>
@@ -48831,11 +48837,14 @@
       <c r="H48" s="29">
         <v>-0.25944</v>
       </c>
+      <c r="I48" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="M48" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16">
+    <row r="49" spans="1:9" ht="16">
       <c r="A49" s="34" t="s">
         <v>133</v>
       </c>
@@ -48858,8 +48867,11 @@
       <c r="H49" s="29">
         <v>-0.52005999999999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="16">
+      <c r="I49" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16">
       <c r="A50" s="34" t="s">
         <v>133</v>
       </c>
@@ -48882,8 +48894,11 @@
       <c r="H50" s="29">
         <v>0.21389</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="16">
+      <c r="I50" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="16">
       <c r="A51" s="34" t="s">
         <v>133</v>
       </c>
@@ -48906,8 +48921,11 @@
       <c r="H51" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="16">
+      <c r="I51" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="16">
       <c r="A52" s="34" t="s">
         <v>133</v>
       </c>
@@ -48930,8 +48948,11 @@
       <c r="H52" s="29">
         <v>-0.22592999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="16">
+      <c r="I52" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16">
       <c r="A53" s="34" t="s">
         <v>133</v>
       </c>
@@ -48954,8 +48975,11 @@
       <c r="H53" s="29">
         <v>-0.67791000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="16">
+      <c r="I53" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="16">
       <c r="A54" s="34" t="s">
         <v>133</v>
       </c>
@@ -48978,8 +49002,11 @@
       <c r="H54" s="29">
         <v>-1.9220000000000001E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="16">
+      <c r="I54" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="16">
       <c r="A55" s="34" t="s">
         <v>133</v>
       </c>
@@ -49002,8 +49029,11 @@
       <c r="H55" s="29">
         <v>-0.22169</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="16">
+      <c r="I55" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="16">
       <c r="A56" s="34" t="s">
         <v>133</v>
       </c>
@@ -49026,8 +49056,11 @@
       <c r="H56" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="16">
+      <c r="I56" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="16">
       <c r="A57" s="34" t="s">
         <v>133</v>
       </c>
@@ -49050,8 +49083,11 @@
       <c r="H57" s="29">
         <v>-0.64468999999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="16">
+      <c r="I57" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="16">
       <c r="A58" s="34" t="s">
         <v>133</v>
       </c>
@@ -49074,8 +49110,11 @@
       <c r="H58" s="29">
         <v>-1.1697299999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="16">
+      <c r="I58" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="16">
       <c r="A59" s="34" t="s">
         <v>133</v>
       </c>
@@ -49098,8 +49137,11 @@
       <c r="H59" s="29">
         <v>-0.45308999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="16">
+      <c r="I59" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="16">
       <c r="A60" s="34" t="s">
         <v>133</v>
       </c>
@@ -49122,8 +49164,11 @@
       <c r="H60" s="29">
         <v>-0.11143</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="16">
+      <c r="I60" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="16">
       <c r="A61" s="34" t="s">
         <v>133</v>
       </c>
@@ -49146,8 +49191,11 @@
       <c r="H61" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="16">
+      <c r="I61" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="16">
       <c r="A62" s="34" t="s">
         <v>133</v>
       </c>
@@ -49170,8 +49218,11 @@
       <c r="H62" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="16">
+      <c r="I62" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="16">
       <c r="A63" s="34" t="s">
         <v>133</v>
       </c>
@@ -49194,8 +49245,11 @@
       <c r="H63" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="16">
+      <c r="I63" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="16">
       <c r="A64" s="34" t="s">
         <v>133</v>
       </c>
@@ -49218,8 +49272,11 @@
       <c r="H64" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="16">
+      <c r="I64" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="16">
       <c r="A65" s="34" t="s">
         <v>133</v>
       </c>
@@ -49242,8 +49299,11 @@
       <c r="H65" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="16">
+      <c r="I65" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="16">
       <c r="A66" s="34" t="s">
         <v>133</v>
       </c>
@@ -49265,6 +49325,9 @@
       </c>
       <c r="H66" s="30">
         <v>0</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all inputs present logic working
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161FEF34-734B-3F49-BE36-0F7113B28F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE8991F-27BB-A846-892B-822F5F228587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="-21500" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="2560" yWindow="-21500" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -782,9 +782,6 @@
     <t>:beta-from-listing</t>
   </si>
   <si>
-    <t>[:spline :x :age-beta1 :age-beta2 age-:beta3]</t>
-  </si>
-  <si>
     <t>:fvc-beta1</t>
   </si>
   <si>
@@ -951,6 +948,9 @@
   </si>
   <si>
     <t>:none</t>
+  </si>
+  <si>
+    <t>[:spline :x :age-beta1 :age-beta2 age-beta3]</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +1752,10 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>287</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>288</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>243</v>
@@ -1770,7 +1770,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>40</v>
@@ -2121,7 +2121,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>176</v>
@@ -2129,7 +2129,7 @@
       <c r="D20" s="40"/>
       <c r="E20" s="44"/>
       <c r="F20" s="82" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>238</v>
@@ -2146,14 +2146,14 @@
         <v>22</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D21" s="40"/>
       <c r="E21" s="44">
         <v>-4.6809999999999997E-2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I21" s="70"/>
       <c r="J21" s="12"/>
@@ -2163,7 +2163,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="40"/>
@@ -2171,7 +2171,7 @@
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I22" s="70"/>
       <c r="J22" s="12"/>
@@ -2181,7 +2181,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="40"/>
@@ -2189,7 +2189,7 @@
         <v>-3.4199999999999999E-3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I23" s="70"/>
       <c r="J23" s="12"/>
@@ -2218,7 +2218,7 @@
         <v>0.12</v>
       </c>
       <c r="F25" s="82" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I25" s="70">
         <v>2.2000000000000002</v>
@@ -2250,7 +2250,7 @@
         <v>-1.8380000000000001E-2</v>
       </c>
       <c r="F27" s="82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>227</v>
@@ -2284,7 +2284,7 @@
         <v>-5.1040000000000005E-4</v>
       </c>
       <c r="F29" s="82" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>226</v>
@@ -2318,7 +2318,7 @@
         <v>-0.33889999999999998</v>
       </c>
       <c r="F31" s="82" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>240</v>
@@ -2359,7 +2359,7 @@
         <v>-0.27877999999999997</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I34" s="70"/>
       <c r="J34" s="12" t="s">
@@ -2381,7 +2381,7 @@
         <v>0.34847</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I35" s="70"/>
       <c r="J35" s="12"/>
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I36" s="70"/>
       <c r="J36" s="12"/>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I37" s="70"/>
       <c r="J37" s="12"/>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I38" s="70"/>
       <c r="J38" s="12"/>
@@ -2457,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I39" s="70"/>
       <c r="J39" s="12"/>
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I40" s="70"/>
       <c r="J40" s="12"/>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I41" s="70"/>
       <c r="J41" s="12"/>
@@ -13244,7 +13244,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -13252,7 +13252,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13276,8 +13276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13302,10 +13302,10 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>287</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>288</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>244</v>
@@ -13320,7 +13320,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J1" s="61" t="s">
         <v>40</v>
@@ -13723,7 +13723,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I24" s="72">
         <v>1.7</v>
@@ -13755,7 +13755,7 @@
         <v>-1.452E-2</v>
       </c>
       <c r="F26" s="82" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I26" s="72">
         <v>1.8</v>
@@ -13785,7 +13785,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I28" s="72">
         <v>10</v>
@@ -13809,7 +13809,7 @@
         <v>-0.10414</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J29" s="60"/>
     </row>
@@ -13828,7 +13828,7 @@
         <v>2.1700000000000001E-3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J30" s="60"/>
     </row>
@@ -13847,7 +13847,7 @@
         <v>1.8270000000000002E-2</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J31" s="60"/>
     </row>
@@ -13865,7 +13865,7 @@
         <v>-8.7040000000000006E-2</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J32" s="60"/>
     </row>
@@ -13884,7 +13884,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J33" s="60"/>
     </row>
@@ -13903,7 +13903,7 @@
         <v>7.2209999999999996E-2</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J34" s="62" t="s">
         <v>223</v>
@@ -13923,7 +13923,7 @@
         <v>-0.29171999999999998</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J35" s="62" t="s">
         <v>224</v>
@@ -13943,7 +13943,7 @@
         <v>-0.36563000000000001</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J36" s="13"/>
     </row>
@@ -13961,7 +13961,7 @@
         <v>7.6780000000000001E-2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J37" s="13"/>
     </row>
@@ -13979,7 +13979,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J38" s="13"/>
     </row>
@@ -13997,7 +13997,7 @@
         <v>0.47683999999999999</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J39" s="13"/>
     </row>
@@ -14015,7 +14015,7 @@
         <v>0.38514999999999999</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J40" s="13"/>
     </row>
@@ -14033,7 +14033,7 @@
         <v>-0.22559999999999999</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J41" s="13"/>
     </row>
@@ -14051,7 +14051,7 @@
         <v>0.57589999999999997</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J42" s="13"/>
     </row>
@@ -14069,7 +14069,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J43" s="13"/>
     </row>
@@ -14087,7 +14087,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J44" s="13"/>
     </row>
@@ -14105,7 +14105,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J45" s="13"/>
     </row>
@@ -14123,7 +14123,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J46" s="13"/>
     </row>
@@ -14141,7 +14141,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J47" s="13"/>
     </row>
@@ -14171,104 +14171,104 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="63" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="63" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -14300,13 +14300,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -14314,10 +14314,10 @@
         <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14325,10 +14325,10 @@
         <v>208</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14336,10 +14336,10 @@
         <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -47515,7 +47515,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -47523,7 +47523,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -47535,8 +47535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47566,10 +47566,10 @@
         <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>287</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>288</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>33</v>
@@ -47593,7 +47593,7 @@
         <v>39</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>40</v>
@@ -48237,7 +48237,7 @@
         <v>107</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>67</v>
@@ -48248,7 +48248,7 @@
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
       <c r="I25" s="81" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>227</v>
@@ -48266,7 +48266,7 @@
         <v>107</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26"/>
@@ -48283,7 +48283,7 @@
         <v>-0.1124</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
@@ -48296,7 +48296,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -48313,7 +48313,7 @@
         <v>0.25652000000000003</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -48323,7 +48323,7 @@
         <v>107</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
@@ -48340,7 +48340,7 @@
         <v>-0.47989999999999999</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="57"/>
@@ -48365,14 +48365,14 @@
         <v>22</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>245</v>
+        <v>301</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="24"/>
       <c r="I30" s="82" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>238</v>
@@ -48407,7 +48407,7 @@
         <v>-3.1900000000000001E-3</v>
       </c>
       <c r="I31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
@@ -48437,7 +48437,7 @@
         <v>3.3849999999999999E-4</v>
       </c>
       <c r="I32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -48467,7 +48467,7 @@
         <v>-8.1760000000000003E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J33" s="54"/>
       <c r="K33" s="14"/>
@@ -48513,7 +48513,7 @@
         <v>-1.899E-2</v>
       </c>
       <c r="I35" s="81" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>239</v>
@@ -48565,7 +48565,7 @@
         <v>-4.6100000000000004E-3</v>
       </c>
       <c r="I37" s="82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>226</v>
@@ -48812,7 +48812,7 @@
         <v>-0.33476</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M47" s="12" t="s">
         <v>86</v>
@@ -48841,7 +48841,7 @@
         <v>-0.25944</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>156</v>
@@ -48871,7 +48871,7 @@
         <v>-0.52005999999999997</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="16">
@@ -48898,7 +48898,7 @@
         <v>0.21389</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="16">
@@ -48925,7 +48925,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="16">
@@ -48952,7 +48952,7 @@
         <v>-0.22592999999999999</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="16">
@@ -48979,7 +48979,7 @@
         <v>-0.67791000000000001</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="16">
@@ -49006,7 +49006,7 @@
         <v>-1.9220000000000001E-2</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="16">
@@ -49033,7 +49033,7 @@
         <v>-0.22169</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="16">
@@ -49060,7 +49060,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="16">
@@ -49087,7 +49087,7 @@
         <v>-0.64468999999999999</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="16">
@@ -49114,7 +49114,7 @@
         <v>-1.1697299999999999</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="16">
@@ -49141,7 +49141,7 @@
         <v>-0.45308999999999999</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="16">
@@ -49168,7 +49168,7 @@
         <v>-0.11143</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="16">
@@ -49195,7 +49195,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="16">
@@ -49222,7 +49222,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="16">
@@ -49249,7 +49249,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="16">
@@ -49276,7 +49276,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="16">
@@ -49303,7 +49303,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="16">
@@ -49330,7 +49330,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -55962,7 +55962,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -55970,7 +55970,7 @@
         <v>199</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>

<commit_message>
updated spreadsheets; new processed bundle fields
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE8991F-27BB-A846-892B-822F5F228587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C1BB91-D9CB-A441-93EE-16291732B732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="-21500" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="3260" yWindow="-21500" windowWidth="29680" windowHeight="21500" firstSheet="3" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
grouped factors now in order
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C1BB91-D9CB-A441-93EE-16291732B732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4BC67-D322-5743-B852-F998E684769E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="-21500" windowWidth="29680" windowHeight="21500" firstSheet="3" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="5820" yWindow="-21800" windowWidth="29680" windowHeight="21500" firstSheet="2" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -47535,22 +47535,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47:L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38" style="3" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5" style="3" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" style="3" customWidth="1"/>
     <col min="12" max="12" width="10.5" style="69" customWidth="1"/>
     <col min="13" max="13" width="60.6640625" style="12" bestFit="1" customWidth="1"/>
@@ -48814,6 +48814,9 @@
       <c r="I47" s="3" t="s">
         <v>300</v>
       </c>
+      <c r="L47" s="69">
+        <v>-1</v>
+      </c>
       <c r="M47" s="12" t="s">
         <v>86</v>
       </c>
@@ -48843,11 +48846,14 @@
       <c r="I48" s="3" t="s">
         <v>300</v>
       </c>
+      <c r="L48" s="69">
+        <v>-1</v>
+      </c>
       <c r="M48" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="16">
+    <row r="49" spans="1:12" ht="16">
       <c r="A49" s="34" t="s">
         <v>133</v>
       </c>
@@ -48873,8 +48879,11 @@
       <c r="I49" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="16">
+      <c r="L49" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="16">
       <c r="A50" s="34" t="s">
         <v>133</v>
       </c>
@@ -48900,8 +48909,11 @@
       <c r="I50" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="16">
+      <c r="L50" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="16">
       <c r="A51" s="34" t="s">
         <v>133</v>
       </c>
@@ -48927,8 +48939,11 @@
       <c r="I51" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="16">
+      <c r="L51" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="16">
       <c r="A52" s="34" t="s">
         <v>133</v>
       </c>
@@ -48954,8 +48969,11 @@
       <c r="I52" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="16">
+      <c r="L52" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="16">
       <c r="A53" s="34" t="s">
         <v>133</v>
       </c>
@@ -48981,8 +48999,11 @@
       <c r="I53" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="16">
+      <c r="L53" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="16">
       <c r="A54" s="34" t="s">
         <v>133</v>
       </c>
@@ -49008,8 +49029,11 @@
       <c r="I54" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="16">
+      <c r="L54" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="16">
       <c r="A55" s="34" t="s">
         <v>133</v>
       </c>
@@ -49035,8 +49059,11 @@
       <c r="I55" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="16">
+      <c r="L55" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="16">
       <c r="A56" s="34" t="s">
         <v>133</v>
       </c>
@@ -49062,8 +49089,11 @@
       <c r="I56" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="16">
+      <c r="L56" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="16">
       <c r="A57" s="34" t="s">
         <v>133</v>
       </c>
@@ -49089,8 +49119,11 @@
       <c r="I57" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="16">
+      <c r="L57" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="16">
       <c r="A58" s="34" t="s">
         <v>133</v>
       </c>
@@ -49116,8 +49149,11 @@
       <c r="I58" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="16">
+      <c r="L58" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="16">
       <c r="A59" s="34" t="s">
         <v>133</v>
       </c>
@@ -49143,8 +49179,11 @@
       <c r="I59" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="16">
+      <c r="L59" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16">
       <c r="A60" s="34" t="s">
         <v>133</v>
       </c>
@@ -49170,8 +49209,11 @@
       <c r="I60" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="16">
+      <c r="L60" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="16">
       <c r="A61" s="34" t="s">
         <v>133</v>
       </c>
@@ -49197,8 +49239,11 @@
       <c r="I61" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="16">
+      <c r="L61" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="16">
       <c r="A62" s="34" t="s">
         <v>133</v>
       </c>
@@ -49224,8 +49269,11 @@
       <c r="I62" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="16">
+      <c r="L62" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="16">
       <c r="A63" s="34" t="s">
         <v>133</v>
       </c>
@@ -49251,8 +49299,11 @@
       <c r="I63" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="16">
+      <c r="L63" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="16">
       <c r="A64" s="34" t="s">
         <v>133</v>
       </c>
@@ -49278,8 +49329,11 @@
       <c r="I64" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="16">
+      <c r="L64" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="16">
       <c r="A65" s="34" t="s">
         <v>133</v>
       </c>
@@ -49305,8 +49359,11 @@
       <c r="I65" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="16">
+      <c r="L65" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="16">
       <c r="A66" s="34" t="s">
         <v>133</v>
       </c>
@@ -49331,6 +49388,9 @@
       </c>
       <c r="I66" s="3" t="s">
         <v>300</v>
+      </c>
+      <c r="L66" s="69">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cross over factors and their level lookups
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115D0845-24BA-3E4D-8984-B097F197F485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDB19A-D3D6-D248-BB17-4019F978B03A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="-22740" windowWidth="29680" windowHeight="21500" firstSheet="2" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1500" yWindow="-23400" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="305">
   <si>
     <t>Notes</t>
   </si>
@@ -383,9 +383,6 @@
     <t>:dd-pred</t>
   </si>
   <si>
-    <t>:0</t>
-  </si>
-  <si>
     <t>:in-hosp</t>
   </si>
   <si>
@@ -438,66 +435,6 @@
   </si>
   <si>
     <t>:centre-d-gp</t>
-  </si>
-  <si>
-    <t>:cf-pap</t>
-  </si>
-  <si>
-    <t>:cf-hare</t>
-  </si>
-  <si>
-    <t>:cf-birm</t>
-  </si>
-  <si>
-    <t>:cf-man</t>
-  </si>
-  <si>
-    <t>:cf-new</t>
-  </si>
-  <si>
-    <t>:other-pap</t>
-  </si>
-  <si>
-    <t>:other-hare</t>
-  </si>
-  <si>
-    <t>:other-birm</t>
-  </si>
-  <si>
-    <t>:other-man</t>
-  </si>
-  <si>
-    <t>:other-new</t>
-  </si>
-  <si>
-    <t>:pf-pap</t>
-  </si>
-  <si>
-    <t>:pf-hare</t>
-  </si>
-  <si>
-    <t>:pf-birm</t>
-  </si>
-  <si>
-    <t>:pf-man</t>
-  </si>
-  <si>
-    <t>:pf-new</t>
-  </si>
-  <si>
-    <t>:copd-pap</t>
-  </si>
-  <si>
-    <t>:copd-hare</t>
-  </si>
-  <si>
-    <t>:copd-birm</t>
-  </si>
-  <si>
-    <t>:copd-man</t>
-  </si>
-  <si>
-    <t>:copd-new</t>
   </si>
   <si>
     <t>:x</t>
@@ -632,34 +569,7 @@
     <t>:donor-smokes</t>
   </si>
   <si>
-    <t>:&lt;15</t>
-  </si>
-  <si>
     <t>:type-d-gp</t>
-  </si>
-  <si>
-    <t>:1-other</t>
-  </si>
-  <si>
-    <t>:1-pf</t>
-  </si>
-  <si>
-    <t>:1-copd</t>
-  </si>
-  <si>
-    <t>;1-cf</t>
-  </si>
-  <si>
-    <t>:2-other</t>
-  </si>
-  <si>
-    <t>:2-pf</t>
-  </si>
-  <si>
-    <t>:2-cf</t>
-  </si>
-  <si>
-    <t>:2-copd</t>
   </si>
   <si>
     <t>:post-transplant</t>
@@ -702,9 +612,6 @@
   </si>
   <si>
     <t>not present in User Interface</t>
-  </si>
-  <si>
-    <t>:pf-new-new</t>
   </si>
   <si>
     <t>I added</t>
@@ -914,9 +821,6 @@
     <t>{:dps 0, :max 100, :min 10, :type :numeric}</t>
   </si>
   <si>
-    <t>{:dps 0, :max 100, :min 0, :type :numeric}</t>
-  </si>
-  <si>
     <t>{:dps 0, :knot1 22, :knot2 46, :knot3 56, :knot4 63, :max 70, :min 16, :type :numeric}</t>
   </si>
   <si>
@@ -954,6 +858,108 @@
   </si>
   <si>
     <t>:pred-15+</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 100, :min 0, :type :numeric}</t>
+  </si>
+  <si>
+    <t>:t1</t>
+  </si>
+  <si>
+    <t>:t2</t>
+  </si>
+  <si>
+    <t>:cf*new</t>
+  </si>
+  <si>
+    <t>:cf*pap</t>
+  </si>
+  <si>
+    <t>:cf*hare</t>
+  </si>
+  <si>
+    <t>:cf*birm</t>
+  </si>
+  <si>
+    <t>:cf*man</t>
+  </si>
+  <si>
+    <t>:other*new</t>
+  </si>
+  <si>
+    <t>:other*pap</t>
+  </si>
+  <si>
+    <t>:other*hare</t>
+  </si>
+  <si>
+    <t>:other*birm</t>
+  </si>
+  <si>
+    <t>:other*man</t>
+  </si>
+  <si>
+    <t>:pf*new</t>
+  </si>
+  <si>
+    <t>:pf*pap</t>
+  </si>
+  <si>
+    <t>:pf*hare</t>
+  </si>
+  <si>
+    <t>:pf*birm</t>
+  </si>
+  <si>
+    <t>:pf*man</t>
+  </si>
+  <si>
+    <t>:copd*new</t>
+  </si>
+  <si>
+    <t>:copd*pap</t>
+  </si>
+  <si>
+    <t>:copd*hare</t>
+  </si>
+  <si>
+    <t>:copd*birm</t>
+  </si>
+  <si>
+    <t>:copd*man</t>
+  </si>
+  <si>
+    <t>:t1*other</t>
+  </si>
+  <si>
+    <t>:t1*pf</t>
+  </si>
+  <si>
+    <t>;t1*cf</t>
+  </si>
+  <si>
+    <t>:t1*copd</t>
+  </si>
+  <si>
+    <t>:t2*other</t>
+  </si>
+  <si>
+    <t>:t2*pf</t>
+  </si>
+  <si>
+    <t>:t2*cf</t>
+  </si>
+  <si>
+    <t>:t2*copd</t>
+  </si>
+  <si>
+    <t>:type*d-gp</t>
+  </si>
+  <si>
+    <t>:centre*d-gp</t>
+  </si>
+  <si>
+    <t>:d-gp*centre</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1755,13 +1761,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>36</v>
@@ -1773,7 +1779,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>39</v>
@@ -1781,16 +1787,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="E2" s="42">
         <v>-0.27407999999999999</v>
@@ -1799,7 +1805,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="I2" s="70">
         <v>2.2999999999999998</v>
@@ -1808,14 +1814,14 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="14" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E3" s="43">
         <v>0</v>
@@ -1836,13 +1842,13 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>63</v>
@@ -1854,18 +1860,18 @@
         <v>42</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="I5" s="70">
         <v>2.1</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="16" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>25</v>
@@ -1881,7 +1887,7 @@
         <v>2.1</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1898,10 +1904,10 @@
         <v>111</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>112</v>
+        <v>268</v>
       </c>
       <c r="C8" s="82" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D8" s="14">
         <v>0</v>
@@ -1913,7 +1919,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="I8" s="70">
         <v>1.4</v>
@@ -1925,11 +1931,11 @@
         <v>111</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>195</v>
+        <v>269</v>
       </c>
       <c r="C9" s="82"/>
       <c r="D9" s="14" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="E9" s="44">
         <v>-0.31792999999999999</v>
@@ -1944,7 +1950,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>156</v>
+        <v>270</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="14" t="s">
@@ -1972,13 +1978,13 @@
         <v>36</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>114</v>
+        <v>272</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="E12" s="44">
         <v>-4.5809999999999997E-2</v>
@@ -1996,11 +2002,11 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>115</v>
+        <v>273</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="14" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="E13" s="46">
         <v>0</v>
@@ -2021,13 +2027,13 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>107</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>78</v>
@@ -2039,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I15" s="70">
         <v>1.7</v>
@@ -2048,7 +2054,7 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>108</v>
@@ -2068,7 +2074,7 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>109</v>
@@ -2081,7 +2087,7 @@
         <v>-0.13768</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I17" s="70">
         <v>1.7</v>
@@ -2090,7 +2096,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>110</v>
@@ -2103,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I18" s="70">
         <v>1.7</v>
@@ -2124,24 +2130,24 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="44"/>
       <c r="F20" s="80" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="I20" s="70">
         <v>1.2</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2149,14 +2155,14 @@
         <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D21" s="40"/>
       <c r="E21" s="44">
         <v>-4.6809999999999997E-2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I21" s="70"/>
       <c r="J21" s="12"/>
@@ -2166,7 +2172,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="40"/>
@@ -2174,7 +2180,7 @@
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I22" s="70"/>
       <c r="J22" s="12"/>
@@ -2184,7 +2190,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="40"/>
@@ -2192,7 +2198,7 @@
         <v>-3.4199999999999999E-3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I23" s="70"/>
       <c r="J23" s="12"/>
@@ -2208,20 +2214,20 @@
     </row>
     <row r="25" spans="1:10" ht="45">
       <c r="A25" s="16" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="44">
         <v>0.12</v>
       </c>
       <c r="F25" s="80" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="I25" s="70">
         <v>2.2000000000000002</v>
@@ -2243,20 +2249,20 @@
         <v>106</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="D27" s="41"/>
       <c r="E27" s="44">
         <v>-1.8380000000000001E-2</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="I27" s="70">
         <v>1.5</v>
@@ -2274,23 +2280,23 @@
     </row>
     <row r="29" spans="1:10" ht="45">
       <c r="A29" s="16" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="48">
         <v>-5.1040000000000005E-4</v>
       </c>
       <c r="F29" s="80" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="I29" s="70">
         <v>1.1000000000000001</v>
@@ -2308,23 +2314,23 @@
     </row>
     <row r="31" spans="1:10" ht="30">
       <c r="A31" s="16" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="D31" s="41"/>
       <c r="E31" s="44">
         <v>-0.33889999999999998</v>
       </c>
       <c r="F31" s="80" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="I31" s="70">
         <v>2.2999999999999998</v>
@@ -2349,156 +2355,156 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>197</v>
+        <v>294</v>
       </c>
       <c r="C34" s="82"/>
       <c r="D34" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="E34" s="44">
         <v>-0.27877999999999997</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I34" s="70"/>
       <c r="J34" s="12" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>198</v>
+        <v>295</v>
       </c>
       <c r="C35" s="82"/>
       <c r="D35" s="3" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E35" s="44">
         <v>0.34847</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I35" s="70"/>
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>200</v>
+        <v>296</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E36" s="46">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I36" s="70"/>
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>199</v>
+        <v>297</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E37" s="46">
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I37" s="70"/>
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>201</v>
+        <v>298</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E38" s="46">
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I38" s="70"/>
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>202</v>
+        <v>299</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="E39" s="46">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I39" s="70"/>
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>203</v>
+        <v>300</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="E40" s="46">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I40" s="70"/>
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>204</v>
+        <v>301</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="E41" s="46">
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I41" s="70"/>
       <c r="J41" s="12"/>
@@ -2578,7 +2584,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -13172,7 +13178,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="52" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>25</v>
@@ -13204,7 +13210,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>110</v>
@@ -13212,7 +13218,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="54" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>62</v>
@@ -13220,7 +13226,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="41" t="s">
         <v>62</v>
@@ -13236,7 +13242,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="14">
         <v>23.038</v>
@@ -13247,15 +13253,15 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13279,8 +13285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13305,13 +13311,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>36</v>
@@ -13323,7 +13329,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="J1" s="61" t="s">
         <v>39</v>
@@ -13522,7 +13528,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>107</v>
@@ -13546,7 +13552,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>108</v>
@@ -13565,7 +13571,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>109</v>
@@ -13584,7 +13590,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>110</v>
@@ -13611,13 +13617,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="16" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>63</v>
@@ -13635,7 +13641,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="16" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>25</v>
@@ -13662,7 +13668,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>26</v>
@@ -13686,7 +13692,7 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>25</v>
@@ -13716,7 +13722,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>65</v>
@@ -13726,13 +13732,13 @@
         <v>2.82E-3</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="I24" s="72">
         <v>1.7</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -13745,10 +13751,10 @@
     </row>
     <row r="26" spans="1:10" ht="42" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>67</v>
@@ -13758,7 +13764,7 @@
         <v>-1.452E-2</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="I26" s="72">
         <v>1.8</v>
@@ -13774,11 +13780,11 @@
       <c r="J27" s="60"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
-      <c r="A28" s="16" t="s">
-        <v>130</v>
+      <c r="A28" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>135</v>
+        <v>274</v>
       </c>
       <c r="C28" s="82"/>
       <c r="D28" s="14" t="s">
@@ -13788,21 +13794,21 @@
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="I28" s="72">
         <v>10</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
-      <c r="A29" s="16" t="s">
-        <v>130</v>
+      <c r="A29" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>131</v>
+        <v>275</v>
       </c>
       <c r="C29" s="82"/>
       <c r="D29" s="14" t="s">
@@ -13812,16 +13818,16 @@
         <v>-0.10414</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="16" t="s">
-        <v>130</v>
+      <c r="A30" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="41" t="s">
@@ -13831,16 +13837,16 @@
         <v>2.1700000000000001E-3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J30" s="60"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="16" t="s">
-        <v>130</v>
+      <c r="A31" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>133</v>
+        <v>277</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="14" t="s">
@@ -13850,16 +13856,16 @@
         <v>1.8270000000000002E-2</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J31" s="60"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="16" t="s">
-        <v>130</v>
+      <c r="A32" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>134</v>
+        <v>278</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>89</v>
@@ -13868,16 +13874,16 @@
         <v>-8.7040000000000006E-2</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J32" s="60"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="16" t="s">
-        <v>130</v>
+      <c r="A33" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>140</v>
+        <v>279</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="14" t="s">
@@ -13887,16 +13893,16 @@
         <v>0</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A34" s="16" t="s">
-        <v>130</v>
+      <c r="A34" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>136</v>
+        <v>280</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="14" t="s">
@@ -13906,18 +13912,18 @@
         <v>7.2209999999999996E-2</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="16" t="s">
-        <v>130</v>
+      <c r="A35" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>137</v>
+        <v>281</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>92</v>
@@ -13926,18 +13932,18 @@
         <v>-0.29171999999999998</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J35" s="62" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="16" t="s">
-        <v>130</v>
+      <c r="A36" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>138</v>
+        <v>282</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>93</v>
@@ -13946,16 +13952,16 @@
         <v>-0.36563000000000001</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="16" t="s">
-        <v>130</v>
+      <c r="A37" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>139</v>
+        <v>283</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>94</v>
@@ -13964,16 +13970,16 @@
         <v>7.6780000000000001E-2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="16" t="s">
-        <v>130</v>
+      <c r="A38" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>219</v>
+        <v>284</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>100</v>
@@ -13982,16 +13988,16 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>285</v>
-      </c>
-      <c r="J38" s="13"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>96</v>
@@ -14000,16 +14006,16 @@
         <v>0.47683999999999999</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="16" t="s">
-        <v>130</v>
+      <c r="A40" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>142</v>
+        <v>286</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>97</v>
@@ -14018,16 +14024,16 @@
         <v>0.38514999999999999</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="16" t="s">
-        <v>130</v>
+      <c r="A41" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>143</v>
+        <v>287</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>98</v>
@@ -14036,16 +14042,16 @@
         <v>-0.22559999999999999</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="16" t="s">
-        <v>130</v>
+      <c r="A42" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>144</v>
+        <v>288</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>99</v>
@@ -14054,16 +14060,16 @@
         <v>0.57589999999999997</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="16" t="s">
-        <v>130</v>
+      <c r="A43" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>150</v>
+        <v>289</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>105</v>
@@ -14072,16 +14078,16 @@
         <v>0</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J43" s="13"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="16" t="s">
-        <v>130</v>
+      <c r="A44" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>101</v>
@@ -14090,16 +14096,16 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="16" t="s">
-        <v>130</v>
+      <c r="A45" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>147</v>
+        <v>291</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>102</v>
@@ -14108,16 +14114,16 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="16" t="s">
-        <v>130</v>
+      <c r="A46" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>148</v>
+        <v>292</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>103</v>
@@ -14126,16 +14132,16 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="16" t="s">
-        <v>130</v>
+      <c r="A47" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>149</v>
+        <v>293</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>104</v>
@@ -14144,7 +14150,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J47" s="13"/>
     </row>
@@ -14174,104 +14180,104 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="C1" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="D1" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="E1" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="63" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>269</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="63" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="63" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="E4" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="63" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="E5" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="63" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -14303,46 +14309,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="35" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="35" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="35" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -14391,7 +14397,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>12</v>
@@ -47412,7 +47418,7 @@
     </row>
     <row r="2" spans="1:9" ht="16">
       <c r="A2" s="20" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>25</v>
@@ -47428,10 +47434,10 @@
     </row>
     <row r="4" spans="1:9" ht="16">
       <c r="A4" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16">
@@ -47444,7 +47450,7 @@
     </row>
     <row r="6" spans="1:9" ht="16">
       <c r="A6" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>110</v>
@@ -47455,12 +47461,12 @@
         <v>111</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16">
       <c r="A8" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>25</v>
@@ -47476,7 +47482,7 @@
     </row>
     <row r="10" spans="1:9" ht="16">
       <c r="A10" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="19">
         <v>23.022400000000001</v>
@@ -47500,7 +47506,7 @@
     </row>
     <row r="13" spans="1:9" ht="16">
       <c r="A13" s="20" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B13" s="19">
         <v>9</v>
@@ -47516,10 +47522,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -47527,7 +47533,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -47539,8 +47545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47570,10 +47576,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>32</v>
@@ -47597,7 +47603,7 @@
         <v>38</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>39</v>
@@ -47685,7 +47691,7 @@
     </row>
     <row r="5" spans="1:13" ht="16">
       <c r="A5" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>107</v>
@@ -47712,10 +47718,10 @@
         <v>46</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L5" s="69">
         <v>1.0900000000000001</v>
@@ -47726,7 +47732,7 @@
     </row>
     <row r="6" spans="1:13" ht="16">
       <c r="A6" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>108</v>
@@ -47755,7 +47761,7 @@
     </row>
     <row r="7" spans="1:13" ht="16">
       <c r="A7" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>109</v>
@@ -47778,7 +47784,7 @@
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="69">
@@ -47787,7 +47793,7 @@
     </row>
     <row r="8" spans="1:13" ht="16">
       <c r="A8" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>110</v>
@@ -47810,7 +47816,7 @@
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="69">
@@ -47834,7 +47840,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="C10" s="81" t="s">
         <v>71</v>
@@ -47858,10 +47864,10 @@
         <v>42</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L10" s="69">
         <v>1.03</v>
@@ -47872,7 +47878,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="C11" s="81"/>
       <c r="D11" s="22" t="s">
@@ -47902,7 +47908,7 @@
         <v>111</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="19" t="s">
@@ -47945,7 +47951,7 @@
     </row>
     <row r="14" spans="1:13" ht="16">
       <c r="A14" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>26</v>
@@ -47973,7 +47979,7 @@
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L14" s="69">
         <v>1.07</v>
@@ -47981,7 +47987,7 @@
     </row>
     <row r="15" spans="1:13" ht="16">
       <c r="A15" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>25</v>
@@ -48026,10 +48032,10 @@
     </row>
     <row r="17" spans="1:15" ht="16">
       <c r="A17" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>75</v>
@@ -48054,7 +48060,7 @@
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L17" s="69">
         <v>1.05</v>
@@ -48062,10 +48068,10 @@
     </row>
     <row r="18" spans="1:15" ht="16">
       <c r="A18" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="19" t="s">
@@ -48091,10 +48097,10 @@
     </row>
     <row r="19" spans="1:15" ht="16">
       <c r="A19" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="19" t="s">
@@ -48120,10 +48126,10 @@
     </row>
     <row r="20" spans="1:15" ht="16">
       <c r="A20" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="19" t="s">
@@ -48241,7 +48247,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>66</v>
@@ -48252,17 +48258,17 @@
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
       <c r="I25" s="79" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="69">
         <v>1.06</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="16">
@@ -48270,7 +48276,7 @@
         <v>106</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26"/>
@@ -48287,12 +48293,12 @@
         <v>-0.1124</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="M26" s="12" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="16">
@@ -48300,7 +48306,7 @@
         <v>106</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -48317,7 +48323,7 @@
         <v>0.25652000000000003</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -48327,7 +48333,7 @@
         <v>106</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
@@ -48344,7 +48350,7 @@
         <v>-0.47989999999999999</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="57"/>
@@ -48369,24 +48375,24 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="24"/>
       <c r="I30" s="80" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="69">
         <v>1.01</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="16">
@@ -48394,7 +48400,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="24"/>
@@ -48411,12 +48417,12 @@
         <v>-3.1900000000000001E-3</v>
       </c>
       <c r="I31" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
       <c r="M31" s="12" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="16">
@@ -48424,7 +48430,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="24"/>
@@ -48441,7 +48447,7 @@
         <v>3.3849999999999999E-4</v>
       </c>
       <c r="I32" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -48454,7 +48460,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="24"/>
@@ -48471,7 +48477,7 @@
         <v>-8.1760000000000003E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="J33" s="54"/>
       <c r="K33" s="14"/>
@@ -48495,10 +48501,10 @@
     </row>
     <row r="35" spans="1:15" ht="46">
       <c r="A35" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>67</v>
@@ -48517,17 +48523,17 @@
         <v>-1.899E-2</v>
       </c>
       <c r="I35" s="79" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="K35" s="14"/>
       <c r="L35" s="69">
         <v>1.1200000000000001</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1">
@@ -48547,10 +48553,10 @@
     </row>
     <row r="37" spans="1:15" s="12" customFormat="1" ht="36" customHeight="1">
       <c r="A37" s="34" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>64</v>
@@ -48569,17 +48575,17 @@
         <v>-4.6100000000000004E-3</v>
       </c>
       <c r="I37" s="80" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="69">
         <v>1.1299999999999999</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="O37" s="3"/>
     </row>
@@ -48596,13 +48602,13 @@
     </row>
     <row r="39" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A39" s="34" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B39" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>63</v>
@@ -48631,7 +48637,7 @@
     </row>
     <row r="40" spans="1:15" s="12" customFormat="1" ht="16">
       <c r="A40" s="34" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>25</v>
@@ -48795,10 +48801,10 @@
     </row>
     <row r="47" spans="1:15" ht="16">
       <c r="A47" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>131</v>
+        <v>304</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>275</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>86</v>
@@ -48816,7 +48822,7 @@
         <v>-0.33476</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L47" s="69">
         <v>-1</v>
@@ -48827,10 +48833,10 @@
     </row>
     <row r="48" spans="1:15" ht="16">
       <c r="A48" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>132</v>
+        <v>304</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>276</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>87</v>
@@ -48848,21 +48854,21 @@
         <v>-0.25944</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L48" s="69">
         <v>-1</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16">
       <c r="A49" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>133</v>
+        <v>304</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>277</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
@@ -48881,7 +48887,7 @@
         <v>-0.52005999999999997</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L49" s="69">
         <v>-1</v>
@@ -48889,10 +48895,10 @@
     </row>
     <row r="50" spans="1:12" ht="16">
       <c r="A50" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>134</v>
+        <v>304</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>278</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="26" t="s">
@@ -48911,7 +48917,7 @@
         <v>0.21389</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L50" s="69">
         <v>-1</v>
@@ -48919,10 +48925,10 @@
     </row>
     <row r="51" spans="1:12" ht="16">
       <c r="A51" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>135</v>
+        <v>304</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>279</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="26" t="s">
@@ -48941,7 +48947,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L51" s="69">
         <v>-1</v>
@@ -48949,10 +48955,10 @@
     </row>
     <row r="52" spans="1:12" ht="16">
       <c r="A52" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" s="34" t="s">
-        <v>136</v>
+        <v>304</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="C52"/>
       <c r="D52" s="19" t="s">
@@ -48971,7 +48977,7 @@
         <v>-0.22592999999999999</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L52" s="69">
         <v>-1</v>
@@ -48979,10 +48985,10 @@
     </row>
     <row r="53" spans="1:12" ht="16">
       <c r="A53" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B53" s="34" t="s">
-        <v>137</v>
+        <v>304</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="24" t="s">
@@ -49001,7 +49007,7 @@
         <v>-0.67791000000000001</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L53" s="69">
         <v>-1</v>
@@ -49009,10 +49015,10 @@
     </row>
     <row r="54" spans="1:12" ht="16">
       <c r="A54" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" s="34" t="s">
-        <v>138</v>
+        <v>304</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>282</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" t="s">
@@ -49031,7 +49037,7 @@
         <v>-1.9220000000000001E-2</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L54" s="69">
         <v>-1</v>
@@ -49039,10 +49045,10 @@
     </row>
     <row r="55" spans="1:12" ht="16">
       <c r="A55" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="34" t="s">
-        <v>139</v>
+        <v>304</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>283</v>
       </c>
       <c r="C55"/>
       <c r="D55" t="s">
@@ -49061,7 +49067,7 @@
         <v>-0.22169</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L55" s="69">
         <v>-1</v>
@@ -49069,10 +49075,10 @@
     </row>
     <row r="56" spans="1:12" ht="16">
       <c r="A56" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B56" s="34" t="s">
-        <v>140</v>
+        <v>304</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>284</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
@@ -49091,7 +49097,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L56" s="69">
         <v>-1</v>
@@ -49099,10 +49105,10 @@
     </row>
     <row r="57" spans="1:12" ht="16">
       <c r="A57" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>141</v>
+        <v>304</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>285</v>
       </c>
       <c r="C57"/>
       <c r="D57" t="s">
@@ -49121,7 +49127,7 @@
         <v>-0.64468999999999999</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L57" s="69">
         <v>-1</v>
@@ -49129,10 +49135,10 @@
     </row>
     <row r="58" spans="1:12" ht="16">
       <c r="A58" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>142</v>
+        <v>304</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>286</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -49151,7 +49157,7 @@
         <v>-1.1697299999999999</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L58" s="69">
         <v>-1</v>
@@ -49159,10 +49165,10 @@
     </row>
     <row r="59" spans="1:12" ht="16">
       <c r="A59" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>143</v>
+        <v>304</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>287</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
@@ -49181,7 +49187,7 @@
         <v>-0.45308999999999999</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L59" s="69">
         <v>-1</v>
@@ -49189,10 +49195,10 @@
     </row>
     <row r="60" spans="1:12" ht="16">
       <c r="A60" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" s="34" t="s">
-        <v>144</v>
+        <v>304</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>288</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
@@ -49211,7 +49217,7 @@
         <v>-0.11143</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L60" s="69">
         <v>-1</v>
@@ -49219,10 +49225,10 @@
     </row>
     <row r="61" spans="1:12" ht="16">
       <c r="A61" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>145</v>
+        <v>304</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
@@ -49241,7 +49247,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L61" s="69">
         <v>-1</v>
@@ -49249,10 +49255,10 @@
     </row>
     <row r="62" spans="1:12" ht="16">
       <c r="A62" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="34" t="s">
-        <v>146</v>
+        <v>304</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>290</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
@@ -49271,7 +49277,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L62" s="69">
         <v>-1</v>
@@ -49279,10 +49285,10 @@
     </row>
     <row r="63" spans="1:12" ht="16">
       <c r="A63" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B63" s="34" t="s">
-        <v>147</v>
+        <v>304</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>291</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
@@ -49301,7 +49307,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L63" s="69">
         <v>-1</v>
@@ -49309,10 +49315,10 @@
     </row>
     <row r="64" spans="1:12" ht="16">
       <c r="A64" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>148</v>
+        <v>304</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
@@ -49331,7 +49337,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L64" s="69">
         <v>-1</v>
@@ -49339,10 +49345,10 @@
     </row>
     <row r="65" spans="1:12" ht="16">
       <c r="A65" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="34" t="s">
-        <v>149</v>
+        <v>304</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>293</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
@@ -49361,7 +49367,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L65" s="69">
         <v>-1</v>
@@ -49369,10 +49375,10 @@
     </row>
     <row r="66" spans="1:12" ht="16">
       <c r="A66" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" s="34" t="s">
-        <v>150</v>
+        <v>304</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -49391,7 +49397,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="L66" s="69">
         <v>-1</v>
@@ -49431,39 +49437,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="35" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>125</v>
-      </c>
       <c r="E1" s="35" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="49" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>106</v>
@@ -49490,12 +49496,12 @@
         <v>3.55</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="49" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>21</v>
@@ -49522,15 +49528,15 @@
         <v>63</v>
       </c>
       <c r="J3" s="64" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="49" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -49542,15 +49548,15 @@
         <v>0</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="49" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -49562,12 +49568,12 @@
         <v>0</v>
       </c>
       <c r="J5" s="64" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="49" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>21</v>
@@ -49594,15 +49600,15 @@
         <v>63</v>
       </c>
       <c r="J6" s="64" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="A7" s="49" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="C7">
         <v>-2.2000000000000002</v>
@@ -49618,12 +49624,12 @@
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7" s="12" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1">
       <c r="A8" s="49" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>106</v>
@@ -49645,10 +49651,10 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1">
       <c r="A9" s="49" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C9" s="45">
         <v>1</v>
@@ -49664,15 +49670,15 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9" s="12" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1">
       <c r="A10" s="49" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="C10" s="45">
         <v>1.3</v>
@@ -49687,7 +49693,7 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1">
       <c r="A11" s="49" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B11" s="49" t="s">
         <v>21</v>
@@ -49702,15 +49708,15 @@
         <v>0</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1">
       <c r="A12" s="49" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="45">
         <v>14</v>
@@ -49864,7 +49870,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -55943,15 +55949,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="67" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="67" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>25</v>
@@ -55962,7 +55968,7 @@
         <v>111</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -55970,12 +55976,12 @@
         <v>36</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>110</v>
@@ -55986,15 +55992,15 @@
         <v>21</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="67" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -56007,7 +56013,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="67" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B10" s="14">
         <v>9</v>
@@ -56015,7 +56021,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="67" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B11" s="14">
         <v>4.9000000000000004</v>
@@ -56026,15 +56032,15 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="67" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>

<commit_message>
beta-xs calculation wip. num inc/dec
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDB19A-D3D6-D248-BB17-4019F978B03A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C055D3-A221-7E43-82DF-FE42625F8834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="-23400" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="12" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1500" yWindow="-23400" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="303">
   <si>
     <t>Notes</t>
   </si>
@@ -845,9 +845,6 @@
     <t>:none</t>
   </si>
   <si>
-    <t>[:spline :x :age-beta1 :age-beta2 age-beta3]</t>
-  </si>
-  <si>
     <t>:cif-all-reasons</t>
   </si>
   <si>
@@ -954,9 +951,6 @@
   </si>
   <si>
     <t>:type*d-gp</t>
-  </si>
-  <si>
-    <t>:centre*d-gp</t>
   </si>
   <si>
     <t>:d-gp*centre</t>
@@ -1735,14 +1729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A41"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
@@ -1904,7 +1898,7 @@
         <v>111</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C8" s="82" t="s">
         <v>148</v>
@@ -1931,7 +1925,7 @@
         <v>111</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="82"/>
       <c r="D9" s="14" t="s">
@@ -1950,7 +1944,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="14" t="s">
@@ -1978,7 +1972,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>149</v>
@@ -2002,7 +1996,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="14" t="s">
@@ -2355,10 +2349,10 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C34" s="82"/>
       <c r="D34" s="3" t="s">
@@ -2377,10 +2371,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C35" s="82"/>
       <c r="D35" s="3" t="s">
@@ -2397,10 +2391,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>164</v>
@@ -2416,10 +2410,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>165</v>
@@ -2435,10 +2429,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>166</v>
@@ -2454,10 +2448,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>167</v>
@@ -2473,10 +2467,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>168</v>
@@ -2492,10 +2486,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>169</v>
@@ -13285,8 +13279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BE17B6-B2E7-0449-9CFC-F43777FD6637}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A28:A29"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B47" sqref="B28:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13781,10 +13775,10 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C28" s="82"/>
       <c r="D28" s="14" t="s">
@@ -13805,10 +13799,10 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" s="82"/>
       <c r="D29" s="14" t="s">
@@ -13824,10 +13818,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="41" t="s">
@@ -13843,10 +13837,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="14" t="s">
@@ -13862,10 +13856,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>89</v>
@@ -13880,10 +13874,10 @@
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
       <c r="A33" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="14" t="s">
@@ -13899,10 +13893,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="14" t="s">
@@ -13920,10 +13914,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>92</v>
@@ -13940,10 +13934,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>93</v>
@@ -13958,10 +13952,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>94</v>
@@ -13976,10 +13970,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>100</v>
@@ -13994,10 +13988,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>96</v>
@@ -14012,10 +14006,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>97</v>
@@ -14030,10 +14024,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>98</v>
@@ -14048,10 +14042,10 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>99</v>
@@ -14066,10 +14060,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>105</v>
@@ -14084,10 +14078,10 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>101</v>
@@ -14102,10 +14096,10 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>102</v>
@@ -14120,10 +14114,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>103</v>
@@ -14138,10 +14132,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>104</v>
@@ -14397,7 +14391,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>12</v>
@@ -47545,8 +47539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47840,7 +47834,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C10" s="81" t="s">
         <v>71</v>
@@ -47878,7 +47872,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C11" s="81"/>
       <c r="D11" s="22" t="s">
@@ -47908,7 +47902,7 @@
         <v>111</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="19" t="s">
@@ -48375,7 +48369,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>65</v>
@@ -48575,7 +48569,7 @@
         <v>-4.6100000000000004E-3</v>
       </c>
       <c r="I37" s="80" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>192</v>
@@ -48801,10 +48795,10 @@
     </row>
     <row r="47" spans="1:15" ht="16">
       <c r="A47" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>86</v>
@@ -48833,10 +48827,10 @@
     </row>
     <row r="48" spans="1:15" ht="16">
       <c r="A48" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>87</v>
@@ -48865,10 +48859,10 @@
     </row>
     <row r="49" spans="1:12" ht="16">
       <c r="A49" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
@@ -48895,10 +48889,10 @@
     </row>
     <row r="50" spans="1:12" ht="16">
       <c r="A50" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="26" t="s">
@@ -48925,10 +48919,10 @@
     </row>
     <row r="51" spans="1:12" ht="16">
       <c r="A51" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="26" t="s">
@@ -48955,10 +48949,10 @@
     </row>
     <row r="52" spans="1:12" ht="16">
       <c r="A52" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C52"/>
       <c r="D52" s="19" t="s">
@@ -48985,10 +48979,10 @@
     </row>
     <row r="53" spans="1:12" ht="16">
       <c r="A53" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="24" t="s">
@@ -49015,10 +49009,10 @@
     </row>
     <row r="54" spans="1:12" ht="16">
       <c r="A54" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" t="s">
@@ -49045,10 +49039,10 @@
     </row>
     <row r="55" spans="1:12" ht="16">
       <c r="A55" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C55"/>
       <c r="D55" t="s">
@@ -49075,10 +49069,10 @@
     </row>
     <row r="56" spans="1:12" ht="16">
       <c r="A56" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
@@ -49105,10 +49099,10 @@
     </row>
     <row r="57" spans="1:12" ht="16">
       <c r="A57" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C57"/>
       <c r="D57" t="s">
@@ -49135,10 +49129,10 @@
     </row>
     <row r="58" spans="1:12" ht="16">
       <c r="A58" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -49165,10 +49159,10 @@
     </row>
     <row r="59" spans="1:12" ht="16">
       <c r="A59" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
@@ -49195,10 +49189,10 @@
     </row>
     <row r="60" spans="1:12" ht="16">
       <c r="A60" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
@@ -49225,10 +49219,10 @@
     </row>
     <row r="61" spans="1:12" ht="16">
       <c r="A61" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
@@ -49255,10 +49249,10 @@
     </row>
     <row r="62" spans="1:12" ht="16">
       <c r="A62" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
@@ -49285,10 +49279,10 @@
     </row>
     <row r="63" spans="1:12" ht="16">
       <c r="A63" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
@@ -49315,10 +49309,10 @@
     </row>
     <row r="64" spans="1:12" ht="16">
       <c r="A64" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
@@ -49345,10 +49339,10 @@
     </row>
     <row r="65" spans="1:12" ht="16">
       <c r="A65" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
@@ -49375,10 +49369,10 @@
     </row>
     <row r="66" spans="1:12" ht="16">
       <c r="A66" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>289</v>
+        <v>302</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>288</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">

</xml_diff>

<commit_message>
lung and kidney models are go
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308AE73D-72B3-E349-A423-8CB9A3443422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B5D91-9D9E-3E4D-AEF2-01924EA1D404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="-23400" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="2160" yWindow="-23200" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="7" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -662,9 +662,6 @@
     <t>mmol/l</t>
   </si>
   <si>
-    <t>:cif-survival</t>
-  </si>
-  <si>
     <t>:cif-from-listing</t>
   </si>
   <si>
@@ -939,6 +936,9 @@
   </si>
   <si>
     <t>:nyha-4</t>
+  </si>
+  <si>
+    <t>:cif-post-transplant</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1740,13 +1740,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>243</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>36</v>
@@ -1758,7 +1758,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>39</v>
@@ -1883,7 +1883,7 @@
         <v>111</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8" s="82" t="s">
         <v>146</v>
@@ -1910,7 +1910,7 @@
         <v>111</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="82"/>
       <c r="D9" s="14" t="s">
@@ -1929,7 +1929,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="14" t="s">
@@ -1957,7 +1957,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>147</v>
@@ -1981,7 +1981,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="14" t="s">
@@ -2109,7 +2109,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>150</v>
@@ -2117,7 +2117,7 @@
       <c r="D20" s="40"/>
       <c r="E20" s="44"/>
       <c r="F20" s="80" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>202</v>
@@ -2141,7 +2141,7 @@
         <v>-4.6809999999999997E-2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I21" s="70"/>
       <c r="J21" s="12"/>
@@ -2159,7 +2159,7 @@
         <v>1.5200000000000001E-3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I22" s="70"/>
       <c r="J22" s="12"/>
@@ -2177,7 +2177,7 @@
         <v>-3.4199999999999999E-3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I23" s="70"/>
       <c r="J23" s="12"/>
@@ -2206,7 +2206,7 @@
         <v>0.12</v>
       </c>
       <c r="F25" s="80" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I25" s="70">
         <v>2.2000000000000002</v>
@@ -2238,7 +2238,7 @@
         <v>-1.8380000000000001E-2</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>191</v>
@@ -2272,7 +2272,7 @@
         <v>-5.1040000000000005E-4</v>
       </c>
       <c r="F29" s="80" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>190</v>
@@ -2306,13 +2306,13 @@
         <v>-0.33889999999999998</v>
       </c>
       <c r="F31" s="80" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>204</v>
       </c>
       <c r="I31" s="70">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="J31" s="12"/>
     </row>
@@ -2334,10 +2334,10 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34" s="82"/>
       <c r="D34" s="3" t="s">
@@ -2347,7 +2347,7 @@
         <v>-0.27877999999999997</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I34" s="70"/>
       <c r="J34" s="12" t="s">
@@ -2356,10 +2356,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C35" s="82"/>
       <c r="D35" s="3" t="s">
@@ -2369,17 +2369,17 @@
         <v>0.34847</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I35" s="70"/>
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>162</v>
@@ -2388,17 +2388,17 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I36" s="70"/>
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>163</v>
@@ -2407,17 +2407,17 @@
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I37" s="70"/>
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>164</v>
@@ -2426,17 +2426,17 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I38" s="70"/>
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>165</v>
@@ -2445,17 +2445,17 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I39" s="70"/>
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>166</v>
@@ -2464,17 +2464,17 @@
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I40" s="70"/>
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>167</v>
@@ -2483,7 +2483,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I41" s="70"/>
       <c r="J41" s="12"/>
@@ -2563,7 +2563,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -13232,7 +13232,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -13240,7 +13240,7 @@
         <v>127</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13290,13 +13290,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>243</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>36</v>
@@ -13308,7 +13308,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J1" s="61" t="s">
         <v>39</v>
@@ -13711,7 +13711,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I24" s="72">
         <v>1.7</v>
@@ -13743,7 +13743,7 @@
         <v>-1.452E-2</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I26" s="72">
         <v>1.8</v>
@@ -13760,10 +13760,10 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" s="82"/>
       <c r="D28" s="14" t="s">
@@ -13773,7 +13773,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I28" s="72">
         <v>10</v>
@@ -13784,10 +13784,10 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C29" s="82"/>
       <c r="D29" s="14" t="s">
@@ -13797,16 +13797,16 @@
         <v>-0.10414</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="41" t="s">
@@ -13816,16 +13816,16 @@
         <v>2.1700000000000001E-3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J30" s="60"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="14" t="s">
@@ -13835,16 +13835,16 @@
         <v>1.8270000000000002E-2</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J31" s="60"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>89</v>
@@ -13853,16 +13853,16 @@
         <v>-8.7040000000000006E-2</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J32" s="60"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
       <c r="A33" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="14" t="s">
@@ -13872,16 +13872,16 @@
         <v>0</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="14" t="s">
@@ -13891,7 +13891,7 @@
         <v>7.2209999999999996E-2</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J34" s="62" t="s">
         <v>187</v>
@@ -13899,10 +13899,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>92</v>
@@ -13911,7 +13911,7 @@
         <v>-0.29171999999999998</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J35" s="62" t="s">
         <v>188</v>
@@ -13919,10 +13919,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>93</v>
@@ -13931,16 +13931,16 @@
         <v>-0.36563000000000001</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>94</v>
@@ -13949,16 +13949,16 @@
         <v>7.6780000000000001E-2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>100</v>
@@ -13967,16 +13967,16 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>96</v>
@@ -13985,16 +13985,16 @@
         <v>0.47683999999999999</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>97</v>
@@ -14003,16 +14003,16 @@
         <v>0.38514999999999999</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>98</v>
@@ -14021,16 +14021,16 @@
         <v>-0.22559999999999999</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>99</v>
@@ -14039,16 +14039,16 @@
         <v>0.57589999999999997</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>105</v>
@@ -14057,16 +14057,16 @@
         <v>0</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J43" s="13"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>101</v>
@@ -14075,16 +14075,16 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>102</v>
@@ -14093,16 +14093,16 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>103</v>
@@ -14111,16 +14111,16 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>104</v>
@@ -14129,7 +14129,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J47" s="13"/>
     </row>
@@ -14159,104 +14159,104 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -14288,13 +14288,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -14302,10 +14302,10 @@
         <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14313,10 +14313,10 @@
         <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14324,10 +14324,10 @@
         <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -14376,7 +14376,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>12</v>
@@ -47504,7 +47504,7 @@
         <v>127</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -47512,7 +47512,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -47555,10 +47555,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>242</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>32</v>
@@ -47582,7 +47582,7 @@
         <v>38</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>39</v>
@@ -47819,7 +47819,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C10" s="81" t="s">
         <v>71</v>
@@ -47857,7 +47857,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="81"/>
       <c r="D11" s="22" t="s">
@@ -47887,7 +47887,7 @@
         <v>111</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="19" t="s">
@@ -48014,7 +48014,7 @@
         <v>115</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>75</v>
@@ -48050,7 +48050,7 @@
         <v>115</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="19" t="s">
@@ -48079,7 +48079,7 @@
         <v>115</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="19" t="s">
@@ -48108,7 +48108,7 @@
         <v>115</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="19" t="s">
@@ -48226,7 +48226,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>66</v>
@@ -48237,7 +48237,7 @@
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
       <c r="I25" s="79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>191</v>
@@ -48272,7 +48272,7 @@
         <v>-0.1124</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
@@ -48302,7 +48302,7 @@
         <v>0.25652000000000003</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -48329,7 +48329,7 @@
         <v>-0.47989999999999999</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="57"/>
@@ -48354,14 +48354,14 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="24"/>
       <c r="I30" s="80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>202</v>
@@ -48396,7 +48396,7 @@
         <v>-3.1900000000000001E-3</v>
       </c>
       <c r="I31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
@@ -48426,7 +48426,7 @@
         <v>3.3849999999999999E-4</v>
       </c>
       <c r="I32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -48456,7 +48456,7 @@
         <v>-8.1760000000000003E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J33" s="54"/>
       <c r="K33" s="14"/>
@@ -48502,7 +48502,7 @@
         <v>-1.899E-2</v>
       </c>
       <c r="I35" s="79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>203</v>
@@ -48554,7 +48554,7 @@
         <v>-4.6100000000000004E-3</v>
       </c>
       <c r="I37" s="80" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>190</v>
@@ -48780,10 +48780,10 @@
     </row>
     <row r="47" spans="1:15" ht="16">
       <c r="A47" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>86</v>
@@ -48801,7 +48801,7 @@
         <v>-0.33476</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L47" s="69">
         <v>-1</v>
@@ -48812,10 +48812,10 @@
     </row>
     <row r="48" spans="1:15" ht="16">
       <c r="A48" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>87</v>
@@ -48833,7 +48833,7 @@
         <v>-0.25944</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L48" s="69">
         <v>-1</v>
@@ -48844,10 +48844,10 @@
     </row>
     <row r="49" spans="1:12" ht="16">
       <c r="A49" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
@@ -48866,7 +48866,7 @@
         <v>-0.52005999999999997</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L49" s="69">
         <v>-1</v>
@@ -48874,10 +48874,10 @@
     </row>
     <row r="50" spans="1:12" ht="16">
       <c r="A50" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="26" t="s">
@@ -48896,7 +48896,7 @@
         <v>0.21389</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L50" s="69">
         <v>-1</v>
@@ -48904,10 +48904,10 @@
     </row>
     <row r="51" spans="1:12" ht="16">
       <c r="A51" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="26" t="s">
@@ -48926,7 +48926,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L51" s="69">
         <v>-1</v>
@@ -48934,10 +48934,10 @@
     </row>
     <row r="52" spans="1:12" ht="16">
       <c r="A52" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C52"/>
       <c r="D52" s="19" t="s">
@@ -48956,7 +48956,7 @@
         <v>-0.22592999999999999</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L52" s="69">
         <v>-1</v>
@@ -48964,10 +48964,10 @@
     </row>
     <row r="53" spans="1:12" ht="16">
       <c r="A53" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="24" t="s">
@@ -48986,7 +48986,7 @@
         <v>-0.67791000000000001</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L53" s="69">
         <v>-1</v>
@@ -48994,10 +48994,10 @@
     </row>
     <row r="54" spans="1:12" ht="16">
       <c r="A54" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" t="s">
@@ -49016,7 +49016,7 @@
         <v>-1.9220000000000001E-2</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L54" s="69">
         <v>-1</v>
@@ -49024,10 +49024,10 @@
     </row>
     <row r="55" spans="1:12" ht="16">
       <c r="A55" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C55"/>
       <c r="D55" t="s">
@@ -49046,7 +49046,7 @@
         <v>-0.22169</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L55" s="69">
         <v>-1</v>
@@ -49054,10 +49054,10 @@
     </row>
     <row r="56" spans="1:12" ht="16">
       <c r="A56" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
@@ -49076,7 +49076,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L56" s="69">
         <v>-1</v>
@@ -49084,10 +49084,10 @@
     </row>
     <row r="57" spans="1:12" ht="16">
       <c r="A57" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C57"/>
       <c r="D57" t="s">
@@ -49106,7 +49106,7 @@
         <v>-0.64468999999999999</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L57" s="69">
         <v>-1</v>
@@ -49114,10 +49114,10 @@
     </row>
     <row r="58" spans="1:12" ht="16">
       <c r="A58" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -49136,7 +49136,7 @@
         <v>-1.1697299999999999</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L58" s="69">
         <v>-1</v>
@@ -49144,10 +49144,10 @@
     </row>
     <row r="59" spans="1:12" ht="16">
       <c r="A59" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
@@ -49166,7 +49166,7 @@
         <v>-0.45308999999999999</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L59" s="69">
         <v>-1</v>
@@ -49174,10 +49174,10 @@
     </row>
     <row r="60" spans="1:12" ht="16">
       <c r="A60" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
@@ -49196,7 +49196,7 @@
         <v>-0.11143</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L60" s="69">
         <v>-1</v>
@@ -49204,10 +49204,10 @@
     </row>
     <row r="61" spans="1:12" ht="16">
       <c r="A61" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
@@ -49226,7 +49226,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L61" s="69">
         <v>-1</v>
@@ -49234,10 +49234,10 @@
     </row>
     <row r="62" spans="1:12" ht="16">
       <c r="A62" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
@@ -49256,7 +49256,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L62" s="69">
         <v>-1</v>
@@ -49264,10 +49264,10 @@
     </row>
     <row r="63" spans="1:12" ht="16">
       <c r="A63" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
@@ -49286,7 +49286,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L63" s="69">
         <v>-1</v>
@@ -49294,10 +49294,10 @@
     </row>
     <row r="64" spans="1:12" ht="16">
       <c r="A64" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
@@ -49316,7 +49316,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L64" s="69">
         <v>-1</v>
@@ -49324,10 +49324,10 @@
     </row>
     <row r="65" spans="1:12" ht="16">
       <c r="A65" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
@@ -49346,7 +49346,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L65" s="69">
         <v>-1</v>
@@ -49354,10 +49354,10 @@
     </row>
     <row r="66" spans="1:12" ht="16">
       <c r="A66" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -49376,7 +49376,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L66" s="69">
         <v>-1</v>
@@ -49819,8 +49819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -49849,7 +49849,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>205</v>
+        <v>297</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -56011,7 +56011,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -56019,7 +56019,7 @@
         <v>172</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>

<commit_message>
added test case files
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10862C3-CF36-B74D-86C1-53EFF52024EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ECBE5A-3D81-C94A-A7B4-215957583120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="-21580" windowWidth="29680" windowHeight="21500" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1840" yWindow="-21140" windowWidth="29680" windowHeight="21140" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -746,9 +746,6 @@
     <t>{:dps 0, :knot1 21, :knot2 44, :knot3 56, :knot4 63, :max 70, :min 16, :type :numeric}</t>
   </si>
   <si>
-    <t>{:dps 0, :max 100, :min 10, :type :numeric}</t>
-  </si>
-  <si>
     <t>{:dps 0, :knot1 22, :knot2 46, :knot3 56, :knot4 63, :max 70, :min 16, :type :numeric}</t>
   </si>
   <si>
@@ -930,6 +927,9 @@
   </si>
   <si>
     <t>kg/m²</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 100, :min 10, :type :numeric}</t>
   </si>
 </sst>
 </file>
@@ -1772,7 +1772,7 @@
         <v>-0.27407999999999999</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>173</v>
@@ -1874,19 +1874,19 @@
         <v>105</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" s="82" t="s">
         <v>140</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E8" s="44">
         <v>-0.51788000000000001</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I8" s="70">
         <v>1.4</v>
@@ -1898,11 +1898,11 @@
         <v>105</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="82"/>
       <c r="D9" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="44">
         <v>-0.31792999999999999</v>
@@ -1917,11 +1917,11 @@
         <v>105</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E10" s="46">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>141</v>
@@ -1957,7 +1957,7 @@
         <v>-4.5809999999999997E-2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I12" s="70">
         <v>1.6</v>
@@ -1969,7 +1969,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="14" t="s">
@@ -2009,7 +2009,7 @@
         <v>-0.49712000000000001</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G15" s="17"/>
       <c r="I15" s="70">
@@ -2091,7 +2091,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>144</v>
@@ -2099,7 +2099,7 @@
       <c r="D20" s="40"/>
       <c r="E20" s="44"/>
       <c r="F20" s="80" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>193</v>
@@ -2188,7 +2188,7 @@
         <v>0.12</v>
       </c>
       <c r="F25" s="80" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I25" s="70">
         <v>2.2000000000000002</v>
@@ -2220,10 +2220,10 @@
         <v>-1.8380000000000001E-2</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I27" s="70">
         <v>1.5</v>
@@ -2254,7 +2254,7 @@
         <v>-5.1040000000000005E-4</v>
       </c>
       <c r="F29" s="80" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>182</v>
@@ -2288,7 +2288,7 @@
         <v>-0.33889999999999998</v>
       </c>
       <c r="F31" s="80" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>194</v>
@@ -2316,10 +2316,10 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C34" s="82"/>
       <c r="D34" s="3" t="s">
@@ -2338,10 +2338,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C35" s="82"/>
       <c r="D35" s="3" t="s">
@@ -2358,10 +2358,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>155</v>
@@ -2377,10 +2377,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>156</v>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>157</v>
@@ -2415,10 +2415,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>158</v>
@@ -2434,10 +2434,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>159</v>
@@ -2453,10 +2453,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>160</v>
@@ -13504,7 +13504,7 @@
         <v>0.44096000000000002</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I13" s="72">
         <v>1.4</v>
@@ -13539,7 +13539,7 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E15" s="3">
         <v>0.62370000000000003</v>
@@ -13693,7 +13693,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>193</v>
@@ -13728,10 +13728,10 @@
         <v>-1.452E-2</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I26" s="72">
         <v>1.8</v>
@@ -13748,10 +13748,10 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C28" s="82"/>
       <c r="D28" s="14" t="s">
@@ -13772,10 +13772,10 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C29" s="82"/>
       <c r="D29" s="14" t="s">
@@ -13791,10 +13791,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="41" t="s">
@@ -13810,10 +13810,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="14" t="s">
@@ -13829,10 +13829,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>83</v>
@@ -13847,10 +13847,10 @@
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
       <c r="A33" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="14" t="s">
@@ -13866,10 +13866,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="14" t="s">
@@ -13887,10 +13887,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>86</v>
@@ -13907,10 +13907,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>87</v>
@@ -13925,10 +13925,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>88</v>
@@ -13943,10 +13943,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>94</v>
@@ -13961,10 +13961,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>90</v>
@@ -13979,10 +13979,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>91</v>
@@ -13997,10 +13997,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>92</v>
@@ -14015,10 +14015,10 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>93</v>
@@ -14033,10 +14033,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>99</v>
@@ -14051,10 +14051,10 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>95</v>
@@ -14069,10 +14069,10 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>96</v>
@@ -14087,10 +14087,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>97</v>
@@ -14105,10 +14105,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>98</v>
@@ -14293,7 +14293,7 @@
         <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14304,7 +14304,7 @@
         <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14315,7 +14315,7 @@
         <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -14364,7 +14364,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>12</v>
@@ -47512,8 +47512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -47682,7 +47682,7 @@
         <v>7.6469999999999996E-2</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>111</v>
@@ -47735,7 +47735,7 @@
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E7">
         <v>-0.23763999999999999</v>
@@ -47807,13 +47807,13 @@
         <v>105</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" s="81" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E10">
         <v>0.30664000000000002</v>
@@ -47828,7 +47828,7 @@
         <v>-0.12415</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14" t="s">
@@ -47843,11 +47843,11 @@
         <v>105</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" s="81"/>
       <c r="D11" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E11">
         <v>0.15256</v>
@@ -47873,11 +47873,11 @@
         <v>105</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -48000,7 +48000,7 @@
         <v>109</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>72</v>
@@ -48036,7 +48036,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="19" t="s">
@@ -48065,7 +48065,7 @@
         <v>109</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="19" t="s">
@@ -48094,7 +48094,7 @@
         <v>109</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="19" t="s">
@@ -48212,7 +48212,7 @@
         <v>100</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>65</v>
@@ -48226,7 +48226,7 @@
         <v>231</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="69">
@@ -48340,7 +48340,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>64</v>
@@ -48488,10 +48488,10 @@
         <v>-1.899E-2</v>
       </c>
       <c r="I35" s="79" t="s">
-        <v>233</v>
+        <v>294</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K35" s="14"/>
       <c r="L35" s="69">
@@ -48540,7 +48540,7 @@
         <v>-4.6100000000000004E-3</v>
       </c>
       <c r="I37" s="80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>182</v>
@@ -48766,10 +48766,10 @@
     </row>
     <row r="47" spans="1:15" ht="16">
       <c r="A47" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>80</v>
@@ -48787,7 +48787,7 @@
         <v>-0.33476</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L47" s="69">
         <v>-1</v>
@@ -48798,10 +48798,10 @@
     </row>
     <row r="48" spans="1:15" ht="16">
       <c r="A48" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>81</v>
@@ -48819,7 +48819,7 @@
         <v>-0.25944</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L48" s="69">
         <v>-1</v>
@@ -48830,10 +48830,10 @@
     </row>
     <row r="49" spans="1:12" ht="16">
       <c r="A49" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
@@ -48852,7 +48852,7 @@
         <v>-0.52005999999999997</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L49" s="69">
         <v>-1</v>
@@ -48860,10 +48860,10 @@
     </row>
     <row r="50" spans="1:12" ht="16">
       <c r="A50" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="26" t="s">
@@ -48882,7 +48882,7 @@
         <v>0.21389</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L50" s="69">
         <v>-1</v>
@@ -48890,10 +48890,10 @@
     </row>
     <row r="51" spans="1:12" ht="16">
       <c r="A51" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="26" t="s">
@@ -48912,7 +48912,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L51" s="69">
         <v>-1</v>
@@ -48920,10 +48920,10 @@
     </row>
     <row r="52" spans="1:12" ht="16">
       <c r="A52" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C52"/>
       <c r="D52" s="19" t="s">
@@ -48942,7 +48942,7 @@
         <v>-0.22592999999999999</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L52" s="69">
         <v>-1</v>
@@ -48950,10 +48950,10 @@
     </row>
     <row r="53" spans="1:12" ht="16">
       <c r="A53" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="24" t="s">
@@ -48972,7 +48972,7 @@
         <v>-0.67791000000000001</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L53" s="69">
         <v>-1</v>
@@ -48980,10 +48980,10 @@
     </row>
     <row r="54" spans="1:12" ht="16">
       <c r="A54" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" t="s">
@@ -49002,7 +49002,7 @@
         <v>-1.9220000000000001E-2</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L54" s="69">
         <v>-1</v>
@@ -49010,10 +49010,10 @@
     </row>
     <row r="55" spans="1:12" ht="16">
       <c r="A55" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C55"/>
       <c r="D55" t="s">
@@ -49032,7 +49032,7 @@
         <v>-0.22169</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L55" s="69">
         <v>-1</v>
@@ -49040,10 +49040,10 @@
     </row>
     <row r="56" spans="1:12" ht="16">
       <c r="A56" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
@@ -49062,7 +49062,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L56" s="69">
         <v>-1</v>
@@ -49070,10 +49070,10 @@
     </row>
     <row r="57" spans="1:12" ht="16">
       <c r="A57" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C57"/>
       <c r="D57" t="s">
@@ -49092,7 +49092,7 @@
         <v>-0.64468999999999999</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L57" s="69">
         <v>-1</v>
@@ -49100,10 +49100,10 @@
     </row>
     <row r="58" spans="1:12" ht="16">
       <c r="A58" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -49122,7 +49122,7 @@
         <v>-1.1697299999999999</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L58" s="69">
         <v>-1</v>
@@ -49130,10 +49130,10 @@
     </row>
     <row r="59" spans="1:12" ht="16">
       <c r="A59" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
@@ -49152,7 +49152,7 @@
         <v>-0.45308999999999999</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L59" s="69">
         <v>-1</v>
@@ -49160,10 +49160,10 @@
     </row>
     <row r="60" spans="1:12" ht="16">
       <c r="A60" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
@@ -49182,7 +49182,7 @@
         <v>-0.11143</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L60" s="69">
         <v>-1</v>
@@ -49190,10 +49190,10 @@
     </row>
     <row r="61" spans="1:12" ht="16">
       <c r="A61" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
@@ -49212,7 +49212,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L61" s="69">
         <v>-1</v>
@@ -49220,10 +49220,10 @@
     </row>
     <row r="62" spans="1:12" ht="16">
       <c r="A62" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
@@ -49242,7 +49242,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L62" s="69">
         <v>-1</v>
@@ -49250,10 +49250,10 @@
     </row>
     <row r="63" spans="1:12" ht="16">
       <c r="A63" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
@@ -49272,7 +49272,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L63" s="69">
         <v>-1</v>
@@ -49280,10 +49280,10 @@
     </row>
     <row r="64" spans="1:12" ht="16">
       <c r="A64" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
@@ -49302,7 +49302,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L64" s="69">
         <v>-1</v>
@@ -49310,10 +49310,10 @@
     </row>
     <row r="65" spans="1:12" ht="16">
       <c r="A65" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
@@ -49332,7 +49332,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L65" s="69">
         <v>-1</v>
@@ -49340,10 +49340,10 @@
     </row>
     <row r="66" spans="1:12" ht="16">
       <c r="A66" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
@@ -49362,7 +49362,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L66" s="69">
         <v>-1</v>
@@ -49835,7 +49835,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F1" s="10"/>
     </row>

</xml_diff>

<commit_message>
revised bar charts, new ethnicity levels
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C84EB-F2C0-F645-817A-E0E08EEAB6B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01892EC5-9D5D-1F46-BDE5-4386E5A2E055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2060" yWindow="-19320" windowWidth="29680" windowHeight="18400" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="680" yWindow="1300" windowWidth="29680" windowHeight="18400" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="303">
   <si>
     <t>Notes</t>
   </si>
@@ -931,6 +931,30 @@
   <si>
     <t xml:space="preserve">for possible outcomes while waiting for a transplant </t>
   </si>
+  <si>
+    <t>:asian</t>
+  </si>
+  <si>
+    <t>:black</t>
+  </si>
+  <si>
+    <t>:mixed</t>
+  </si>
+  <si>
+    <t>:chinese</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
 </sst>
 </file>
 
@@ -14263,7 +14287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -14327,7 +14351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:L3206"/>
   <sheetViews>
-    <sheetView topLeftCell="A1338" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A605" sqref="A605"/>
     </sheetView>
   </sheetViews>
@@ -47510,10 +47534,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -47995,7 +48019,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>109</v>
       </c>
@@ -48031,7 +48055,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>109</v>
       </c>
@@ -48060,7 +48084,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>109</v>
       </c>
@@ -48089,7 +48113,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>109</v>
       </c>
@@ -48119,7 +48143,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="21"/>
@@ -48131,33 +48155,33 @@
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>24</v>
+        <v>295</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>47</v>
+        <v>299</v>
       </c>
       <c r="E22">
-        <v>-3.7679999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>-0.17666000000000001</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0.44979000000000002</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>8.8719999999999993E-2</v>
+        <v>0</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>42</v>
+        <v>285</v>
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
@@ -48165,16 +48189,16 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>51</v>
+        <v>296</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="19" t="s">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -48195,721 +48219,714 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
+    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>298</v>
+      </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="19"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
+      <c r="D24" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:15" ht="76" x14ac:dyDescent="0.2">
+      <c r="L24" s="69">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="79" t="s">
-        <v>230</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>290</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="69">
-        <v>1.06</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26"/>
-      <c r="E26" s="29">
-        <v>0.28376000000000001</v>
-      </c>
-      <c r="F26" s="29">
-        <v>3.2649999999999998E-2</v>
-      </c>
-      <c r="G26" s="29">
-        <v>-0.52522999999999997</v>
-      </c>
-      <c r="H26" s="29">
-        <v>-0.1124</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>229</v>
+        <v>24</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26">
+        <v>-3.7679999999999998E-2</v>
+      </c>
+      <c r="F26">
+        <v>-0.17666000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.44979000000000002</v>
+      </c>
+      <c r="H26">
+        <v>8.8719999999999993E-2</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
-      <c r="M26" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="L26" s="69">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27" s="29">
-        <v>0.23757</v>
-      </c>
-      <c r="F27" s="29">
-        <v>0.13516</v>
-      </c>
-      <c r="G27" s="29">
-        <v>-0.59109</v>
-      </c>
-      <c r="H27" s="29">
-        <v>0.25652000000000003</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>229</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="14"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="1:15" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="L27" s="69">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="19"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="75">
-        <v>-0.69055999999999995</v>
-      </c>
-      <c r="F28" s="75">
-        <v>-0.45455000000000001</v>
-      </c>
-      <c r="G28" s="75">
-        <v>1.65744</v>
-      </c>
-      <c r="H28" s="75">
-        <v>-0.47989999999999999</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="B29" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="79" t="s">
+        <v>230</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="69">
+        <v>1.06</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30"/>
+      <c r="E30" s="29">
+        <v>0.28376000000000001</v>
+      </c>
+      <c r="F30" s="29">
+        <v>3.2649999999999998E-2</v>
+      </c>
+      <c r="G30" s="29">
+        <v>-0.52522999999999997</v>
+      </c>
+      <c r="H30" s="29">
+        <v>-0.1124</v>
+      </c>
+      <c r="I30" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="76"/>
-    </row>
-    <row r="29" spans="1:15" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="76"/>
-    </row>
-    <row r="30" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="24"/>
-      <c r="I30" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>193</v>
-      </c>
+      <c r="J30" s="14"/>
       <c r="K30" s="14"/>
-      <c r="L30" s="69">
-        <v>1.01</v>
-      </c>
       <c r="M30" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
       <c r="E31" s="29">
-        <v>5.0699999999999999E-3</v>
+        <v>0.23757</v>
       </c>
       <c r="F31" s="29">
-        <v>6.0069999999999998E-2</v>
+        <v>0.13516</v>
       </c>
       <c r="G31" s="29">
-        <v>-1.9789999999999999E-2</v>
+        <v>-0.59109</v>
       </c>
       <c r="H31" s="29">
-        <v>-3.1900000000000001E-3</v>
-      </c>
-      <c r="I31" t="s">
+        <v>0.25652000000000003</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>229</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="M31" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:13" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="75">
+        <v>-0.69055999999999995</v>
+      </c>
+      <c r="F32" s="75">
+        <v>-0.45455000000000001</v>
+      </c>
+      <c r="G32" s="75">
+        <v>1.65744</v>
+      </c>
+      <c r="H32" s="75">
+        <v>-0.47989999999999999</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="76"/>
+    </row>
+    <row r="33" spans="1:15" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="76"/>
+    </row>
+    <row r="34" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="32">
-        <v>-4.2719999999999998E-4</v>
-      </c>
-      <c r="F32" s="29">
-        <v>-1.58E-3</v>
-      </c>
-      <c r="G32" s="29">
-        <v>1.58E-3</v>
-      </c>
-      <c r="H32" s="32">
-        <v>3.3849999999999999E-4</v>
-      </c>
-      <c r="I32" t="s">
-        <v>229</v>
-      </c>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="13"/>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+      <c r="B34" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="I34" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="69">
+        <v>1.01</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="29">
-        <v>1.92E-3</v>
-      </c>
-      <c r="F33" s="29">
-        <v>4.47E-3</v>
-      </c>
-      <c r="G33" s="29">
-        <v>-5.77E-3</v>
-      </c>
-      <c r="H33" s="32">
-        <v>-8.1760000000000003E-4</v>
-      </c>
-      <c r="I33" t="s">
-        <v>229</v>
-      </c>
-      <c r="J33" s="54"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="69"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="69"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" ht="46" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="B35" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>66</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="24"/>
       <c r="E35" s="29">
-        <v>1.457E-2</v>
+        <v>5.0699999999999999E-3</v>
       </c>
       <c r="F35" s="29">
-        <v>-1.618E-2</v>
+        <v>6.0069999999999998E-2</v>
       </c>
       <c r="G35" s="29">
-        <v>-4.8980000000000003E-2</v>
+        <v>-1.9789999999999999E-2</v>
       </c>
       <c r="H35" s="29">
-        <v>-1.899E-2</v>
-      </c>
-      <c r="I35" s="79" t="s">
-        <v>292</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>291</v>
-      </c>
+        <v>-3.1900000000000001E-3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>229</v>
+      </c>
+      <c r="J35" s="14"/>
       <c r="K35" s="14"/>
-      <c r="L35" s="69">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="M35" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
+      <c r="M35" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="C36" s="25"/>
       <c r="D36" s="24"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="14"/>
+      <c r="E36" s="32">
+        <v>-4.2719999999999998E-4</v>
+      </c>
+      <c r="F36" s="29">
+        <v>-1.58E-3</v>
+      </c>
+      <c r="G36" s="29">
+        <v>1.58E-3</v>
+      </c>
+      <c r="H36" s="32">
+        <v>3.3849999999999999E-4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>229</v>
+      </c>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
       <c r="L36" s="69"/>
+      <c r="M36" s="13"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="1:15" s="12" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="32">
-        <v>-4.0910000000000002E-4</v>
+    <row r="37" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="29">
+        <v>1.92E-3</v>
       </c>
       <c r="F37" s="29">
-        <v>-4.8529999999999997E-2</v>
-      </c>
-      <c r="G37" s="32">
-        <v>-4.6600000000000001E-5</v>
-      </c>
-      <c r="H37" s="29">
-        <v>-4.6100000000000004E-3</v>
-      </c>
-      <c r="I37" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="69">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>130</v>
-      </c>
+        <v>4.47E-3</v>
+      </c>
+      <c r="G37" s="29">
+        <v>-5.77E-3</v>
+      </c>
+      <c r="H37" s="32">
+        <v>-8.1760000000000003E-4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>229</v>
+      </c>
+      <c r="J37" s="54"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="69"/>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="26"/>
+    <row r="38" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
       <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>26</v>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="69"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" ht="46" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>62</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D39" s="24"/>
       <c r="E39" s="29">
-        <v>0.44663999999999998</v>
+        <v>1.457E-2</v>
       </c>
       <c r="F39" s="29">
-        <v>-0.49208000000000002</v>
+        <v>-1.618E-2</v>
       </c>
       <c r="G39" s="29">
-        <v>-0.14221</v>
+        <v>-4.8980000000000003E-2</v>
       </c>
       <c r="H39" s="29">
-        <v>0.30010999999999999</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+        <v>-1.899E-2</v>
+      </c>
+      <c r="I39" s="79" t="s">
+        <v>292</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="K39" s="14"/>
       <c r="L39" s="69">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="30">
-        <v>0</v>
-      </c>
-      <c r="F40" s="30">
-        <v>0</v>
-      </c>
-      <c r="G40" s="30">
-        <v>0</v>
-      </c>
-      <c r="H40" s="30">
-        <v>0</v>
-      </c>
-      <c r="I40" s="37"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
       <c r="L40" s="69"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
+    <row r="41" spans="1:15" s="12" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="26"/>
+      <c r="E41" s="32">
+        <v>-4.0910000000000002E-4</v>
+      </c>
+      <c r="F41" s="29">
+        <v>-4.8529999999999997E-2</v>
+      </c>
+      <c r="G41" s="32">
+        <v>-4.6600000000000001E-5</v>
+      </c>
+      <c r="H41" s="29">
+        <v>-4.6100000000000004E-3</v>
+      </c>
+      <c r="I41" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K41" s="3"/>
+      <c r="L41" s="69">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="O41" s="3"/>
     </row>
     <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="29">
-        <v>-0.78983000000000003</v>
-      </c>
-      <c r="F42" s="29">
-        <v>0.68652000000000002</v>
-      </c>
-      <c r="G42" s="29">
-        <v>0.51990000000000003</v>
-      </c>
-      <c r="H42" s="29">
-        <v>-0.54949000000000003</v>
-      </c>
-      <c r="I42" s="3" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="29">
+        <v>0.44663999999999998</v>
+      </c>
+      <c r="F43" s="29">
+        <v>-0.49208000000000002</v>
+      </c>
+      <c r="G43" s="29">
+        <v>-0.14221</v>
+      </c>
+      <c r="H43" s="29">
+        <v>0.30010999999999999</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L42" s="69">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="29">
-        <v>-0.24740999999999999</v>
-      </c>
-      <c r="F43" s="29">
-        <v>0.40747</v>
-      </c>
-      <c r="G43" s="29">
-        <v>0.17821000000000001</v>
-      </c>
-      <c r="H43" s="29">
-        <v>-7.1730000000000002E-2</v>
-      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
       <c r="L43" s="69">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M43" s="18"/>
-    </row>
-    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>58</v>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>25</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="30">
+        <v>0</v>
+      </c>
+      <c r="F44" s="30">
+        <v>0</v>
+      </c>
+      <c r="G44" s="30">
+        <v>0</v>
+      </c>
+      <c r="H44" s="30">
+        <v>0</v>
+      </c>
+      <c r="I44" s="37"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="69"/>
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+    </row>
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="29">
+        <v>-0.78983000000000003</v>
+      </c>
+      <c r="F46" s="29">
+        <v>0.68652000000000002</v>
+      </c>
+      <c r="G46" s="29">
+        <v>0.51990000000000003</v>
+      </c>
+      <c r="H46" s="29">
+        <v>-0.54949000000000003</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L46" s="69">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="23"/>
+      <c r="D47" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="29">
+        <v>-0.24740999999999999</v>
+      </c>
+      <c r="F47" s="29">
+        <v>0.40747</v>
+      </c>
+      <c r="G47" s="29">
+        <v>0.17821000000000001</v>
+      </c>
+      <c r="H47" s="29">
+        <v>-7.1730000000000002E-2</v>
+      </c>
+      <c r="L47" s="69">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M47" s="18"/>
+    </row>
+    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="21"/>
+      <c r="D48" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29">
+      <c r="E48" s="29">
         <v>-0.73794000000000004</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F48" s="29">
         <v>1.07247</v>
       </c>
-      <c r="G44" s="29">
+      <c r="G48" s="29">
         <v>0.48502000000000001</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H48" s="29">
         <v>-0.41354000000000002</v>
       </c>
-      <c r="L44" s="69">
+      <c r="L48" s="69">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M44" s="18"/>
-    </row>
-    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+      <c r="M48" s="18"/>
+    </row>
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B49" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="30">
-        <v>0</v>
-      </c>
-      <c r="F45" s="30">
-        <v>0</v>
-      </c>
-      <c r="G45" s="30">
-        <v>0</v>
-      </c>
-      <c r="H45" s="30">
-        <v>0</v>
-      </c>
-      <c r="L45" s="69">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-    </row>
-    <row r="47" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="29">
-        <v>-2.613E-2</v>
-      </c>
-      <c r="F47" s="29">
-        <v>1.26464</v>
-      </c>
-      <c r="G47" s="29">
-        <v>1.28871</v>
-      </c>
-      <c r="H47" s="29">
-        <v>-0.33476</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="L47" s="69">
-        <v>-1</v>
-      </c>
-      <c r="M47" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="29">
-        <v>0.31215999999999999</v>
-      </c>
-      <c r="F48" s="29">
-        <v>-2.2751800000000002</v>
-      </c>
-      <c r="G48" s="29">
-        <v>-0.45154</v>
-      </c>
-      <c r="H48" s="29">
-        <v>-0.25944</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="L48" s="69">
-        <v>-1</v>
-      </c>
-      <c r="M48" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" s="29">
-        <v>-0.11212</v>
-      </c>
-      <c r="F49" s="29">
-        <v>-12.06884</v>
-      </c>
-      <c r="G49" s="29">
-        <v>-4.922E-2</v>
-      </c>
-      <c r="H49" s="29">
-        <v>-0.52005999999999997</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>239</v>
+        <v>59</v>
+      </c>
+      <c r="E49" s="30">
+        <v>0</v>
+      </c>
+      <c r="F49" s="30">
+        <v>0</v>
+      </c>
+      <c r="G49" s="30">
+        <v>0</v>
+      </c>
+      <c r="H49" s="30">
+        <v>0</v>
       </c>
       <c r="L49" s="69">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>251</v>
-      </c>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E50" s="29">
-        <v>0.48975000000000002</v>
-      </c>
-      <c r="F50" s="29">
-        <v>8.4699999999999998E-2</v>
-      </c>
-      <c r="G50" s="29">
-        <v>-0.60707999999999995</v>
-      </c>
-      <c r="H50" s="29">
-        <v>0.21389</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="L50" s="69">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="D50" s="19"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+    </row>
+    <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="30">
-        <v>0</v>
-      </c>
-      <c r="F51" s="31">
-        <v>0</v>
-      </c>
-      <c r="G51" s="30">
-        <v>0</v>
-      </c>
-      <c r="H51" s="30">
-        <v>0</v>
+        <v>248</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="29">
+        <v>-2.613E-2</v>
+      </c>
+      <c r="F51" s="29">
+        <v>1.26464</v>
+      </c>
+      <c r="G51" s="29">
+        <v>1.28871</v>
+      </c>
+      <c r="H51" s="29">
+        <v>-0.33476</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>239</v>
@@ -48917,29 +48934,31 @@
       <c r="L51" s="69">
         <v>-1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M51" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="C52"/>
-      <c r="D52" s="19" t="s">
-        <v>85</v>
+        <v>249</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="E52" s="29">
-        <v>-0.33046999999999999</v>
+        <v>0.31215999999999999</v>
       </c>
       <c r="F52" s="29">
-        <v>-0.10303</v>
+        <v>-2.2751800000000002</v>
       </c>
       <c r="G52" s="29">
-        <v>2.2827700000000002</v>
+        <v>-0.45154</v>
       </c>
       <c r="H52" s="29">
-        <v>-0.22592999999999999</v>
+        <v>-0.25944</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>239</v>
@@ -48947,29 +48966,32 @@
       <c r="L52" s="69">
         <v>-1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M52" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="24" t="s">
-        <v>86</v>
+        <v>250</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="E53" s="29">
-        <v>-0.43278</v>
+        <v>-0.11212</v>
       </c>
       <c r="F53" s="29">
-        <v>-1.3212900000000001</v>
-      </c>
-      <c r="G53" s="33">
-        <v>1.21E-4</v>
+        <v>-12.06884</v>
+      </c>
+      <c r="G53" s="29">
+        <v>-4.922E-2</v>
       </c>
       <c r="H53" s="29">
-        <v>-0.67791000000000001</v>
+        <v>-0.52005999999999997</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>239</v>
@@ -48978,28 +49000,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C54" s="27"/>
-      <c r="D54" t="s">
-        <v>87</v>
+        <v>251</v>
+      </c>
+      <c r="C54" s="21"/>
+      <c r="D54" s="26" t="s">
+        <v>83</v>
       </c>
       <c r="E54" s="29">
-        <v>-7.2679999999999995E-2</v>
+        <v>0.48975000000000002</v>
       </c>
       <c r="F54" s="29">
-        <v>-0.76593</v>
+        <v>8.4699999999999998E-2</v>
       </c>
       <c r="G54" s="29">
-        <v>0.17354</v>
+        <v>-0.60707999999999995</v>
       </c>
       <c r="H54" s="29">
-        <v>-1.9220000000000001E-2</v>
+        <v>0.21389</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>239</v>
@@ -49008,28 +49030,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="C55"/>
-      <c r="D55" t="s">
-        <v>88</v>
-      </c>
-      <c r="E55" s="29">
-        <v>-0.22628000000000001</v>
-      </c>
-      <c r="F55" s="29">
-        <v>-1.2003299999999999</v>
-      </c>
-      <c r="G55" s="29">
-        <v>0.68025000000000002</v>
-      </c>
-      <c r="H55" s="29">
-        <v>-0.22169</v>
+        <v>247</v>
+      </c>
+      <c r="C55" s="21"/>
+      <c r="D55" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" s="30">
+        <v>0</v>
+      </c>
+      <c r="F55" s="31">
+        <v>0</v>
+      </c>
+      <c r="G55" s="30">
+        <v>0</v>
+      </c>
+      <c r="H55" s="30">
+        <v>0</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>239</v>
@@ -49038,28 +49060,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C56"/>
-      <c r="D56" t="s">
-        <v>89</v>
-      </c>
-      <c r="E56" s="30">
-        <v>0</v>
-      </c>
-      <c r="F56" s="31">
-        <v>0</v>
-      </c>
-      <c r="G56" s="30">
-        <v>0</v>
-      </c>
-      <c r="H56" s="30">
-        <v>0</v>
+      <c r="D56" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="29">
+        <v>-0.33046999999999999</v>
+      </c>
+      <c r="F56" s="29">
+        <v>-0.10303</v>
+      </c>
+      <c r="G56" s="29">
+        <v>2.2827700000000002</v>
+      </c>
+      <c r="H56" s="29">
+        <v>-0.22592999999999999</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>239</v>
@@ -49068,28 +49090,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C57"/>
-      <c r="D57" t="s">
-        <v>90</v>
+        <v>254</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="E57" s="29">
-        <v>-0.56503999999999999</v>
+        <v>-0.43278</v>
       </c>
       <c r="F57" s="29">
-        <v>1.18842</v>
-      </c>
-      <c r="G57" s="29">
-        <v>2.0230800000000002</v>
+        <v>-1.3212900000000001</v>
+      </c>
+      <c r="G57" s="33">
+        <v>1.21E-4</v>
       </c>
       <c r="H57" s="29">
-        <v>-0.64468999999999999</v>
+        <v>-0.67791000000000001</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>239</v>
@@ -49098,28 +49120,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C58"/>
+        <v>255</v>
+      </c>
+      <c r="C58" s="27"/>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E58" s="29">
-        <v>-1.5776300000000001</v>
+        <v>-7.2679999999999995E-2</v>
       </c>
       <c r="F58" s="29">
-        <v>0.44257000000000002</v>
+        <v>-0.76593</v>
       </c>
       <c r="G58" s="29">
-        <v>0.62558999999999998</v>
+        <v>0.17354</v>
       </c>
       <c r="H58" s="29">
-        <v>-1.1697299999999999</v>
+        <v>-1.9220000000000001E-2</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>239</v>
@@ -49128,28 +49150,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E59" s="29">
-        <v>-0.10624</v>
+        <v>-0.22628000000000001</v>
       </c>
       <c r="F59" s="29">
-        <v>0.11786000000000001</v>
+        <v>-1.2003299999999999</v>
       </c>
       <c r="G59" s="29">
-        <v>-0.35576000000000002</v>
+        <v>0.68025000000000002</v>
       </c>
       <c r="H59" s="29">
-        <v>-0.45308999999999999</v>
+        <v>-0.22169</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>239</v>
@@ -49158,28 +49180,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
-        <v>93</v>
-      </c>
-      <c r="E60" s="29">
-        <v>-0.14899999999999999</v>
-      </c>
-      <c r="F60" s="29">
-        <v>-8.2640000000000005E-2</v>
-      </c>
-      <c r="G60" s="29">
-        <v>0.33577000000000001</v>
-      </c>
-      <c r="H60" s="29">
-        <v>-0.11143</v>
+        <v>89</v>
+      </c>
+      <c r="E60" s="30">
+        <v>0</v>
+      </c>
+      <c r="F60" s="31">
+        <v>0</v>
+      </c>
+      <c r="G60" s="30">
+        <v>0</v>
+      </c>
+      <c r="H60" s="30">
+        <v>0</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>239</v>
@@ -49188,28 +49210,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C61"/>
       <c r="D61" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" s="30">
-        <v>0</v>
-      </c>
-      <c r="F61" s="31">
-        <v>0</v>
-      </c>
-      <c r="G61" s="31">
-        <v>0</v>
-      </c>
-      <c r="H61" s="31">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="E61" s="29">
+        <v>-0.56503999999999999</v>
+      </c>
+      <c r="F61" s="29">
+        <v>1.18842</v>
+      </c>
+      <c r="G61" s="29">
+        <v>2.0230800000000002</v>
+      </c>
+      <c r="H61" s="29">
+        <v>-0.64468999999999999</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>239</v>
@@ -49218,28 +49240,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
-        <v>95</v>
-      </c>
-      <c r="E62" s="30">
-        <v>0</v>
-      </c>
-      <c r="F62" s="31">
-        <v>0</v>
-      </c>
-      <c r="G62" s="30">
-        <v>0</v>
-      </c>
-      <c r="H62" s="30">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="E62" s="29">
+        <v>-1.5776300000000001</v>
+      </c>
+      <c r="F62" s="29">
+        <v>0.44257000000000002</v>
+      </c>
+      <c r="G62" s="29">
+        <v>0.62558999999999998</v>
+      </c>
+      <c r="H62" s="29">
+        <v>-1.1697299999999999</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>239</v>
@@ -49248,28 +49270,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C63"/>
       <c r="D63" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" s="30">
-        <v>0</v>
-      </c>
-      <c r="F63" s="31">
-        <v>0</v>
-      </c>
-      <c r="G63" s="30">
-        <v>0</v>
-      </c>
-      <c r="H63" s="30">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E63" s="29">
+        <v>-0.10624</v>
+      </c>
+      <c r="F63" s="29">
+        <v>0.11786000000000001</v>
+      </c>
+      <c r="G63" s="29">
+        <v>-0.35576000000000002</v>
+      </c>
+      <c r="H63" s="29">
+        <v>-0.45308999999999999</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>239</v>
@@ -49278,28 +49300,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="34" t="s">
         <v>276</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C64"/>
       <c r="D64" t="s">
-        <v>97</v>
-      </c>
-      <c r="E64" s="30">
-        <v>0</v>
-      </c>
-      <c r="F64" s="31">
-        <v>0</v>
-      </c>
-      <c r="G64" s="30">
-        <v>0</v>
-      </c>
-      <c r="H64" s="30">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="E64" s="29">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="F64" s="29">
+        <v>-8.2640000000000005E-2</v>
+      </c>
+      <c r="G64" s="29">
+        <v>0.33577000000000001</v>
+      </c>
+      <c r="H64" s="29">
+        <v>-0.11143</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>239</v>
@@ -49313,11 +49335,11 @@
         <v>276</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C65"/>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E65" s="30">
         <v>0</v>
@@ -49325,10 +49347,10 @@
       <c r="F65" s="31">
         <v>0</v>
       </c>
-      <c r="G65" s="30">
+      <c r="G65" s="31">
         <v>0</v>
       </c>
-      <c r="H65" s="30">
+      <c r="H65" s="31">
         <v>0</v>
       </c>
       <c r="I65" s="3" t="s">
@@ -49343,11 +49365,11 @@
         <v>276</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C66"/>
       <c r="D66" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E66" s="30">
         <v>0</v>
@@ -49365,6 +49387,126 @@
         <v>239</v>
       </c>
       <c r="L66" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C67"/>
+      <c r="D67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E67" s="30">
+        <v>0</v>
+      </c>
+      <c r="F67" s="31">
+        <v>0</v>
+      </c>
+      <c r="G67" s="30">
+        <v>0</v>
+      </c>
+      <c r="H67" s="30">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L67" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" s="30">
+        <v>0</v>
+      </c>
+      <c r="F68" s="31">
+        <v>0</v>
+      </c>
+      <c r="G68" s="30">
+        <v>0</v>
+      </c>
+      <c r="H68" s="30">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L68" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69"/>
+      <c r="D69" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="30">
+        <v>0</v>
+      </c>
+      <c r="F69" s="31">
+        <v>0</v>
+      </c>
+      <c r="G69" s="30">
+        <v>0</v>
+      </c>
+      <c r="H69" s="30">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L69" s="69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70"/>
+      <c r="D70" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" s="30">
+        <v>0</v>
+      </c>
+      <c r="F70" s="31">
+        <v>0</v>
+      </c>
+      <c r="G70" s="30">
+        <v>0</v>
+      </c>
+      <c r="H70" s="30">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L70" s="69">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lung background info added as a tool
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01892EC5-9D5D-1F46-BDE5-4386E5A2E055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560F3F5A-6C13-2046-B996-B937311929F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1300" windowWidth="29680" windowHeight="18400" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="680" yWindow="1300" windowWidth="29680" windowHeight="18400" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3405" uniqueCount="306">
   <si>
     <t>Notes</t>
   </si>
@@ -955,6 +955,15 @@
   <si>
     <t>Mixed</t>
   </si>
+  <si>
+    <t>:guidance</t>
+  </si>
+  <si>
+    <t>Background Guidance</t>
+  </si>
+  <si>
+    <t>a page of guidance</t>
+  </si>
 </sst>
 </file>
 
@@ -14285,10 +14294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14340,6 +14349,17 @@
       </c>
       <c r="C4" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -47536,7 +47556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reorganised data and docs
added configuration README
</commit_message>
<xml_diff>
--- a/data/lung-models-master.xlsx
+++ b/data/lung-models-master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants.shadow/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3190281-9EE7-2844-8625-9FD9FFA3B31E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FBACB1-3C9B-A341-8519-D8B0EDE92B53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26240" yWindow="6340" windowWidth="34360" windowHeight="21040" activeTab="3" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="52640" yWindow="4540" windowWidth="34360" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="209">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -662,6 +662,15 @@
   <si>
     <t>Notes</t>
   </si>
+  <si>
+    <t>{:dps 1, :max 9, :min 1.3, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 0, :max 77, :min 1, :type :numeric}</t>
+  </si>
+  <si>
+    <t>{:dps 1, :max 4.5, :min -2.2, :type :numeric}</t>
+  </si>
 </sst>
 </file>
 
@@ -781,7 +790,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -914,6 +923,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1616,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:J3206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1126" sqref="F1126"/>
     </sheetView>
   </sheetViews>
@@ -32013,8 +32025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -32258,7 +32270,7 @@
       <c r="B10" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="57" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="52" t="s">
@@ -32288,7 +32300,7 @@
       <c r="B11" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="56"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="54" t="s">
         <v>189</v>
       </c>
@@ -33263,7 +33275,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="57"/>
+      <c r="F12" s="58"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -33279,7 +33291,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="57"/>
+      <c r="F13" s="58"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -41036,7 +41048,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -41206,7 +41218,7 @@
       <c r="B8" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -41230,7 +41242,7 @@
       <c r="B9" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="57"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="19" t="s">
         <v>164</v>
       </c>
@@ -41503,7 +41515,7 @@
       <c r="I24" s="42"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="46" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>104</v>
       </c>
@@ -41517,7 +41529,9 @@
       <c r="E25">
         <v>9.7850000000000006E-2</v>
       </c>
-      <c r="F25" s="49"/>
+      <c r="F25" s="49" t="s">
+        <v>208</v>
+      </c>
       <c r="I25" s="42">
         <v>2.2000000000000002</v>
       </c>
@@ -41533,7 +41547,7 @@
       <c r="I26" s="42"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="46" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>60</v>
       </c>
@@ -41547,7 +41561,9 @@
       <c r="E27">
         <v>-1.966E-2</v>
       </c>
-      <c r="F27" s="49"/>
+      <c r="F27" s="56" t="s">
+        <v>207</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>166</v>
       </c>
@@ -41565,7 +41581,7 @@
       <c r="I28" s="42"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="46" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>80</v>
       </c>
@@ -41579,7 +41595,9 @@
       <c r="E29">
         <v>1.32E-3</v>
       </c>
-      <c r="F29" s="49"/>
+      <c r="F29" s="49" t="s">
+        <v>207</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>113</v>
       </c>
@@ -41597,7 +41615,7 @@
       <c r="I30" s="42"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="31" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>105</v>
       </c>
@@ -41611,7 +41629,9 @@
       <c r="E31">
         <v>-3.5779999999999999E-2</v>
       </c>
-      <c r="F31" s="49"/>
+      <c r="F31" s="49" t="s">
+        <v>206</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>115</v>
       </c>
@@ -41639,7 +41659,7 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="57"/>
+      <c r="C34" s="58"/>
       <c r="E34" s="31"/>
       <c r="I34" s="42"/>
       <c r="J34" s="9" t="s">
@@ -41649,7 +41669,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="57"/>
+      <c r="C35" s="58"/>
       <c r="E35" s="31"/>
       <c r="I35" s="42"/>
       <c r="J35" s="9"/>

</xml_diff>